<commit_message>
Zotavení po přerušení komunikace
</commit_message>
<xml_diff>
--- a/MDM/WorkSheet.xlsx
+++ b/MDM/WorkSheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Úvodní schůze</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t>Úvodní sekvence</t>
+  </si>
+  <si>
+    <t>Ovládání kanálu</t>
   </si>
 </sst>
 </file>
@@ -946,10 +949,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H72"/>
+  <dimension ref="A1:H74"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="C72" sqref="C72"/>
+      <selection activeCell="A74" sqref="A74:C74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -987,11 +990,11 @@
       </c>
       <c r="F2" s="4">
         <f>SUM(C:C)</f>
-        <v>323</v>
+        <v>335</v>
       </c>
       <c r="H2" s="5">
         <f>F2*300</f>
-        <v>96900</v>
+        <v>100500</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1568,6 +1571,9 @@
       <c r="A69" s="1">
         <v>42896</v>
       </c>
+      <c r="B69" t="s">
+        <v>19</v>
+      </c>
       <c r="C69">
         <v>6</v>
       </c>
@@ -1594,6 +1600,22 @@
       </c>
       <c r="C72">
         <v>6</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="1">
+        <v>42902</v>
+      </c>
+      <c r="C73">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="1">
+        <v>42903</v>
+      </c>
+      <c r="C74">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revize startu a autotestu
</commit_message>
<xml_diff>
--- a/MDM/WorkSheet.xlsx
+++ b/MDM/WorkSheet.xlsx
@@ -949,10 +949,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H74"/>
+  <dimension ref="A1:H75"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="A74" sqref="A74:C74"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="A75" sqref="A75:C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -990,11 +990,11 @@
       </c>
       <c r="F2" s="4">
         <f>SUM(C:C)</f>
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="H2" s="5">
         <f>F2*300</f>
-        <v>100500</v>
+        <v>101400</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1616,6 +1616,14 @@
       </c>
       <c r="C74">
         <v>8</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="1">
+        <v>42904</v>
+      </c>
+      <c r="C75">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Opravy chyb po konzultaci
</commit_message>
<xml_diff>
--- a/MDM/WorkSheet.xlsx
+++ b/MDM/WorkSheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Úvodní schůze</t>
   </si>
@@ -74,6 +74,15 @@
   </si>
   <si>
     <t>Ovládání kanálu</t>
+  </si>
+  <si>
+    <t>Prezentace hotového</t>
+  </si>
+  <si>
+    <t>Databáze</t>
+  </si>
+  <si>
+    <t>Opravy chyb po konzultaci</t>
   </si>
 </sst>
 </file>
@@ -949,10 +958,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H75"/>
+  <dimension ref="A1:H80"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="A75" sqref="A75:C75"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="A80" sqref="A80:C80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -990,11 +999,11 @@
       </c>
       <c r="F2" s="4">
         <f>SUM(C:C)</f>
-        <v>338</v>
+        <v>359</v>
       </c>
       <c r="H2" s="5">
         <f>F2*300</f>
-        <v>101400</v>
+        <v>107700</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1624,6 +1633,58 @@
       </c>
       <c r="C75">
         <v>3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="1">
+        <v>42907</v>
+      </c>
+      <c r="B76" t="s">
+        <v>20</v>
+      </c>
+      <c r="C76">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="1">
+        <v>42911</v>
+      </c>
+      <c r="C77">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="1">
+        <v>42914</v>
+      </c>
+      <c r="B78" t="s">
+        <v>21</v>
+      </c>
+      <c r="C78">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="1">
+        <v>42915</v>
+      </c>
+      <c r="B79" t="s">
+        <v>21</v>
+      </c>
+      <c r="C79">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="1">
+        <v>42916</v>
+      </c>
+      <c r="B80" t="s">
+        <v>22</v>
+      </c>
+      <c r="C80">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revize, pokus o překlad v 64bit - nefunguje DesignMode pro Form a UserControl
</commit_message>
<xml_diff>
--- a/MDM/WorkSheet.xlsx
+++ b/MDM/WorkSheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>Úvodní schůze</t>
   </si>
@@ -86,6 +86,9 @@
   </si>
   <si>
     <t>Nastavování proudu</t>
+  </si>
+  <si>
+    <t>Revize</t>
   </si>
 </sst>
 </file>
@@ -961,10 +964,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H82"/>
+  <dimension ref="A1:H85"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="A82" sqref="A82:C82"/>
+      <selection activeCell="A85" sqref="A85:C85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1002,11 +1005,11 @@
       </c>
       <c r="F2" s="4">
         <f>SUM(C:C)</f>
-        <v>375</v>
+        <v>391</v>
       </c>
       <c r="H2" s="5">
         <f>F2*300</f>
-        <v>112500</v>
+        <v>117300</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1710,6 +1713,33 @@
       </c>
       <c r="C82">
         <v>8</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="1">
+        <v>42921</v>
+      </c>
+      <c r="B83" t="s">
+        <v>24</v>
+      </c>
+      <c r="C83">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="1">
+        <v>42922</v>
+      </c>
+      <c r="C84">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="1">
+        <v>42923</v>
+      </c>
+      <c r="C85">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Filtr na pacienty a jejich procedury
</commit_message>
<xml_diff>
--- a/MDM/WorkSheet.xlsx
+++ b/MDM/WorkSheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>Úvodní schůze</t>
   </si>
@@ -92,6 +92,18 @@
   </si>
   <si>
     <t>Procedura</t>
+  </si>
+  <si>
+    <t>Monitor</t>
+  </si>
+  <si>
+    <t>Opravy chyb, revize</t>
+  </si>
+  <si>
+    <t>Backup</t>
+  </si>
+  <si>
+    <t>Vkládání průběhů signálu</t>
   </si>
 </sst>
 </file>
@@ -967,10 +979,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H90"/>
+  <dimension ref="A1:H94"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="A90" sqref="A90:C90"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="A94" sqref="A94:C94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1008,11 +1020,11 @@
       </c>
       <c r="F2" s="4">
         <f>SUM(C:C)</f>
-        <v>417</v>
+        <v>431</v>
       </c>
       <c r="H2" s="5">
         <f>F2*300</f>
-        <v>125100</v>
+        <v>129300</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1784,8 +1796,52 @@
       <c r="A90" s="1">
         <v>42938</v>
       </c>
+      <c r="B90" t="s">
+        <v>26</v>
+      </c>
       <c r="C90">
         <v>6</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="1">
+        <v>42939</v>
+      </c>
+      <c r="B91" t="s">
+        <v>29</v>
+      </c>
+      <c r="C91">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="1">
+        <v>42940</v>
+      </c>
+      <c r="B92" t="s">
+        <v>27</v>
+      </c>
+      <c r="C92">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="1">
+        <v>42941</v>
+      </c>
+      <c r="C93">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="1">
+        <v>42942</v>
+      </c>
+      <c r="B94" t="s">
+        <v>28</v>
+      </c>
+      <c r="C94">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pomalý běh po přepnutí jazyka, revize
</commit_message>
<xml_diff>
--- a/MDM/WorkSheet.xlsx
+++ b/MDM/WorkSheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
   <si>
     <t>Úvodní schůze</t>
   </si>
@@ -104,6 +104,9 @@
   </si>
   <si>
     <t>Vkládání průběhů signálu</t>
+  </si>
+  <si>
+    <t>Pomalý běh po přepnutí jazyka, revize</t>
   </si>
 </sst>
 </file>
@@ -979,10 +982,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H94"/>
+  <dimension ref="A1:H95"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="A94" sqref="A94:C94"/>
+      <selection activeCell="A95" sqref="A95:C95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1020,11 +1023,11 @@
       </c>
       <c r="F2" s="4">
         <f>SUM(C:C)</f>
-        <v>431</v>
+        <v>435</v>
       </c>
       <c r="H2" s="5">
         <f>F2*300</f>
-        <v>129300</v>
+        <v>130500</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1842,6 +1845,17 @@
       </c>
       <c r="C94">
         <v>3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="1">
+        <v>42943</v>
+      </c>
+      <c r="B95" t="s">
+        <v>30</v>
+      </c>
+      <c r="C95">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Úpravy trackbaru pro nastavení proudu
</commit_message>
<xml_diff>
--- a/MDM/WorkSheet.xlsx
+++ b/MDM/WorkSheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
   <si>
     <t>Úvodní schůze</t>
   </si>
@@ -107,6 +107,9 @@
   </si>
   <si>
     <t>Pomalý běh po přepnutí jazyka, revize</t>
+  </si>
+  <si>
+    <t>Úpravy trackbaru nastavení proudu</t>
   </si>
 </sst>
 </file>
@@ -982,10 +985,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H95"/>
+  <dimension ref="A1:H97"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="A95" sqref="A95:C95"/>
+      <selection activeCell="A97" sqref="A97:C97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1023,11 +1026,11 @@
       </c>
       <c r="F2" s="4">
         <f>SUM(C:C)</f>
-        <v>435</v>
+        <v>441</v>
       </c>
       <c r="H2" s="5">
         <f>F2*300</f>
-        <v>130500</v>
+        <v>132300</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1855,6 +1858,28 @@
         <v>30</v>
       </c>
       <c r="C95">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="1">
+        <v>42944</v>
+      </c>
+      <c r="B96" t="s">
+        <v>24</v>
+      </c>
+      <c r="C96">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="1">
+        <v>42945</v>
+      </c>
+      <c r="B97" t="s">
+        <v>31</v>
+      </c>
+      <c r="C97">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Rekompilování do 64bit/Release, zápisy léčení do logu, revize splash screenu
</commit_message>
<xml_diff>
--- a/MDM/WorkSheet.xlsx
+++ b/MDM/WorkSheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
   <si>
     <t>Úvodní schůze</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t>Úpravy trackbaru nastavení proudu</t>
+  </si>
+  <si>
+    <t>Zápis léčení do logu, revize splash screenu</t>
   </si>
 </sst>
 </file>
@@ -985,10 +988,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H97"/>
+  <dimension ref="A1:H98"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="A97" sqref="A97:C97"/>
+      <selection activeCell="A98" sqref="A98:C98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1026,11 +1029,11 @@
       </c>
       <c r="F2" s="4">
         <f>SUM(C:C)</f>
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="H2" s="5">
         <f>F2*300</f>
-        <v>132300</v>
+        <v>132900</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1881,6 +1884,17 @@
       </c>
       <c r="C97">
         <v>4</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="1">
+        <v>42946</v>
+      </c>
+      <c r="B98" t="s">
+        <v>32</v>
+      </c>
+      <c r="C98">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Oprava přechodu mezi stavy "Active" a "Ready"
</commit_message>
<xml_diff>
--- a/MDM/WorkSheet.xlsx
+++ b/MDM/WorkSheet.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="20940" windowHeight="10110"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="20940" windowHeight="10110" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="WorkSheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Připomínky" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="58">
   <si>
     <t>Úvodní schůze</t>
   </si>
@@ -125,6 +126,69 @@
   </si>
   <si>
     <t>Opravy připomínek</t>
+  </si>
+  <si>
+    <t>hardwarový klíč</t>
+  </si>
+  <si>
+    <t>při přepínání segmentů se objeví D13 = 1</t>
+  </si>
+  <si>
+    <t>zadání pacienta: chybové hlášky se skryjí za okno pacienta</t>
+  </si>
+  <si>
+    <t>při pozastavení špatně funguje událost vysokého odporu</t>
+  </si>
+  <si>
+    <t>režim 2 jen při léčení! Při měření a událostech nastavit režim 0</t>
+  </si>
+  <si>
+    <t>upravit monitor pro různé role uživatelů</t>
+  </si>
+  <si>
+    <t>help ve formě PDF (jazykové mutace)</t>
+  </si>
+  <si>
+    <t>dlouhé nabíhání proudu ve stavu Připraven</t>
+  </si>
+  <si>
+    <t>procedura se započítá pokud prošlý čas je větší (roven) než 20 minut. Hodnota limitu do konfigurace.</t>
+  </si>
+  <si>
+    <t>procedury lze opakovat po uplynutí 4 hodin. Hodnota limitu do konfigurace.</t>
+  </si>
+  <si>
+    <t>zakódovat konfiguraci. Pro Superadmina udělat dialogové okno s konfigurací.</t>
+  </si>
+  <si>
+    <t>zálohu duplikovat na flashdisk, písmeno flashky do konfigurace</t>
+  </si>
+  <si>
+    <t>po zadání pacienta se nesmí dát modifikovat základní závislé údaje o pacientovi</t>
+  </si>
+  <si>
+    <t>funkce "Odstranit pacienta" nefunguje. Management pacienta je "divný".</t>
+  </si>
+  <si>
+    <t>přidat tlačítka "Procedury" a "Seznam pacientů" na hlavní toolbar</t>
+  </si>
+  <si>
+    <t>implementovat pípnutí při HR a na konci procedury</t>
+  </si>
+  <si>
+    <t>Chybové hlášení zkoušky výstupního kanálu při vstupním testu – umazat hlášku „Příliš vysoká impedance“, zbytek ponechat</t>
+  </si>
+  <si>
+    <t>obrázky do kanálů, každý kanál má jinou barvu konektoru</t>
+  </si>
+  <si>
+    <t>Hypertyp, 56+, muž – chybně zadané časové intervaly segmentů procedury</t>
+  </si>
+  <si>
+    <t>chybné chování při "rychlé" změně odporu ve stavech "Připraven" a "Léčení" (zřejmě souvisí s 5)</t>
+  </si>
+  <si>
+    <t>hlavní okno musí zůstat zafixováno na ploše</t>
   </si>
 </sst>
 </file>
@@ -289,7 +353,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -478,6 +542,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -642,7 +712,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="3" applyAlignment="1">
@@ -657,6 +727,13 @@
     <xf numFmtId="164" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="5"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1000,10 +1077,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H103"/>
+  <dimension ref="A1:H105"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="A103" sqref="A103:C103"/>
+    <sheetView showGridLines="0" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="A105" sqref="A105:C105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1041,11 +1118,11 @@
       </c>
       <c r="F2" s="4">
         <f>SUM(C:C)</f>
-        <v>460</v>
+        <v>464</v>
       </c>
       <c r="H2" s="5">
         <f>F2*300</f>
-        <v>138000</v>
+        <v>139200</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1961,7 +2038,1343 @@
         <v>3</v>
       </c>
     </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" s="1">
+        <v>42954</v>
+      </c>
+      <c r="C104">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" s="1">
+        <v>42955</v>
+      </c>
+      <c r="C105">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:P61"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9:P9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
+        <v>2</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="8"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
+        <v>4</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="9"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
+        <v>5</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
+        <v>7</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="8"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="8"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="8"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
+        <v>12</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="9"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
+        <v>13</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9"/>
+      <c r="P14" s="9"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="8"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
+      <c r="O17" s="8"/>
+      <c r="P17" s="8"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
+      <c r="O18" s="8"/>
+      <c r="P18" s="8"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="8"/>
+      <c r="O19" s="8"/>
+      <c r="P19" s="8"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A20" s="7">
+        <v>19</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9"/>
+      <c r="O20" s="9"/>
+      <c r="P20" s="9"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="8"/>
+      <c r="N21" s="8"/>
+      <c r="O21" s="8"/>
+      <c r="P21" s="8"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A22" s="7">
+        <v>21</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="9"/>
+      <c r="P22" s="9"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="8"/>
+      <c r="M23" s="8"/>
+      <c r="N23" s="8"/>
+      <c r="O23" s="8"/>
+      <c r="P23" s="8"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
+      <c r="K24" s="8"/>
+      <c r="L24" s="8"/>
+      <c r="M24" s="8"/>
+      <c r="N24" s="8"/>
+      <c r="O24" s="8"/>
+      <c r="P24" s="8"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
+      <c r="K25" s="8"/>
+      <c r="L25" s="8"/>
+      <c r="M25" s="8"/>
+      <c r="N25" s="8"/>
+      <c r="O25" s="8"/>
+      <c r="P25" s="8"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="8"/>
+      <c r="L26" s="8"/>
+      <c r="M26" s="8"/>
+      <c r="N26" s="8"/>
+      <c r="O26" s="8"/>
+      <c r="P26" s="8"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="8"/>
+      <c r="L27" s="8"/>
+      <c r="M27" s="8"/>
+      <c r="N27" s="8"/>
+      <c r="O27" s="8"/>
+      <c r="P27" s="8"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="8"/>
+      <c r="J28" s="8"/>
+      <c r="K28" s="8"/>
+      <c r="L28" s="8"/>
+      <c r="M28" s="8"/>
+      <c r="N28" s="8"/>
+      <c r="O28" s="8"/>
+      <c r="P28" s="8"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="8"/>
+      <c r="L29" s="8"/>
+      <c r="M29" s="8"/>
+      <c r="N29" s="8"/>
+      <c r="O29" s="8"/>
+      <c r="P29" s="8"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="8"/>
+      <c r="K30" s="8"/>
+      <c r="L30" s="8"/>
+      <c r="M30" s="8"/>
+      <c r="N30" s="8"/>
+      <c r="O30" s="8"/>
+      <c r="P30" s="8"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" s="8"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="8"/>
+      <c r="K31" s="8"/>
+      <c r="L31" s="8"/>
+      <c r="M31" s="8"/>
+      <c r="N31" s="8"/>
+      <c r="O31" s="8"/>
+      <c r="P31" s="8"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" s="8"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="8"/>
+      <c r="I32" s="8"/>
+      <c r="J32" s="8"/>
+      <c r="K32" s="8"/>
+      <c r="L32" s="8"/>
+      <c r="M32" s="8"/>
+      <c r="N32" s="8"/>
+      <c r="O32" s="8"/>
+      <c r="P32" s="8"/>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="8"/>
+      <c r="J33" s="8"/>
+      <c r="K33" s="8"/>
+      <c r="L33" s="8"/>
+      <c r="M33" s="8"/>
+      <c r="N33" s="8"/>
+      <c r="O33" s="8"/>
+      <c r="P33" s="8"/>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="8"/>
+      <c r="H34" s="8"/>
+      <c r="I34" s="8"/>
+      <c r="J34" s="8"/>
+      <c r="K34" s="8"/>
+      <c r="L34" s="8"/>
+      <c r="M34" s="8"/>
+      <c r="N34" s="8"/>
+      <c r="O34" s="8"/>
+      <c r="P34" s="8"/>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" s="8"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="8"/>
+      <c r="F35" s="8"/>
+      <c r="G35" s="8"/>
+      <c r="H35" s="8"/>
+      <c r="I35" s="8"/>
+      <c r="J35" s="8"/>
+      <c r="K35" s="8"/>
+      <c r="L35" s="8"/>
+      <c r="M35" s="8"/>
+      <c r="N35" s="8"/>
+      <c r="O35" s="8"/>
+      <c r="P35" s="8"/>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" s="8"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="8"/>
+      <c r="H36" s="8"/>
+      <c r="I36" s="8"/>
+      <c r="J36" s="8"/>
+      <c r="K36" s="8"/>
+      <c r="L36" s="8"/>
+      <c r="M36" s="8"/>
+      <c r="N36" s="8"/>
+      <c r="O36" s="8"/>
+      <c r="P36" s="8"/>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" s="8"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="8"/>
+      <c r="J37" s="8"/>
+      <c r="K37" s="8"/>
+      <c r="L37" s="8"/>
+      <c r="M37" s="8"/>
+      <c r="N37" s="8"/>
+      <c r="O37" s="8"/>
+      <c r="P37" s="8"/>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" s="8"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="8"/>
+      <c r="I38" s="8"/>
+      <c r="J38" s="8"/>
+      <c r="K38" s="8"/>
+      <c r="L38" s="8"/>
+      <c r="M38" s="8"/>
+      <c r="N38" s="8"/>
+      <c r="O38" s="8"/>
+      <c r="P38" s="8"/>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" s="8"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="8"/>
+      <c r="I39" s="8"/>
+      <c r="J39" s="8"/>
+      <c r="K39" s="8"/>
+      <c r="L39" s="8"/>
+      <c r="M39" s="8"/>
+      <c r="N39" s="8"/>
+      <c r="O39" s="8"/>
+      <c r="P39" s="8"/>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" s="8"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="8"/>
+      <c r="G40" s="8"/>
+      <c r="H40" s="8"/>
+      <c r="I40" s="8"/>
+      <c r="J40" s="8"/>
+      <c r="K40" s="8"/>
+      <c r="L40" s="8"/>
+      <c r="M40" s="8"/>
+      <c r="N40" s="8"/>
+      <c r="O40" s="8"/>
+      <c r="P40" s="8"/>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" s="8"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="8"/>
+      <c r="H41" s="8"/>
+      <c r="I41" s="8"/>
+      <c r="J41" s="8"/>
+      <c r="K41" s="8"/>
+      <c r="L41" s="8"/>
+      <c r="M41" s="8"/>
+      <c r="N41" s="8"/>
+      <c r="O41" s="8"/>
+      <c r="P41" s="8"/>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" s="8"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="8"/>
+      <c r="F42" s="8"/>
+      <c r="G42" s="8"/>
+      <c r="H42" s="8"/>
+      <c r="I42" s="8"/>
+      <c r="J42" s="8"/>
+      <c r="K42" s="8"/>
+      <c r="L42" s="8"/>
+      <c r="M42" s="8"/>
+      <c r="N42" s="8"/>
+      <c r="O42" s="8"/>
+      <c r="P42" s="8"/>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" s="8"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="8"/>
+      <c r="E43" s="8"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="8"/>
+      <c r="H43" s="8"/>
+      <c r="I43" s="8"/>
+      <c r="J43" s="8"/>
+      <c r="K43" s="8"/>
+      <c r="L43" s="8"/>
+      <c r="M43" s="8"/>
+      <c r="N43" s="8"/>
+      <c r="O43" s="8"/>
+      <c r="P43" s="8"/>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" s="8"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="8"/>
+      <c r="E44" s="8"/>
+      <c r="F44" s="8"/>
+      <c r="G44" s="8"/>
+      <c r="H44" s="8"/>
+      <c r="I44" s="8"/>
+      <c r="J44" s="8"/>
+      <c r="K44" s="8"/>
+      <c r="L44" s="8"/>
+      <c r="M44" s="8"/>
+      <c r="N44" s="8"/>
+      <c r="O44" s="8"/>
+      <c r="P44" s="8"/>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" s="8"/>
+      <c r="C45" s="8"/>
+      <c r="D45" s="8"/>
+      <c r="E45" s="8"/>
+      <c r="F45" s="8"/>
+      <c r="G45" s="8"/>
+      <c r="H45" s="8"/>
+      <c r="I45" s="8"/>
+      <c r="J45" s="8"/>
+      <c r="K45" s="8"/>
+      <c r="L45" s="8"/>
+      <c r="M45" s="8"/>
+      <c r="N45" s="8"/>
+      <c r="O45" s="8"/>
+      <c r="P45" s="8"/>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" s="8"/>
+      <c r="C46" s="8"/>
+      <c r="D46" s="8"/>
+      <c r="E46" s="8"/>
+      <c r="F46" s="8"/>
+      <c r="G46" s="8"/>
+      <c r="H46" s="8"/>
+      <c r="I46" s="8"/>
+      <c r="J46" s="8"/>
+      <c r="K46" s="8"/>
+      <c r="L46" s="8"/>
+      <c r="M46" s="8"/>
+      <c r="N46" s="8"/>
+      <c r="O46" s="8"/>
+      <c r="P46" s="8"/>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" s="8"/>
+      <c r="C47" s="8"/>
+      <c r="D47" s="8"/>
+      <c r="E47" s="8"/>
+      <c r="F47" s="8"/>
+      <c r="G47" s="8"/>
+      <c r="H47" s="8"/>
+      <c r="I47" s="8"/>
+      <c r="J47" s="8"/>
+      <c r="K47" s="8"/>
+      <c r="L47" s="8"/>
+      <c r="M47" s="8"/>
+      <c r="N47" s="8"/>
+      <c r="O47" s="8"/>
+      <c r="P47" s="8"/>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" s="8"/>
+      <c r="C48" s="8"/>
+      <c r="D48" s="8"/>
+      <c r="E48" s="8"/>
+      <c r="F48" s="8"/>
+      <c r="G48" s="8"/>
+      <c r="H48" s="8"/>
+      <c r="I48" s="8"/>
+      <c r="J48" s="8"/>
+      <c r="K48" s="8"/>
+      <c r="L48" s="8"/>
+      <c r="M48" s="8"/>
+      <c r="N48" s="8"/>
+      <c r="O48" s="8"/>
+      <c r="P48" s="8"/>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" s="8"/>
+      <c r="C49" s="8"/>
+      <c r="D49" s="8"/>
+      <c r="E49" s="8"/>
+      <c r="F49" s="8"/>
+      <c r="G49" s="8"/>
+      <c r="H49" s="8"/>
+      <c r="I49" s="8"/>
+      <c r="J49" s="8"/>
+      <c r="K49" s="8"/>
+      <c r="L49" s="8"/>
+      <c r="M49" s="8"/>
+      <c r="N49" s="8"/>
+      <c r="O49" s="8"/>
+      <c r="P49" s="8"/>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" s="8"/>
+      <c r="C50" s="8"/>
+      <c r="D50" s="8"/>
+      <c r="E50" s="8"/>
+      <c r="F50" s="8"/>
+      <c r="G50" s="8"/>
+      <c r="H50" s="8"/>
+      <c r="I50" s="8"/>
+      <c r="J50" s="8"/>
+      <c r="K50" s="8"/>
+      <c r="L50" s="8"/>
+      <c r="M50" s="8"/>
+      <c r="N50" s="8"/>
+      <c r="O50" s="8"/>
+      <c r="P50" s="8"/>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" s="8"/>
+      <c r="C51" s="8"/>
+      <c r="D51" s="8"/>
+      <c r="E51" s="8"/>
+      <c r="F51" s="8"/>
+      <c r="G51" s="8"/>
+      <c r="H51" s="8"/>
+      <c r="I51" s="8"/>
+      <c r="J51" s="8"/>
+      <c r="K51" s="8"/>
+      <c r="L51" s="8"/>
+      <c r="M51" s="8"/>
+      <c r="N51" s="8"/>
+      <c r="O51" s="8"/>
+      <c r="P51" s="8"/>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" s="8"/>
+      <c r="C52" s="8"/>
+      <c r="D52" s="8"/>
+      <c r="E52" s="8"/>
+      <c r="F52" s="8"/>
+      <c r="G52" s="8"/>
+      <c r="H52" s="8"/>
+      <c r="I52" s="8"/>
+      <c r="J52" s="8"/>
+      <c r="K52" s="8"/>
+      <c r="L52" s="8"/>
+      <c r="M52" s="8"/>
+      <c r="N52" s="8"/>
+      <c r="O52" s="8"/>
+      <c r="P52" s="8"/>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" s="8"/>
+      <c r="C53" s="8"/>
+      <c r="D53" s="8"/>
+      <c r="E53" s="8"/>
+      <c r="F53" s="8"/>
+      <c r="G53" s="8"/>
+      <c r="H53" s="8"/>
+      <c r="I53" s="8"/>
+      <c r="J53" s="8"/>
+      <c r="K53" s="8"/>
+      <c r="L53" s="8"/>
+      <c r="M53" s="8"/>
+      <c r="N53" s="8"/>
+      <c r="O53" s="8"/>
+      <c r="P53" s="8"/>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" s="8"/>
+      <c r="C54" s="8"/>
+      <c r="D54" s="8"/>
+      <c r="E54" s="8"/>
+      <c r="F54" s="8"/>
+      <c r="G54" s="8"/>
+      <c r="H54" s="8"/>
+      <c r="I54" s="8"/>
+      <c r="J54" s="8"/>
+      <c r="K54" s="8"/>
+      <c r="L54" s="8"/>
+      <c r="M54" s="8"/>
+      <c r="N54" s="8"/>
+      <c r="O54" s="8"/>
+      <c r="P54" s="8"/>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" s="8"/>
+      <c r="C55" s="8"/>
+      <c r="D55" s="8"/>
+      <c r="E55" s="8"/>
+      <c r="F55" s="8"/>
+      <c r="G55" s="8"/>
+      <c r="H55" s="8"/>
+      <c r="I55" s="8"/>
+      <c r="J55" s="8"/>
+      <c r="K55" s="8"/>
+      <c r="L55" s="8"/>
+      <c r="M55" s="8"/>
+      <c r="N55" s="8"/>
+      <c r="O55" s="8"/>
+      <c r="P55" s="8"/>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" s="8"/>
+      <c r="C56" s="8"/>
+      <c r="D56" s="8"/>
+      <c r="E56" s="8"/>
+      <c r="F56" s="8"/>
+      <c r="G56" s="8"/>
+      <c r="H56" s="8"/>
+      <c r="I56" s="8"/>
+      <c r="J56" s="8"/>
+      <c r="K56" s="8"/>
+      <c r="L56" s="8"/>
+      <c r="M56" s="8"/>
+      <c r="N56" s="8"/>
+      <c r="O56" s="8"/>
+      <c r="P56" s="8"/>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" s="8"/>
+      <c r="C57" s="8"/>
+      <c r="D57" s="8"/>
+      <c r="E57" s="8"/>
+      <c r="F57" s="8"/>
+      <c r="G57" s="8"/>
+      <c r="H57" s="8"/>
+      <c r="I57" s="8"/>
+      <c r="J57" s="8"/>
+      <c r="K57" s="8"/>
+      <c r="L57" s="8"/>
+      <c r="M57" s="8"/>
+      <c r="N57" s="8"/>
+      <c r="O57" s="8"/>
+      <c r="P57" s="8"/>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" s="8"/>
+      <c r="C58" s="8"/>
+      <c r="D58" s="8"/>
+      <c r="E58" s="8"/>
+      <c r="F58" s="8"/>
+      <c r="G58" s="8"/>
+      <c r="H58" s="8"/>
+      <c r="I58" s="8"/>
+      <c r="J58" s="8"/>
+      <c r="K58" s="8"/>
+      <c r="L58" s="8"/>
+      <c r="M58" s="8"/>
+      <c r="N58" s="8"/>
+      <c r="O58" s="8"/>
+      <c r="P58" s="8"/>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" s="8"/>
+      <c r="C59" s="8"/>
+      <c r="D59" s="8"/>
+      <c r="E59" s="8"/>
+      <c r="F59" s="8"/>
+      <c r="G59" s="8"/>
+      <c r="H59" s="8"/>
+      <c r="I59" s="8"/>
+      <c r="J59" s="8"/>
+      <c r="K59" s="8"/>
+      <c r="L59" s="8"/>
+      <c r="M59" s="8"/>
+      <c r="N59" s="8"/>
+      <c r="O59" s="8"/>
+      <c r="P59" s="8"/>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" s="8"/>
+      <c r="C60" s="8"/>
+      <c r="D60" s="8"/>
+      <c r="E60" s="8"/>
+      <c r="F60" s="8"/>
+      <c r="G60" s="8"/>
+      <c r="H60" s="8"/>
+      <c r="I60" s="8"/>
+      <c r="J60" s="8"/>
+      <c r="K60" s="8"/>
+      <c r="L60" s="8"/>
+      <c r="M60" s="8"/>
+      <c r="N60" s="8"/>
+      <c r="O60" s="8"/>
+      <c r="P60" s="8"/>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" s="8"/>
+      <c r="C61" s="8"/>
+      <c r="D61" s="8"/>
+      <c r="E61" s="8"/>
+      <c r="F61" s="8"/>
+      <c r="G61" s="8"/>
+      <c r="H61" s="8"/>
+      <c r="I61" s="8"/>
+      <c r="J61" s="8"/>
+      <c r="K61" s="8"/>
+      <c r="L61" s="8"/>
+      <c r="M61" s="8"/>
+      <c r="N61" s="8"/>
+      <c r="O61" s="8"/>
+      <c r="P61" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="60">
+    <mergeCell ref="B13:P13"/>
+    <mergeCell ref="B2:P2"/>
+    <mergeCell ref="B3:P3"/>
+    <mergeCell ref="B4:P4"/>
+    <mergeCell ref="B5:P5"/>
+    <mergeCell ref="B6:P6"/>
+    <mergeCell ref="B7:P7"/>
+    <mergeCell ref="B8:P8"/>
+    <mergeCell ref="B9:P9"/>
+    <mergeCell ref="B10:P10"/>
+    <mergeCell ref="B11:P11"/>
+    <mergeCell ref="B12:P12"/>
+    <mergeCell ref="B25:P25"/>
+    <mergeCell ref="B14:P14"/>
+    <mergeCell ref="B15:P15"/>
+    <mergeCell ref="B16:P16"/>
+    <mergeCell ref="B17:P17"/>
+    <mergeCell ref="B18:P18"/>
+    <mergeCell ref="B19:P19"/>
+    <mergeCell ref="B20:P20"/>
+    <mergeCell ref="B21:P21"/>
+    <mergeCell ref="B22:P22"/>
+    <mergeCell ref="B23:P23"/>
+    <mergeCell ref="B24:P24"/>
+    <mergeCell ref="B37:P37"/>
+    <mergeCell ref="B26:P26"/>
+    <mergeCell ref="B27:P27"/>
+    <mergeCell ref="B28:P28"/>
+    <mergeCell ref="B29:P29"/>
+    <mergeCell ref="B30:P30"/>
+    <mergeCell ref="B31:P31"/>
+    <mergeCell ref="B32:P32"/>
+    <mergeCell ref="B33:P33"/>
+    <mergeCell ref="B34:P34"/>
+    <mergeCell ref="B35:P35"/>
+    <mergeCell ref="B36:P36"/>
+    <mergeCell ref="B49:P49"/>
+    <mergeCell ref="B38:P38"/>
+    <mergeCell ref="B39:P39"/>
+    <mergeCell ref="B40:P40"/>
+    <mergeCell ref="B41:P41"/>
+    <mergeCell ref="B42:P42"/>
+    <mergeCell ref="B43:P43"/>
+    <mergeCell ref="B44:P44"/>
+    <mergeCell ref="B45:P45"/>
+    <mergeCell ref="B46:P46"/>
+    <mergeCell ref="B47:P47"/>
+    <mergeCell ref="B48:P48"/>
+    <mergeCell ref="B61:P61"/>
+    <mergeCell ref="B50:P50"/>
+    <mergeCell ref="B51:P51"/>
+    <mergeCell ref="B52:P52"/>
+    <mergeCell ref="B53:P53"/>
+    <mergeCell ref="B54:P54"/>
+    <mergeCell ref="B55:P55"/>
+    <mergeCell ref="B56:P56"/>
+    <mergeCell ref="B57:P57"/>
+    <mergeCell ref="B58:P58"/>
+    <mergeCell ref="B59:P59"/>
+    <mergeCell ref="B60:P60"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Oprava stavu HR a dalších připomínek
</commit_message>
<xml_diff>
--- a/MDM/WorkSheet.xlsx
+++ b/MDM/WorkSheet.xlsx
@@ -729,10 +729,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="5"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="5"/>
     </xf>
   </cellXfs>
@@ -1077,10 +1077,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H105"/>
+  <dimension ref="A1:H106"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="A105" sqref="A105:C105"/>
+      <selection activeCell="A106" sqref="A106:C106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1118,11 +1118,11 @@
       </c>
       <c r="F2" s="4">
         <f>SUM(C:C)</f>
-        <v>464</v>
+        <v>467</v>
       </c>
       <c r="H2" s="5">
         <f>F2*300</f>
-        <v>139200</v>
+        <v>140100</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -2052,6 +2052,14 @@
       </c>
       <c r="C105">
         <v>2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" s="1">
+        <v>42957</v>
+      </c>
+      <c r="C106">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -2064,7 +2072,7 @@
   <dimension ref="A2:P61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:P9"/>
+      <selection activeCell="B10" sqref="B10:P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2073,48 +2081,48 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
-      <c r="P2" s="8"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>2</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="9"/>
-      <c r="P3" s="9"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="7">
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
@@ -2139,158 +2147,158 @@
       <c r="A5" s="7">
         <v>4</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
-      <c r="M5" s="9"/>
-      <c r="N5" s="9"/>
-      <c r="O5" s="9"/>
-      <c r="P5" s="9"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>5</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
-      <c r="M6" s="9"/>
-      <c r="N6" s="9"/>
-      <c r="O6" s="9"/>
-      <c r="P6" s="9"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="8"/>
+      <c r="P6" s="8"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>6</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="9"/>
-      <c r="M7" s="9"/>
-      <c r="N7" s="9"/>
-      <c r="O7" s="9"/>
-      <c r="P7" s="9"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="8"/>
+      <c r="O7" s="8"/>
+      <c r="P7" s="8"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>7</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="9"/>
-      <c r="N8" s="9"/>
-      <c r="O8" s="9"/>
-      <c r="P8" s="9"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="8"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8"/>
-      <c r="P9" s="8"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="8"/>
-      <c r="O10" s="8"/>
-      <c r="P10" s="8"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="9"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="8"/>
-      <c r="O11" s="8"/>
-      <c r="P11" s="8"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="9"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="A12" s="7">
         <v>11</v>
       </c>
       <c r="B12" s="8" t="s">
@@ -2315,136 +2323,136 @@
       <c r="A13" s="7">
         <v>12</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="9"/>
-      <c r="O13" s="9"/>
-      <c r="P13" s="9"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="8"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>13</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="9"/>
-      <c r="L14" s="9"/>
-      <c r="M14" s="9"/>
-      <c r="N14" s="9"/>
-      <c r="O14" s="9"/>
-      <c r="P14" s="9"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
-      <c r="M15" s="8"/>
-      <c r="N15" s="8"/>
-      <c r="O15" s="8"/>
-      <c r="P15" s="8"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="9"/>
+      <c r="P15" s="9"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8"/>
-      <c r="M16" s="8"/>
-      <c r="N16" s="8"/>
-      <c r="O16" s="8"/>
-      <c r="P16" s="8"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
+      <c r="P16" s="9"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="8"/>
-      <c r="M17" s="8"/>
-      <c r="N17" s="8"/>
-      <c r="O17" s="8"/>
-      <c r="P17" s="8"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
+      <c r="O17" s="9"/>
+      <c r="P17" s="9"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="8"/>
-      <c r="M18" s="8"/>
-      <c r="N18" s="8"/>
-      <c r="O18" s="8"/>
-      <c r="P18" s="8"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="9"/>
+      <c r="O18" s="9"/>
+      <c r="P18" s="9"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19">
+      <c r="A19" s="7">
         <v>18</v>
       </c>
       <c r="B19" s="8" t="s">
@@ -2469,26 +2477,26 @@
       <c r="A20" s="7">
         <v>19</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
-      <c r="L20" s="9"/>
-      <c r="M20" s="9"/>
-      <c r="N20" s="9"/>
-      <c r="O20" s="9"/>
-      <c r="P20" s="9"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
+      <c r="L20" s="8"/>
+      <c r="M20" s="8"/>
+      <c r="N20" s="8"/>
+      <c r="O20" s="8"/>
+      <c r="P20" s="8"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21">
+      <c r="A21" s="7">
         <v>20</v>
       </c>
       <c r="B21" s="8" t="s">
@@ -2513,806 +2521,854 @@
       <c r="A22" s="7">
         <v>21</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
-      <c r="J22" s="9"/>
-      <c r="K22" s="9"/>
-      <c r="L22" s="9"/>
-      <c r="M22" s="9"/>
-      <c r="N22" s="9"/>
-      <c r="O22" s="9"/>
-      <c r="P22" s="9"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8"/>
+      <c r="M22" s="8"/>
+      <c r="N22" s="8"/>
+      <c r="O22" s="8"/>
+      <c r="P22" s="8"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
-      <c r="J23" s="8"/>
-      <c r="K23" s="8"/>
-      <c r="L23" s="8"/>
-      <c r="M23" s="8"/>
-      <c r="N23" s="8"/>
-      <c r="O23" s="8"/>
-      <c r="P23" s="8"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="9"/>
+      <c r="N23" s="9"/>
+      <c r="O23" s="9"/>
+      <c r="P23" s="9"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="8"/>
-      <c r="J24" s="8"/>
-      <c r="K24" s="8"/>
-      <c r="L24" s="8"/>
-      <c r="M24" s="8"/>
-      <c r="N24" s="8"/>
-      <c r="O24" s="8"/>
-      <c r="P24" s="8"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="9"/>
+      <c r="M24" s="9"/>
+      <c r="N24" s="9"/>
+      <c r="O24" s="9"/>
+      <c r="P24" s="9"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="8"/>
-      <c r="K25" s="8"/>
-      <c r="L25" s="8"/>
-      <c r="M25" s="8"/>
-      <c r="N25" s="8"/>
-      <c r="O25" s="8"/>
-      <c r="P25" s="8"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="9"/>
+      <c r="L25" s="9"/>
+      <c r="M25" s="9"/>
+      <c r="N25" s="9"/>
+      <c r="O25" s="9"/>
+      <c r="P25" s="9"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="8"/>
-      <c r="K26" s="8"/>
-      <c r="L26" s="8"/>
-      <c r="M26" s="8"/>
-      <c r="N26" s="8"/>
-      <c r="O26" s="8"/>
-      <c r="P26" s="8"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
+      <c r="K26" s="9"/>
+      <c r="L26" s="9"/>
+      <c r="M26" s="9"/>
+      <c r="N26" s="9"/>
+      <c r="O26" s="9"/>
+      <c r="P26" s="9"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
-      <c r="I27" s="8"/>
-      <c r="J27" s="8"/>
-      <c r="K27" s="8"/>
-      <c r="L27" s="8"/>
-      <c r="M27" s="8"/>
-      <c r="N27" s="8"/>
-      <c r="O27" s="8"/>
-      <c r="P27" s="8"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="9"/>
+      <c r="K27" s="9"/>
+      <c r="L27" s="9"/>
+      <c r="M27" s="9"/>
+      <c r="N27" s="9"/>
+      <c r="O27" s="9"/>
+      <c r="P27" s="9"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="8"/>
-      <c r="K28" s="8"/>
-      <c r="L28" s="8"/>
-      <c r="M28" s="8"/>
-      <c r="N28" s="8"/>
-      <c r="O28" s="8"/>
-      <c r="P28" s="8"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="9"/>
+      <c r="K28" s="9"/>
+      <c r="L28" s="9"/>
+      <c r="M28" s="9"/>
+      <c r="N28" s="9"/>
+      <c r="O28" s="9"/>
+      <c r="P28" s="9"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8"/>
-      <c r="K29" s="8"/>
-      <c r="L29" s="8"/>
-      <c r="M29" s="8"/>
-      <c r="N29" s="8"/>
-      <c r="O29" s="8"/>
-      <c r="P29" s="8"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9"/>
+      <c r="K29" s="9"/>
+      <c r="L29" s="9"/>
+      <c r="M29" s="9"/>
+      <c r="N29" s="9"/>
+      <c r="O29" s="9"/>
+      <c r="P29" s="9"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
-      <c r="J30" s="8"/>
-      <c r="K30" s="8"/>
-      <c r="L30" s="8"/>
-      <c r="M30" s="8"/>
-      <c r="N30" s="8"/>
-      <c r="O30" s="8"/>
-      <c r="P30" s="8"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
+      <c r="K30" s="9"/>
+      <c r="L30" s="9"/>
+      <c r="M30" s="9"/>
+      <c r="N30" s="9"/>
+      <c r="O30" s="9"/>
+      <c r="P30" s="9"/>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="8"/>
-      <c r="K31" s="8"/>
-      <c r="L31" s="8"/>
-      <c r="M31" s="8"/>
-      <c r="N31" s="8"/>
-      <c r="O31" s="8"/>
-      <c r="P31" s="8"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="9"/>
+      <c r="K31" s="9"/>
+      <c r="L31" s="9"/>
+      <c r="M31" s="9"/>
+      <c r="N31" s="9"/>
+      <c r="O31" s="9"/>
+      <c r="P31" s="9"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
-      <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="8"/>
-      <c r="H32" s="8"/>
-      <c r="I32" s="8"/>
-      <c r="J32" s="8"/>
-      <c r="K32" s="8"/>
-      <c r="L32" s="8"/>
-      <c r="M32" s="8"/>
-      <c r="N32" s="8"/>
-      <c r="O32" s="8"/>
-      <c r="P32" s="8"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="9"/>
+      <c r="K32" s="9"/>
+      <c r="L32" s="9"/>
+      <c r="M32" s="9"/>
+      <c r="N32" s="9"/>
+      <c r="O32" s="9"/>
+      <c r="P32" s="9"/>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="8"/>
-      <c r="I33" s="8"/>
-      <c r="J33" s="8"/>
-      <c r="K33" s="8"/>
-      <c r="L33" s="8"/>
-      <c r="M33" s="8"/>
-      <c r="N33" s="8"/>
-      <c r="O33" s="8"/>
-      <c r="P33" s="8"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="9"/>
+      <c r="J33" s="9"/>
+      <c r="K33" s="9"/>
+      <c r="L33" s="9"/>
+      <c r="M33" s="9"/>
+      <c r="N33" s="9"/>
+      <c r="O33" s="9"/>
+      <c r="P33" s="9"/>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8"/>
-      <c r="G34" s="8"/>
-      <c r="H34" s="8"/>
-      <c r="I34" s="8"/>
-      <c r="J34" s="8"/>
-      <c r="K34" s="8"/>
-      <c r="L34" s="8"/>
-      <c r="M34" s="8"/>
-      <c r="N34" s="8"/>
-      <c r="O34" s="8"/>
-      <c r="P34" s="8"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="9"/>
+      <c r="J34" s="9"/>
+      <c r="K34" s="9"/>
+      <c r="L34" s="9"/>
+      <c r="M34" s="9"/>
+      <c r="N34" s="9"/>
+      <c r="O34" s="9"/>
+      <c r="P34" s="9"/>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
-      <c r="B35" s="8"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="8"/>
-      <c r="I35" s="8"/>
-      <c r="J35" s="8"/>
-      <c r="K35" s="8"/>
-      <c r="L35" s="8"/>
-      <c r="M35" s="8"/>
-      <c r="N35" s="8"/>
-      <c r="O35" s="8"/>
-      <c r="P35" s="8"/>
+      <c r="B35" s="9"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="9"/>
+      <c r="I35" s="9"/>
+      <c r="J35" s="9"/>
+      <c r="K35" s="9"/>
+      <c r="L35" s="9"/>
+      <c r="M35" s="9"/>
+      <c r="N35" s="9"/>
+      <c r="O35" s="9"/>
+      <c r="P35" s="9"/>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
-      <c r="B36" s="8"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="8"/>
-      <c r="F36" s="8"/>
-      <c r="G36" s="8"/>
-      <c r="H36" s="8"/>
-      <c r="I36" s="8"/>
-      <c r="J36" s="8"/>
-      <c r="K36" s="8"/>
-      <c r="L36" s="8"/>
-      <c r="M36" s="8"/>
-      <c r="N36" s="8"/>
-      <c r="O36" s="8"/>
-      <c r="P36" s="8"/>
+      <c r="B36" s="9"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="9"/>
+      <c r="I36" s="9"/>
+      <c r="J36" s="9"/>
+      <c r="K36" s="9"/>
+      <c r="L36" s="9"/>
+      <c r="M36" s="9"/>
+      <c r="N36" s="9"/>
+      <c r="O36" s="9"/>
+      <c r="P36" s="9"/>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
-      <c r="B37" s="8"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="8"/>
-      <c r="I37" s="8"/>
-      <c r="J37" s="8"/>
-      <c r="K37" s="8"/>
-      <c r="L37" s="8"/>
-      <c r="M37" s="8"/>
-      <c r="N37" s="8"/>
-      <c r="O37" s="8"/>
-      <c r="P37" s="8"/>
+      <c r="B37" s="9"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="9"/>
+      <c r="I37" s="9"/>
+      <c r="J37" s="9"/>
+      <c r="K37" s="9"/>
+      <c r="L37" s="9"/>
+      <c r="M37" s="9"/>
+      <c r="N37" s="9"/>
+      <c r="O37" s="9"/>
+      <c r="P37" s="9"/>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
-      <c r="B38" s="8"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="8"/>
-      <c r="F38" s="8"/>
-      <c r="G38" s="8"/>
-      <c r="H38" s="8"/>
-      <c r="I38" s="8"/>
-      <c r="J38" s="8"/>
-      <c r="K38" s="8"/>
-      <c r="L38" s="8"/>
-      <c r="M38" s="8"/>
-      <c r="N38" s="8"/>
-      <c r="O38" s="8"/>
-      <c r="P38" s="8"/>
+      <c r="B38" s="9"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="9"/>
+      <c r="I38" s="9"/>
+      <c r="J38" s="9"/>
+      <c r="K38" s="9"/>
+      <c r="L38" s="9"/>
+      <c r="M38" s="9"/>
+      <c r="N38" s="9"/>
+      <c r="O38" s="9"/>
+      <c r="P38" s="9"/>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
-      <c r="B39" s="8"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="8"/>
-      <c r="F39" s="8"/>
-      <c r="G39" s="8"/>
-      <c r="H39" s="8"/>
-      <c r="I39" s="8"/>
-      <c r="J39" s="8"/>
-      <c r="K39" s="8"/>
-      <c r="L39" s="8"/>
-      <c r="M39" s="8"/>
-      <c r="N39" s="8"/>
-      <c r="O39" s="8"/>
-      <c r="P39" s="8"/>
+      <c r="B39" s="9"/>
+      <c r="C39" s="9"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="9"/>
+      <c r="H39" s="9"/>
+      <c r="I39" s="9"/>
+      <c r="J39" s="9"/>
+      <c r="K39" s="9"/>
+      <c r="L39" s="9"/>
+      <c r="M39" s="9"/>
+      <c r="N39" s="9"/>
+      <c r="O39" s="9"/>
+      <c r="P39" s="9"/>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
-      <c r="B40" s="8"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="8"/>
-      <c r="E40" s="8"/>
-      <c r="F40" s="8"/>
-      <c r="G40" s="8"/>
-      <c r="H40" s="8"/>
-      <c r="I40" s="8"/>
-      <c r="J40" s="8"/>
-      <c r="K40" s="8"/>
-      <c r="L40" s="8"/>
-      <c r="M40" s="8"/>
-      <c r="N40" s="8"/>
-      <c r="O40" s="8"/>
-      <c r="P40" s="8"/>
+      <c r="B40" s="9"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="9"/>
+      <c r="H40" s="9"/>
+      <c r="I40" s="9"/>
+      <c r="J40" s="9"/>
+      <c r="K40" s="9"/>
+      <c r="L40" s="9"/>
+      <c r="M40" s="9"/>
+      <c r="N40" s="9"/>
+      <c r="O40" s="9"/>
+      <c r="P40" s="9"/>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
-      <c r="B41" s="8"/>
-      <c r="C41" s="8"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="8"/>
-      <c r="F41" s="8"/>
-      <c r="G41" s="8"/>
-      <c r="H41" s="8"/>
-      <c r="I41" s="8"/>
-      <c r="J41" s="8"/>
-      <c r="K41" s="8"/>
-      <c r="L41" s="8"/>
-      <c r="M41" s="8"/>
-      <c r="N41" s="8"/>
-      <c r="O41" s="8"/>
-      <c r="P41" s="8"/>
+      <c r="B41" s="9"/>
+      <c r="C41" s="9"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="9"/>
+      <c r="H41" s="9"/>
+      <c r="I41" s="9"/>
+      <c r="J41" s="9"/>
+      <c r="K41" s="9"/>
+      <c r="L41" s="9"/>
+      <c r="M41" s="9"/>
+      <c r="N41" s="9"/>
+      <c r="O41" s="9"/>
+      <c r="P41" s="9"/>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
-      <c r="B42" s="8"/>
-      <c r="C42" s="8"/>
-      <c r="D42" s="8"/>
-      <c r="E42" s="8"/>
-      <c r="F42" s="8"/>
-      <c r="G42" s="8"/>
-      <c r="H42" s="8"/>
-      <c r="I42" s="8"/>
-      <c r="J42" s="8"/>
-      <c r="K42" s="8"/>
-      <c r="L42" s="8"/>
-      <c r="M42" s="8"/>
-      <c r="N42" s="8"/>
-      <c r="O42" s="8"/>
-      <c r="P42" s="8"/>
+      <c r="B42" s="9"/>
+      <c r="C42" s="9"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
+      <c r="G42" s="9"/>
+      <c r="H42" s="9"/>
+      <c r="I42" s="9"/>
+      <c r="J42" s="9"/>
+      <c r="K42" s="9"/>
+      <c r="L42" s="9"/>
+      <c r="M42" s="9"/>
+      <c r="N42" s="9"/>
+      <c r="O42" s="9"/>
+      <c r="P42" s="9"/>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
-      <c r="B43" s="8"/>
-      <c r="C43" s="8"/>
-      <c r="D43" s="8"/>
-      <c r="E43" s="8"/>
-      <c r="F43" s="8"/>
-      <c r="G43" s="8"/>
-      <c r="H43" s="8"/>
-      <c r="I43" s="8"/>
-      <c r="J43" s="8"/>
-      <c r="K43" s="8"/>
-      <c r="L43" s="8"/>
-      <c r="M43" s="8"/>
-      <c r="N43" s="8"/>
-      <c r="O43" s="8"/>
-      <c r="P43" s="8"/>
+      <c r="B43" s="9"/>
+      <c r="C43" s="9"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
+      <c r="G43" s="9"/>
+      <c r="H43" s="9"/>
+      <c r="I43" s="9"/>
+      <c r="J43" s="9"/>
+      <c r="K43" s="9"/>
+      <c r="L43" s="9"/>
+      <c r="M43" s="9"/>
+      <c r="N43" s="9"/>
+      <c r="O43" s="9"/>
+      <c r="P43" s="9"/>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
-      <c r="B44" s="8"/>
-      <c r="C44" s="8"/>
-      <c r="D44" s="8"/>
-      <c r="E44" s="8"/>
-      <c r="F44" s="8"/>
-      <c r="G44" s="8"/>
-      <c r="H44" s="8"/>
-      <c r="I44" s="8"/>
-      <c r="J44" s="8"/>
-      <c r="K44" s="8"/>
-      <c r="L44" s="8"/>
-      <c r="M44" s="8"/>
-      <c r="N44" s="8"/>
-      <c r="O44" s="8"/>
-      <c r="P44" s="8"/>
+      <c r="B44" s="9"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="9"/>
+      <c r="F44" s="9"/>
+      <c r="G44" s="9"/>
+      <c r="H44" s="9"/>
+      <c r="I44" s="9"/>
+      <c r="J44" s="9"/>
+      <c r="K44" s="9"/>
+      <c r="L44" s="9"/>
+      <c r="M44" s="9"/>
+      <c r="N44" s="9"/>
+      <c r="O44" s="9"/>
+      <c r="P44" s="9"/>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
-      <c r="B45" s="8"/>
-      <c r="C45" s="8"/>
-      <c r="D45" s="8"/>
-      <c r="E45" s="8"/>
-      <c r="F45" s="8"/>
-      <c r="G45" s="8"/>
-      <c r="H45" s="8"/>
-      <c r="I45" s="8"/>
-      <c r="J45" s="8"/>
-      <c r="K45" s="8"/>
-      <c r="L45" s="8"/>
-      <c r="M45" s="8"/>
-      <c r="N45" s="8"/>
-      <c r="O45" s="8"/>
-      <c r="P45" s="8"/>
+      <c r="B45" s="9"/>
+      <c r="C45" s="9"/>
+      <c r="D45" s="9"/>
+      <c r="E45" s="9"/>
+      <c r="F45" s="9"/>
+      <c r="G45" s="9"/>
+      <c r="H45" s="9"/>
+      <c r="I45" s="9"/>
+      <c r="J45" s="9"/>
+      <c r="K45" s="9"/>
+      <c r="L45" s="9"/>
+      <c r="M45" s="9"/>
+      <c r="N45" s="9"/>
+      <c r="O45" s="9"/>
+      <c r="P45" s="9"/>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
-      <c r="B46" s="8"/>
-      <c r="C46" s="8"/>
-      <c r="D46" s="8"/>
-      <c r="E46" s="8"/>
-      <c r="F46" s="8"/>
-      <c r="G46" s="8"/>
-      <c r="H46" s="8"/>
-      <c r="I46" s="8"/>
-      <c r="J46" s="8"/>
-      <c r="K46" s="8"/>
-      <c r="L46" s="8"/>
-      <c r="M46" s="8"/>
-      <c r="N46" s="8"/>
-      <c r="O46" s="8"/>
-      <c r="P46" s="8"/>
+      <c r="B46" s="9"/>
+      <c r="C46" s="9"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="9"/>
+      <c r="F46" s="9"/>
+      <c r="G46" s="9"/>
+      <c r="H46" s="9"/>
+      <c r="I46" s="9"/>
+      <c r="J46" s="9"/>
+      <c r="K46" s="9"/>
+      <c r="L46" s="9"/>
+      <c r="M46" s="9"/>
+      <c r="N46" s="9"/>
+      <c r="O46" s="9"/>
+      <c r="P46" s="9"/>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
-      <c r="B47" s="8"/>
-      <c r="C47" s="8"/>
-      <c r="D47" s="8"/>
-      <c r="E47" s="8"/>
-      <c r="F47" s="8"/>
-      <c r="G47" s="8"/>
-      <c r="H47" s="8"/>
-      <c r="I47" s="8"/>
-      <c r="J47" s="8"/>
-      <c r="K47" s="8"/>
-      <c r="L47" s="8"/>
-      <c r="M47" s="8"/>
-      <c r="N47" s="8"/>
-      <c r="O47" s="8"/>
-      <c r="P47" s="8"/>
+      <c r="B47" s="9"/>
+      <c r="C47" s="9"/>
+      <c r="D47" s="9"/>
+      <c r="E47" s="9"/>
+      <c r="F47" s="9"/>
+      <c r="G47" s="9"/>
+      <c r="H47" s="9"/>
+      <c r="I47" s="9"/>
+      <c r="J47" s="9"/>
+      <c r="K47" s="9"/>
+      <c r="L47" s="9"/>
+      <c r="M47" s="9"/>
+      <c r="N47" s="9"/>
+      <c r="O47" s="9"/>
+      <c r="P47" s="9"/>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
-      <c r="B48" s="8"/>
-      <c r="C48" s="8"/>
-      <c r="D48" s="8"/>
-      <c r="E48" s="8"/>
-      <c r="F48" s="8"/>
-      <c r="G48" s="8"/>
-      <c r="H48" s="8"/>
-      <c r="I48" s="8"/>
-      <c r="J48" s="8"/>
-      <c r="K48" s="8"/>
-      <c r="L48" s="8"/>
-      <c r="M48" s="8"/>
-      <c r="N48" s="8"/>
-      <c r="O48" s="8"/>
-      <c r="P48" s="8"/>
+      <c r="B48" s="9"/>
+      <c r="C48" s="9"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="9"/>
+      <c r="G48" s="9"/>
+      <c r="H48" s="9"/>
+      <c r="I48" s="9"/>
+      <c r="J48" s="9"/>
+      <c r="K48" s="9"/>
+      <c r="L48" s="9"/>
+      <c r="M48" s="9"/>
+      <c r="N48" s="9"/>
+      <c r="O48" s="9"/>
+      <c r="P48" s="9"/>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
-      <c r="B49" s="8"/>
-      <c r="C49" s="8"/>
-      <c r="D49" s="8"/>
-      <c r="E49" s="8"/>
-      <c r="F49" s="8"/>
-      <c r="G49" s="8"/>
-      <c r="H49" s="8"/>
-      <c r="I49" s="8"/>
-      <c r="J49" s="8"/>
-      <c r="K49" s="8"/>
-      <c r="L49" s="8"/>
-      <c r="M49" s="8"/>
-      <c r="N49" s="8"/>
-      <c r="O49" s="8"/>
-      <c r="P49" s="8"/>
+      <c r="B49" s="9"/>
+      <c r="C49" s="9"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="9"/>
+      <c r="F49" s="9"/>
+      <c r="G49" s="9"/>
+      <c r="H49" s="9"/>
+      <c r="I49" s="9"/>
+      <c r="J49" s="9"/>
+      <c r="K49" s="9"/>
+      <c r="L49" s="9"/>
+      <c r="M49" s="9"/>
+      <c r="N49" s="9"/>
+      <c r="O49" s="9"/>
+      <c r="P49" s="9"/>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
-      <c r="B50" s="8"/>
-      <c r="C50" s="8"/>
-      <c r="D50" s="8"/>
-      <c r="E50" s="8"/>
-      <c r="F50" s="8"/>
-      <c r="G50" s="8"/>
-      <c r="H50" s="8"/>
-      <c r="I50" s="8"/>
-      <c r="J50" s="8"/>
-      <c r="K50" s="8"/>
-      <c r="L50" s="8"/>
-      <c r="M50" s="8"/>
-      <c r="N50" s="8"/>
-      <c r="O50" s="8"/>
-      <c r="P50" s="8"/>
+      <c r="B50" s="9"/>
+      <c r="C50" s="9"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="9"/>
+      <c r="F50" s="9"/>
+      <c r="G50" s="9"/>
+      <c r="H50" s="9"/>
+      <c r="I50" s="9"/>
+      <c r="J50" s="9"/>
+      <c r="K50" s="9"/>
+      <c r="L50" s="9"/>
+      <c r="M50" s="9"/>
+      <c r="N50" s="9"/>
+      <c r="O50" s="9"/>
+      <c r="P50" s="9"/>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
-      <c r="B51" s="8"/>
-      <c r="C51" s="8"/>
-      <c r="D51" s="8"/>
-      <c r="E51" s="8"/>
-      <c r="F51" s="8"/>
-      <c r="G51" s="8"/>
-      <c r="H51" s="8"/>
-      <c r="I51" s="8"/>
-      <c r="J51" s="8"/>
-      <c r="K51" s="8"/>
-      <c r="L51" s="8"/>
-      <c r="M51" s="8"/>
-      <c r="N51" s="8"/>
-      <c r="O51" s="8"/>
-      <c r="P51" s="8"/>
+      <c r="B51" s="9"/>
+      <c r="C51" s="9"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="9"/>
+      <c r="F51" s="9"/>
+      <c r="G51" s="9"/>
+      <c r="H51" s="9"/>
+      <c r="I51" s="9"/>
+      <c r="J51" s="9"/>
+      <c r="K51" s="9"/>
+      <c r="L51" s="9"/>
+      <c r="M51" s="9"/>
+      <c r="N51" s="9"/>
+      <c r="O51" s="9"/>
+      <c r="P51" s="9"/>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
-      <c r="B52" s="8"/>
-      <c r="C52" s="8"/>
-      <c r="D52" s="8"/>
-      <c r="E52" s="8"/>
-      <c r="F52" s="8"/>
-      <c r="G52" s="8"/>
-      <c r="H52" s="8"/>
-      <c r="I52" s="8"/>
-      <c r="J52" s="8"/>
-      <c r="K52" s="8"/>
-      <c r="L52" s="8"/>
-      <c r="M52" s="8"/>
-      <c r="N52" s="8"/>
-      <c r="O52" s="8"/>
-      <c r="P52" s="8"/>
+      <c r="B52" s="9"/>
+      <c r="C52" s="9"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="9"/>
+      <c r="F52" s="9"/>
+      <c r="G52" s="9"/>
+      <c r="H52" s="9"/>
+      <c r="I52" s="9"/>
+      <c r="J52" s="9"/>
+      <c r="K52" s="9"/>
+      <c r="L52" s="9"/>
+      <c r="M52" s="9"/>
+      <c r="N52" s="9"/>
+      <c r="O52" s="9"/>
+      <c r="P52" s="9"/>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
-      <c r="B53" s="8"/>
-      <c r="C53" s="8"/>
-      <c r="D53" s="8"/>
-      <c r="E53" s="8"/>
-      <c r="F53" s="8"/>
-      <c r="G53" s="8"/>
-      <c r="H53" s="8"/>
-      <c r="I53" s="8"/>
-      <c r="J53" s="8"/>
-      <c r="K53" s="8"/>
-      <c r="L53" s="8"/>
-      <c r="M53" s="8"/>
-      <c r="N53" s="8"/>
-      <c r="O53" s="8"/>
-      <c r="P53" s="8"/>
+      <c r="B53" s="9"/>
+      <c r="C53" s="9"/>
+      <c r="D53" s="9"/>
+      <c r="E53" s="9"/>
+      <c r="F53" s="9"/>
+      <c r="G53" s="9"/>
+      <c r="H53" s="9"/>
+      <c r="I53" s="9"/>
+      <c r="J53" s="9"/>
+      <c r="K53" s="9"/>
+      <c r="L53" s="9"/>
+      <c r="M53" s="9"/>
+      <c r="N53" s="9"/>
+      <c r="O53" s="9"/>
+      <c r="P53" s="9"/>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
-      <c r="B54" s="8"/>
-      <c r="C54" s="8"/>
-      <c r="D54" s="8"/>
-      <c r="E54" s="8"/>
-      <c r="F54" s="8"/>
-      <c r="G54" s="8"/>
-      <c r="H54" s="8"/>
-      <c r="I54" s="8"/>
-      <c r="J54" s="8"/>
-      <c r="K54" s="8"/>
-      <c r="L54" s="8"/>
-      <c r="M54" s="8"/>
-      <c r="N54" s="8"/>
-      <c r="O54" s="8"/>
-      <c r="P54" s="8"/>
+      <c r="B54" s="9"/>
+      <c r="C54" s="9"/>
+      <c r="D54" s="9"/>
+      <c r="E54" s="9"/>
+      <c r="F54" s="9"/>
+      <c r="G54" s="9"/>
+      <c r="H54" s="9"/>
+      <c r="I54" s="9"/>
+      <c r="J54" s="9"/>
+      <c r="K54" s="9"/>
+      <c r="L54" s="9"/>
+      <c r="M54" s="9"/>
+      <c r="N54" s="9"/>
+      <c r="O54" s="9"/>
+      <c r="P54" s="9"/>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
-      <c r="B55" s="8"/>
-      <c r="C55" s="8"/>
-      <c r="D55" s="8"/>
-      <c r="E55" s="8"/>
-      <c r="F55" s="8"/>
-      <c r="G55" s="8"/>
-      <c r="H55" s="8"/>
-      <c r="I55" s="8"/>
-      <c r="J55" s="8"/>
-      <c r="K55" s="8"/>
-      <c r="L55" s="8"/>
-      <c r="M55" s="8"/>
-      <c r="N55" s="8"/>
-      <c r="O55" s="8"/>
-      <c r="P55" s="8"/>
+      <c r="B55" s="9"/>
+      <c r="C55" s="9"/>
+      <c r="D55" s="9"/>
+      <c r="E55" s="9"/>
+      <c r="F55" s="9"/>
+      <c r="G55" s="9"/>
+      <c r="H55" s="9"/>
+      <c r="I55" s="9"/>
+      <c r="J55" s="9"/>
+      <c r="K55" s="9"/>
+      <c r="L55" s="9"/>
+      <c r="M55" s="9"/>
+      <c r="N55" s="9"/>
+      <c r="O55" s="9"/>
+      <c r="P55" s="9"/>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
-      <c r="B56" s="8"/>
-      <c r="C56" s="8"/>
-      <c r="D56" s="8"/>
-      <c r="E56" s="8"/>
-      <c r="F56" s="8"/>
-      <c r="G56" s="8"/>
-      <c r="H56" s="8"/>
-      <c r="I56" s="8"/>
-      <c r="J56" s="8"/>
-      <c r="K56" s="8"/>
-      <c r="L56" s="8"/>
-      <c r="M56" s="8"/>
-      <c r="N56" s="8"/>
-      <c r="O56" s="8"/>
-      <c r="P56" s="8"/>
+      <c r="B56" s="9"/>
+      <c r="C56" s="9"/>
+      <c r="D56" s="9"/>
+      <c r="E56" s="9"/>
+      <c r="F56" s="9"/>
+      <c r="G56" s="9"/>
+      <c r="H56" s="9"/>
+      <c r="I56" s="9"/>
+      <c r="J56" s="9"/>
+      <c r="K56" s="9"/>
+      <c r="L56" s="9"/>
+      <c r="M56" s="9"/>
+      <c r="N56" s="9"/>
+      <c r="O56" s="9"/>
+      <c r="P56" s="9"/>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
-      <c r="B57" s="8"/>
-      <c r="C57" s="8"/>
-      <c r="D57" s="8"/>
-      <c r="E57" s="8"/>
-      <c r="F57" s="8"/>
-      <c r="G57" s="8"/>
-      <c r="H57" s="8"/>
-      <c r="I57" s="8"/>
-      <c r="J57" s="8"/>
-      <c r="K57" s="8"/>
-      <c r="L57" s="8"/>
-      <c r="M57" s="8"/>
-      <c r="N57" s="8"/>
-      <c r="O57" s="8"/>
-      <c r="P57" s="8"/>
+      <c r="B57" s="9"/>
+      <c r="C57" s="9"/>
+      <c r="D57" s="9"/>
+      <c r="E57" s="9"/>
+      <c r="F57" s="9"/>
+      <c r="G57" s="9"/>
+      <c r="H57" s="9"/>
+      <c r="I57" s="9"/>
+      <c r="J57" s="9"/>
+      <c r="K57" s="9"/>
+      <c r="L57" s="9"/>
+      <c r="M57" s="9"/>
+      <c r="N57" s="9"/>
+      <c r="O57" s="9"/>
+      <c r="P57" s="9"/>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
-      <c r="B58" s="8"/>
-      <c r="C58" s="8"/>
-      <c r="D58" s="8"/>
-      <c r="E58" s="8"/>
-      <c r="F58" s="8"/>
-      <c r="G58" s="8"/>
-      <c r="H58" s="8"/>
-      <c r="I58" s="8"/>
-      <c r="J58" s="8"/>
-      <c r="K58" s="8"/>
-      <c r="L58" s="8"/>
-      <c r="M58" s="8"/>
-      <c r="N58" s="8"/>
-      <c r="O58" s="8"/>
-      <c r="P58" s="8"/>
+      <c r="B58" s="9"/>
+      <c r="C58" s="9"/>
+      <c r="D58" s="9"/>
+      <c r="E58" s="9"/>
+      <c r="F58" s="9"/>
+      <c r="G58" s="9"/>
+      <c r="H58" s="9"/>
+      <c r="I58" s="9"/>
+      <c r="J58" s="9"/>
+      <c r="K58" s="9"/>
+      <c r="L58" s="9"/>
+      <c r="M58" s="9"/>
+      <c r="N58" s="9"/>
+      <c r="O58" s="9"/>
+      <c r="P58" s="9"/>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
-      <c r="B59" s="8"/>
-      <c r="C59" s="8"/>
-      <c r="D59" s="8"/>
-      <c r="E59" s="8"/>
-      <c r="F59" s="8"/>
-      <c r="G59" s="8"/>
-      <c r="H59" s="8"/>
-      <c r="I59" s="8"/>
-      <c r="J59" s="8"/>
-      <c r="K59" s="8"/>
-      <c r="L59" s="8"/>
-      <c r="M59" s="8"/>
-      <c r="N59" s="8"/>
-      <c r="O59" s="8"/>
-      <c r="P59" s="8"/>
+      <c r="B59" s="9"/>
+      <c r="C59" s="9"/>
+      <c r="D59" s="9"/>
+      <c r="E59" s="9"/>
+      <c r="F59" s="9"/>
+      <c r="G59" s="9"/>
+      <c r="H59" s="9"/>
+      <c r="I59" s="9"/>
+      <c r="J59" s="9"/>
+      <c r="K59" s="9"/>
+      <c r="L59" s="9"/>
+      <c r="M59" s="9"/>
+      <c r="N59" s="9"/>
+      <c r="O59" s="9"/>
+      <c r="P59" s="9"/>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
-      <c r="B60" s="8"/>
-      <c r="C60" s="8"/>
-      <c r="D60" s="8"/>
-      <c r="E60" s="8"/>
-      <c r="F60" s="8"/>
-      <c r="G60" s="8"/>
-      <c r="H60" s="8"/>
-      <c r="I60" s="8"/>
-      <c r="J60" s="8"/>
-      <c r="K60" s="8"/>
-      <c r="L60" s="8"/>
-      <c r="M60" s="8"/>
-      <c r="N60" s="8"/>
-      <c r="O60" s="8"/>
-      <c r="P60" s="8"/>
+      <c r="B60" s="9"/>
+      <c r="C60" s="9"/>
+      <c r="D60" s="9"/>
+      <c r="E60" s="9"/>
+      <c r="F60" s="9"/>
+      <c r="G60" s="9"/>
+      <c r="H60" s="9"/>
+      <c r="I60" s="9"/>
+      <c r="J60" s="9"/>
+      <c r="K60" s="9"/>
+      <c r="L60" s="9"/>
+      <c r="M60" s="9"/>
+      <c r="N60" s="9"/>
+      <c r="O60" s="9"/>
+      <c r="P60" s="9"/>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
-      <c r="B61" s="8"/>
-      <c r="C61" s="8"/>
-      <c r="D61" s="8"/>
-      <c r="E61" s="8"/>
-      <c r="F61" s="8"/>
-      <c r="G61" s="8"/>
-      <c r="H61" s="8"/>
-      <c r="I61" s="8"/>
-      <c r="J61" s="8"/>
-      <c r="K61" s="8"/>
-      <c r="L61" s="8"/>
-      <c r="M61" s="8"/>
-      <c r="N61" s="8"/>
-      <c r="O61" s="8"/>
-      <c r="P61" s="8"/>
+      <c r="B61" s="9"/>
+      <c r="C61" s="9"/>
+      <c r="D61" s="9"/>
+      <c r="E61" s="9"/>
+      <c r="F61" s="9"/>
+      <c r="G61" s="9"/>
+      <c r="H61" s="9"/>
+      <c r="I61" s="9"/>
+      <c r="J61" s="9"/>
+      <c r="K61" s="9"/>
+      <c r="L61" s="9"/>
+      <c r="M61" s="9"/>
+      <c r="N61" s="9"/>
+      <c r="O61" s="9"/>
+      <c r="P61" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="60">
+    <mergeCell ref="B61:P61"/>
+    <mergeCell ref="B50:P50"/>
+    <mergeCell ref="B51:P51"/>
+    <mergeCell ref="B52:P52"/>
+    <mergeCell ref="B53:P53"/>
+    <mergeCell ref="B54:P54"/>
+    <mergeCell ref="B55:P55"/>
+    <mergeCell ref="B56:P56"/>
+    <mergeCell ref="B57:P57"/>
+    <mergeCell ref="B58:P58"/>
+    <mergeCell ref="B59:P59"/>
+    <mergeCell ref="B60:P60"/>
+    <mergeCell ref="B49:P49"/>
+    <mergeCell ref="B38:P38"/>
+    <mergeCell ref="B39:P39"/>
+    <mergeCell ref="B40:P40"/>
+    <mergeCell ref="B41:P41"/>
+    <mergeCell ref="B42:P42"/>
+    <mergeCell ref="B43:P43"/>
+    <mergeCell ref="B44:P44"/>
+    <mergeCell ref="B45:P45"/>
+    <mergeCell ref="B46:P46"/>
+    <mergeCell ref="B47:P47"/>
+    <mergeCell ref="B48:P48"/>
+    <mergeCell ref="B37:P37"/>
+    <mergeCell ref="B26:P26"/>
+    <mergeCell ref="B27:P27"/>
+    <mergeCell ref="B28:P28"/>
+    <mergeCell ref="B29:P29"/>
+    <mergeCell ref="B30:P30"/>
+    <mergeCell ref="B31:P31"/>
+    <mergeCell ref="B32:P32"/>
+    <mergeCell ref="B33:P33"/>
+    <mergeCell ref="B34:P34"/>
+    <mergeCell ref="B35:P35"/>
+    <mergeCell ref="B36:P36"/>
+    <mergeCell ref="B25:P25"/>
+    <mergeCell ref="B14:P14"/>
+    <mergeCell ref="B15:P15"/>
+    <mergeCell ref="B16:P16"/>
+    <mergeCell ref="B17:P17"/>
+    <mergeCell ref="B18:P18"/>
+    <mergeCell ref="B19:P19"/>
+    <mergeCell ref="B20:P20"/>
+    <mergeCell ref="B21:P21"/>
+    <mergeCell ref="B22:P22"/>
+    <mergeCell ref="B23:P23"/>
+    <mergeCell ref="B24:P24"/>
     <mergeCell ref="B13:P13"/>
     <mergeCell ref="B2:P2"/>
     <mergeCell ref="B3:P3"/>
@@ -3325,54 +3381,6 @@
     <mergeCell ref="B10:P10"/>
     <mergeCell ref="B11:P11"/>
     <mergeCell ref="B12:P12"/>
-    <mergeCell ref="B25:P25"/>
-    <mergeCell ref="B14:P14"/>
-    <mergeCell ref="B15:P15"/>
-    <mergeCell ref="B16:P16"/>
-    <mergeCell ref="B17:P17"/>
-    <mergeCell ref="B18:P18"/>
-    <mergeCell ref="B19:P19"/>
-    <mergeCell ref="B20:P20"/>
-    <mergeCell ref="B21:P21"/>
-    <mergeCell ref="B22:P22"/>
-    <mergeCell ref="B23:P23"/>
-    <mergeCell ref="B24:P24"/>
-    <mergeCell ref="B37:P37"/>
-    <mergeCell ref="B26:P26"/>
-    <mergeCell ref="B27:P27"/>
-    <mergeCell ref="B28:P28"/>
-    <mergeCell ref="B29:P29"/>
-    <mergeCell ref="B30:P30"/>
-    <mergeCell ref="B31:P31"/>
-    <mergeCell ref="B32:P32"/>
-    <mergeCell ref="B33:P33"/>
-    <mergeCell ref="B34:P34"/>
-    <mergeCell ref="B35:P35"/>
-    <mergeCell ref="B36:P36"/>
-    <mergeCell ref="B49:P49"/>
-    <mergeCell ref="B38:P38"/>
-    <mergeCell ref="B39:P39"/>
-    <mergeCell ref="B40:P40"/>
-    <mergeCell ref="B41:P41"/>
-    <mergeCell ref="B42:P42"/>
-    <mergeCell ref="B43:P43"/>
-    <mergeCell ref="B44:P44"/>
-    <mergeCell ref="B45:P45"/>
-    <mergeCell ref="B46:P46"/>
-    <mergeCell ref="B47:P47"/>
-    <mergeCell ref="B48:P48"/>
-    <mergeCell ref="B61:P61"/>
-    <mergeCell ref="B50:P50"/>
-    <mergeCell ref="B51:P51"/>
-    <mergeCell ref="B52:P52"/>
-    <mergeCell ref="B53:P53"/>
-    <mergeCell ref="B54:P54"/>
-    <mergeCell ref="B55:P55"/>
-    <mergeCell ref="B56:P56"/>
-    <mergeCell ref="B57:P57"/>
-    <mergeCell ref="B58:P58"/>
-    <mergeCell ref="B59:P59"/>
-    <mergeCell ref="B60:P60"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Některé připomínky viz WorkSheet.xlsx
</commit_message>
<xml_diff>
--- a/MDM/WorkSheet.xlsx
+++ b/MDM/WorkSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7635" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24240" windowHeight="12210" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="WorkSheet" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="80">
   <si>
     <t>Úvodní schůze</t>
   </si>
@@ -225,6 +225,36 @@
   </si>
   <si>
     <t>Pro roli Super administrátora vytvořit možnost nasatvení času definujícího dobu trvání procedrur pro její započtení a času, který určuje délka přestávky mezi započtenými procedurami. (Hotovo, nelze zakódovat, v konfiguraci chybí IP adresa a přidání/ubrání jazyka)</t>
+  </si>
+  <si>
+    <t>Do Nastavení konfigurace přidat možnost nastavení určité IP adresy LAN desky.</t>
+  </si>
+  <si>
+    <t>Odstranit hlášky "Zapínání kanálu X" při inicializaci programu.</t>
+  </si>
+  <si>
+    <t>V dialogu tvorby nového pacienta změnit nadpis "Sex" na "Pohlaví".</t>
+  </si>
+  <si>
+    <t>V seznamu pacientů přidat sloupeček "Dokončeno", ve kterém se bude zobrazovat označení (např. fajvka) u daného pacienta, který již dokončil všech 13 procedur. Takového pacienta nebude možné vybrat k další proceduře.</t>
+  </si>
+  <si>
+    <t>Výstražný zvuk změnit na jedno důrazné "pípnutí".</t>
+  </si>
+  <si>
+    <t>Odstranit hlášku "Pacient dokončil proceduru číslo 0 v 0. cyklu za 0 minut a 0 sekund" vyvolanou chybovým hlášením: Chyba přístorj MDM nereaguje (viz. obrázek)</t>
+  </si>
+  <si>
+    <t>Výstražný zvuk přidat ke všem chybový hlášením.(stačí pouze jedno pípnutí).</t>
+  </si>
+  <si>
+    <t>Pro roli Uživatel upravit Stavové pole průběhu: odstranit ukazatel času do změny segmentu a možná i uplynulého času.</t>
+  </si>
+  <si>
+    <t>Při přechodu ze šesti použitelných kanálů na méně zanechat zobrazení všech kanálů. Nepřístupné kanály označit hláškou "Nepřístupný"(nebo "Vypnutý").</t>
+  </si>
+  <si>
+    <t>Přidat upozornění pro uživatele, že není přihlášen, pokud se omylem po vybrání pacienta odhlásí. V tu chvíli se znemožní používání tlačítek pro ovládání procedury (zešednou) a uživatel by mohl být zmatený. (zabráněno odhlášení)</t>
   </si>
 </sst>
 </file>
@@ -397,7 +427,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="46">
+  <fills count="47">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -652,6 +682,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF99FF66"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -816,7 +852,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="3" applyAlignment="1">
@@ -847,29 +883,54 @@
     <xf numFmtId="0" fontId="18" fillId="43" borderId="0" xfId="7" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="44" borderId="0" xfId="7" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="45" borderId="0" xfId="7" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="46" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="5"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="46" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="5"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="5"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="5"/>
+      <alignment horizontal="left" vertical="top" indent="5"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -941,6 +1002,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>7392</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>7175</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>519954</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>86114</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Obrázek 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1053FDDA-A9AC-4562-AAF3-9412BEC8FAC0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="616992" y="10648281"/>
+          <a:ext cx="5998962" cy="3386916"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1230,10 +1340,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H110"/>
+  <dimension ref="A1:H111"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="A110" sqref="A110:C110"/>
+      <selection activeCell="A111" sqref="A111:C111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1271,11 +1381,11 @@
       </c>
       <c r="F2" s="4">
         <f>SUM(C:C)</f>
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="H2" s="5">
         <f>F2*300</f>
-        <v>143400</v>
+        <v>144000</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -2245,6 +2355,14 @@
       </c>
       <c r="C110">
         <v>4</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" s="1">
+        <v>42968</v>
+      </c>
+      <c r="C111">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -2254,10 +2372,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:P63"/>
+  <dimension ref="A2:P69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57:P57"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62:P62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2269,592 +2387,592 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="21"/>
-      <c r="N2" s="21"/>
-      <c r="O2" s="21"/>
-      <c r="P2" s="21"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="26"/>
+      <c r="M2" s="26"/>
+      <c r="N2" s="26"/>
+      <c r="O2" s="26"/>
+      <c r="P2" s="26"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>2</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="20"/>
-      <c r="M3" s="20"/>
-      <c r="N3" s="20"/>
-      <c r="O3" s="20"/>
-      <c r="P3" s="20"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="28"/>
+      <c r="M3" s="28"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="28"/>
+      <c r="P3" s="28"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>3</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="20"/>
-      <c r="L4" s="20"/>
-      <c r="M4" s="20"/>
-      <c r="N4" s="20"/>
-      <c r="O4" s="20"/>
-      <c r="P4" s="20"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="28"/>
+      <c r="L4" s="28"/>
+      <c r="M4" s="28"/>
+      <c r="N4" s="28"/>
+      <c r="O4" s="28"/>
+      <c r="P4" s="28"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>4</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="20"/>
-      <c r="M5" s="20"/>
-      <c r="N5" s="20"/>
-      <c r="O5" s="20"/>
-      <c r="P5" s="20"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="28"/>
+      <c r="J5" s="28"/>
+      <c r="K5" s="28"/>
+      <c r="L5" s="28"/>
+      <c r="M5" s="28"/>
+      <c r="N5" s="28"/>
+      <c r="O5" s="28"/>
+      <c r="P5" s="28"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>5</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="20"/>
-      <c r="L6" s="20"/>
-      <c r="M6" s="20"/>
-      <c r="N6" s="20"/>
-      <c r="O6" s="20"/>
-      <c r="P6" s="20"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="28"/>
+      <c r="K6" s="28"/>
+      <c r="L6" s="28"/>
+      <c r="M6" s="28"/>
+      <c r="N6" s="28"/>
+      <c r="O6" s="28"/>
+      <c r="P6" s="28"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>6</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="20"/>
-      <c r="L7" s="20"/>
-      <c r="M7" s="20"/>
-      <c r="N7" s="20"/>
-      <c r="O7" s="20"/>
-      <c r="P7" s="20"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="28"/>
+      <c r="L7" s="28"/>
+      <c r="M7" s="28"/>
+      <c r="N7" s="28"/>
+      <c r="O7" s="28"/>
+      <c r="P7" s="28"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>7</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="20"/>
-      <c r="M8" s="20"/>
-      <c r="N8" s="20"/>
-      <c r="O8" s="20"/>
-      <c r="P8" s="20"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
+      <c r="K8" s="28"/>
+      <c r="L8" s="28"/>
+      <c r="M8" s="28"/>
+      <c r="N8" s="28"/>
+      <c r="O8" s="28"/>
+      <c r="P8" s="28"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>8</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="20"/>
-      <c r="J9" s="20"/>
-      <c r="K9" s="20"/>
-      <c r="L9" s="20"/>
-      <c r="M9" s="20"/>
-      <c r="N9" s="20"/>
-      <c r="O9" s="20"/>
-      <c r="P9" s="20"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="28"/>
+      <c r="M9" s="28"/>
+      <c r="N9" s="28"/>
+      <c r="O9" s="28"/>
+      <c r="P9" s="28"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>9</v>
       </c>
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="22"/>
-      <c r="J10" s="22"/>
-      <c r="K10" s="22"/>
-      <c r="L10" s="22"/>
-      <c r="M10" s="22"/>
-      <c r="N10" s="22"/>
-      <c r="O10" s="22"/>
-      <c r="P10" s="22"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="31"/>
+      <c r="L10" s="31"/>
+      <c r="M10" s="31"/>
+      <c r="N10" s="31"/>
+      <c r="O10" s="31"/>
+      <c r="P10" s="31"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>10</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="20"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="20"/>
-      <c r="L11" s="20"/>
-      <c r="M11" s="20"/>
-      <c r="N11" s="20"/>
-      <c r="O11" s="20"/>
-      <c r="P11" s="20"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="28"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="28"/>
+      <c r="L11" s="28"/>
+      <c r="M11" s="28"/>
+      <c r="N11" s="28"/>
+      <c r="O11" s="28"/>
+      <c r="P11" s="28"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>11</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="20"/>
-      <c r="J12" s="20"/>
-      <c r="K12" s="20"/>
-      <c r="L12" s="20"/>
-      <c r="M12" s="20"/>
-      <c r="N12" s="20"/>
-      <c r="O12" s="20"/>
-      <c r="P12" s="20"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="28"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="28"/>
+      <c r="M12" s="28"/>
+      <c r="N12" s="28"/>
+      <c r="O12" s="28"/>
+      <c r="P12" s="28"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>12</v>
       </c>
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="20"/>
-      <c r="K13" s="20"/>
-      <c r="L13" s="20"/>
-      <c r="M13" s="20"/>
-      <c r="N13" s="20"/>
-      <c r="O13" s="20"/>
-      <c r="P13" s="20"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="28"/>
+      <c r="J13" s="28"/>
+      <c r="K13" s="28"/>
+      <c r="L13" s="28"/>
+      <c r="M13" s="28"/>
+      <c r="N13" s="28"/>
+      <c r="O13" s="28"/>
+      <c r="P13" s="28"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>13</v>
       </c>
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="20"/>
-      <c r="J14" s="20"/>
-      <c r="K14" s="20"/>
-      <c r="L14" s="20"/>
-      <c r="M14" s="20"/>
-      <c r="N14" s="20"/>
-      <c r="O14" s="20"/>
-      <c r="P14" s="20"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="28"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="28"/>
+      <c r="L14" s="28"/>
+      <c r="M14" s="28"/>
+      <c r="N14" s="28"/>
+      <c r="O14" s="28"/>
+      <c r="P14" s="28"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>14</v>
       </c>
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="22"/>
-      <c r="I15" s="22"/>
-      <c r="J15" s="22"/>
-      <c r="K15" s="22"/>
-      <c r="L15" s="22"/>
-      <c r="M15" s="22"/>
-      <c r="N15" s="22"/>
-      <c r="O15" s="22"/>
-      <c r="P15" s="22"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="31"/>
+      <c r="I15" s="31"/>
+      <c r="J15" s="31"/>
+      <c r="K15" s="31"/>
+      <c r="L15" s="31"/>
+      <c r="M15" s="31"/>
+      <c r="N15" s="31"/>
+      <c r="O15" s="31"/>
+      <c r="P15" s="31"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="21"/>
-      <c r="J16" s="21"/>
-      <c r="K16" s="21"/>
-      <c r="L16" s="21"/>
-      <c r="M16" s="21"/>
-      <c r="N16" s="21"/>
-      <c r="O16" s="21"/>
-      <c r="P16" s="21"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="26"/>
+      <c r="K16" s="26"/>
+      <c r="L16" s="26"/>
+      <c r="M16" s="26"/>
+      <c r="N16" s="26"/>
+      <c r="O16" s="26"/>
+      <c r="P16" s="26"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>16</v>
       </c>
-      <c r="B17" s="20" t="s">
+      <c r="B17" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="20"/>
-      <c r="I17" s="20"/>
-      <c r="J17" s="20"/>
-      <c r="K17" s="20"/>
-      <c r="L17" s="20"/>
-      <c r="M17" s="20"/>
-      <c r="N17" s="20"/>
-      <c r="O17" s="20"/>
-      <c r="P17" s="20"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="28"/>
+      <c r="J17" s="28"/>
+      <c r="K17" s="28"/>
+      <c r="L17" s="28"/>
+      <c r="M17" s="28"/>
+      <c r="N17" s="28"/>
+      <c r="O17" s="28"/>
+      <c r="P17" s="28"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <v>17</v>
       </c>
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="20"/>
-      <c r="J18" s="20"/>
-      <c r="K18" s="20"/>
-      <c r="L18" s="20"/>
-      <c r="M18" s="20"/>
-      <c r="N18" s="20"/>
-      <c r="O18" s="20"/>
-      <c r="P18" s="20"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="28"/>
+      <c r="J18" s="28"/>
+      <c r="K18" s="28"/>
+      <c r="L18" s="28"/>
+      <c r="M18" s="28"/>
+      <c r="N18" s="28"/>
+      <c r="O18" s="28"/>
+      <c r="P18" s="28"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>18</v>
       </c>
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="20"/>
-      <c r="J19" s="20"/>
-      <c r="K19" s="20"/>
-      <c r="L19" s="20"/>
-      <c r="M19" s="20"/>
-      <c r="N19" s="20"/>
-      <c r="O19" s="20"/>
-      <c r="P19" s="20"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="28"/>
+      <c r="K19" s="28"/>
+      <c r="L19" s="28"/>
+      <c r="M19" s="28"/>
+      <c r="N19" s="28"/>
+      <c r="O19" s="28"/>
+      <c r="P19" s="28"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
         <v>19</v>
       </c>
-      <c r="B20" s="20" t="s">
+      <c r="B20" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="20"/>
-      <c r="I20" s="20"/>
-      <c r="J20" s="20"/>
-      <c r="K20" s="20"/>
-      <c r="L20" s="20"/>
-      <c r="M20" s="20"/>
-      <c r="N20" s="20"/>
-      <c r="O20" s="20"/>
-      <c r="P20" s="20"/>
+      <c r="C20" s="28"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="28"/>
+      <c r="I20" s="28"/>
+      <c r="J20" s="28"/>
+      <c r="K20" s="28"/>
+      <c r="L20" s="28"/>
+      <c r="M20" s="28"/>
+      <c r="N20" s="28"/>
+      <c r="O20" s="28"/>
+      <c r="P20" s="28"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
         <v>20</v>
       </c>
-      <c r="B21" s="20" t="s">
+      <c r="B21" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
-      <c r="I21" s="20"/>
-      <c r="J21" s="20"/>
-      <c r="K21" s="20"/>
-      <c r="L21" s="20"/>
-      <c r="M21" s="20"/>
-      <c r="N21" s="20"/>
-      <c r="O21" s="20"/>
-      <c r="P21" s="20"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="28"/>
+      <c r="I21" s="28"/>
+      <c r="J21" s="28"/>
+      <c r="K21" s="28"/>
+      <c r="L21" s="28"/>
+      <c r="M21" s="28"/>
+      <c r="N21" s="28"/>
+      <c r="O21" s="28"/>
+      <c r="P21" s="28"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
         <v>21</v>
       </c>
-      <c r="B22" s="20" t="s">
+      <c r="B22" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="20"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="20"/>
-      <c r="K22" s="20"/>
-      <c r="L22" s="20"/>
-      <c r="M22" s="20"/>
-      <c r="N22" s="20"/>
-      <c r="O22" s="20"/>
-      <c r="P22" s="20"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="28"/>
+      <c r="H22" s="28"/>
+      <c r="I22" s="28"/>
+      <c r="J22" s="28"/>
+      <c r="K22" s="28"/>
+      <c r="L22" s="28"/>
+      <c r="M22" s="28"/>
+      <c r="N22" s="28"/>
+      <c r="O22" s="28"/>
+      <c r="P22" s="28"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="9">
         <v>22</v>
       </c>
-      <c r="B23" s="22" t="s">
+      <c r="B23" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="C23" s="22"/>
-      <c r="D23" s="22"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="22"/>
-      <c r="G23" s="22"/>
-      <c r="H23" s="22"/>
-      <c r="I23" s="22"/>
-      <c r="J23" s="22"/>
-      <c r="K23" s="22"/>
-      <c r="L23" s="22"/>
-      <c r="M23" s="22"/>
-      <c r="N23" s="22"/>
-      <c r="O23" s="22"/>
-      <c r="P23" s="22"/>
+      <c r="C23" s="31"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="31"/>
+      <c r="G23" s="31"/>
+      <c r="H23" s="31"/>
+      <c r="I23" s="31"/>
+      <c r="J23" s="31"/>
+      <c r="K23" s="31"/>
+      <c r="L23" s="31"/>
+      <c r="M23" s="31"/>
+      <c r="N23" s="31"/>
+      <c r="O23" s="31"/>
+      <c r="P23" s="31"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
         <v>23</v>
       </c>
-      <c r="B24" s="20" t="s">
+      <c r="B24" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="20"/>
-      <c r="I24" s="20"/>
-      <c r="J24" s="20"/>
-      <c r="K24" s="20"/>
-      <c r="L24" s="20"/>
-      <c r="M24" s="20"/>
-      <c r="N24" s="20"/>
-      <c r="O24" s="20"/>
-      <c r="P24" s="20"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="28"/>
+      <c r="H24" s="28"/>
+      <c r="I24" s="28"/>
+      <c r="J24" s="28"/>
+      <c r="K24" s="28"/>
+      <c r="L24" s="28"/>
+      <c r="M24" s="28"/>
+      <c r="N24" s="28"/>
+      <c r="O24" s="28"/>
+      <c r="P24" s="28"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="9">
         <v>24</v>
       </c>
-      <c r="B25" s="22" t="s">
+      <c r="B25" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="C25" s="22"/>
-      <c r="D25" s="22"/>
-      <c r="E25" s="22"/>
-      <c r="F25" s="22"/>
-      <c r="G25" s="22"/>
-      <c r="H25" s="22"/>
-      <c r="I25" s="22"/>
-      <c r="J25" s="22"/>
-      <c r="K25" s="22"/>
-      <c r="L25" s="22"/>
-      <c r="M25" s="22"/>
-      <c r="N25" s="22"/>
-      <c r="O25" s="22"/>
-      <c r="P25" s="22"/>
+      <c r="C25" s="31"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="31"/>
+      <c r="F25" s="31"/>
+      <c r="G25" s="31"/>
+      <c r="H25" s="31"/>
+      <c r="I25" s="31"/>
+      <c r="J25" s="31"/>
+      <c r="K25" s="31"/>
+      <c r="L25" s="31"/>
+      <c r="M25" s="31"/>
+      <c r="N25" s="31"/>
+      <c r="O25" s="31"/>
+      <c r="P25" s="31"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
         <v>25</v>
       </c>
-      <c r="B26" s="20" t="s">
+      <c r="B26" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20"/>
-      <c r="H26" s="20"/>
-      <c r="I26" s="20"/>
-      <c r="J26" s="20"/>
-      <c r="K26" s="20"/>
-      <c r="L26" s="20"/>
-      <c r="M26" s="20"/>
-      <c r="N26" s="20"/>
-      <c r="O26" s="20"/>
-      <c r="P26" s="20"/>
+      <c r="C26" s="28"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="28"/>
+      <c r="F26" s="28"/>
+      <c r="G26" s="28"/>
+      <c r="H26" s="28"/>
+      <c r="I26" s="28"/>
+      <c r="J26" s="28"/>
+      <c r="K26" s="28"/>
+      <c r="L26" s="28"/>
+      <c r="M26" s="28"/>
+      <c r="N26" s="28"/>
+      <c r="O26" s="28"/>
+      <c r="P26" s="28"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
-      <c r="B27" s="21"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="21"/>
-      <c r="I27" s="21"/>
-      <c r="J27" s="21"/>
-      <c r="K27" s="21"/>
-      <c r="L27" s="21"/>
-      <c r="M27" s="21"/>
-      <c r="N27" s="21"/>
-      <c r="O27" s="21"/>
-      <c r="P27" s="21"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="26"/>
+      <c r="G27" s="26"/>
+      <c r="H27" s="26"/>
+      <c r="I27" s="26"/>
+      <c r="J27" s="26"/>
+      <c r="K27" s="26"/>
+      <c r="L27" s="26"/>
+      <c r="M27" s="26"/>
+      <c r="N27" s="26"/>
+      <c r="O27" s="26"/>
+      <c r="P27" s="26"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A28">
+      <c r="A28" s="7">
         <v>27</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="8"/>
-      <c r="K28" s="8"/>
-      <c r="L28" s="8"/>
-      <c r="M28" s="8"/>
-      <c r="N28" s="8"/>
-      <c r="O28" s="8"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="24"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="24"/>
+      <c r="J28" s="24"/>
+      <c r="K28" s="24"/>
+      <c r="L28" s="24"/>
+      <c r="M28" s="24"/>
+      <c r="N28" s="24"/>
+      <c r="O28" s="24"/>
       <c r="P28" s="8"/>
     </row>
     <row r="29" spans="1:16" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
@@ -3367,156 +3485,156 @@
       <c r="A52">
         <v>28</v>
       </c>
-      <c r="B52" s="21"/>
-      <c r="C52" s="21"/>
-      <c r="D52" s="21"/>
-      <c r="E52" s="21"/>
-      <c r="F52" s="21"/>
-      <c r="G52" s="21"/>
-      <c r="H52" s="21"/>
-      <c r="I52" s="21"/>
-      <c r="J52" s="21"/>
-      <c r="K52" s="21"/>
-      <c r="L52" s="21"/>
-      <c r="M52" s="21"/>
-      <c r="N52" s="21"/>
-      <c r="O52" s="21"/>
-      <c r="P52" s="21"/>
+      <c r="B52" s="26"/>
+      <c r="C52" s="26"/>
+      <c r="D52" s="26"/>
+      <c r="E52" s="26"/>
+      <c r="F52" s="26"/>
+      <c r="G52" s="26"/>
+      <c r="H52" s="26"/>
+      <c r="I52" s="26"/>
+      <c r="J52" s="26"/>
+      <c r="K52" s="26"/>
+      <c r="L52" s="26"/>
+      <c r="M52" s="26"/>
+      <c r="N52" s="26"/>
+      <c r="O52" s="26"/>
+      <c r="P52" s="26"/>
     </row>
     <row r="53" spans="1:16" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="24">
+      <c r="A53" s="20">
         <v>29</v>
       </c>
-      <c r="B53" s="25" t="s">
+      <c r="B53" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="C53" s="25"/>
-      <c r="D53" s="25"/>
-      <c r="E53" s="25"/>
-      <c r="F53" s="25"/>
-      <c r="G53" s="25"/>
-      <c r="H53" s="25"/>
-      <c r="I53" s="25"/>
-      <c r="J53" s="25"/>
-      <c r="K53" s="25"/>
-      <c r="L53" s="25"/>
-      <c r="M53" s="25"/>
-      <c r="N53" s="25"/>
-      <c r="O53" s="25"/>
-      <c r="P53" s="25"/>
+      <c r="C53" s="30"/>
+      <c r="D53" s="30"/>
+      <c r="E53" s="30"/>
+      <c r="F53" s="30"/>
+      <c r="G53" s="30"/>
+      <c r="H53" s="30"/>
+      <c r="I53" s="30"/>
+      <c r="J53" s="30"/>
+      <c r="K53" s="30"/>
+      <c r="L53" s="30"/>
+      <c r="M53" s="30"/>
+      <c r="N53" s="30"/>
+      <c r="O53" s="30"/>
+      <c r="P53" s="30"/>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>30</v>
       </c>
-      <c r="B54" s="21" t="s">
+      <c r="B54" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="C54" s="21"/>
-      <c r="D54" s="21"/>
-      <c r="E54" s="21"/>
-      <c r="F54" s="21"/>
-      <c r="G54" s="21"/>
-      <c r="H54" s="21"/>
-      <c r="I54" s="21"/>
-      <c r="J54" s="21"/>
-      <c r="K54" s="21"/>
-      <c r="L54" s="21"/>
-      <c r="M54" s="21"/>
-      <c r="N54" s="21"/>
-      <c r="O54" s="21"/>
-      <c r="P54" s="21"/>
+      <c r="C54" s="26"/>
+      <c r="D54" s="26"/>
+      <c r="E54" s="26"/>
+      <c r="F54" s="26"/>
+      <c r="G54" s="26"/>
+      <c r="H54" s="26"/>
+      <c r="I54" s="26"/>
+      <c r="J54" s="26"/>
+      <c r="K54" s="26"/>
+      <c r="L54" s="26"/>
+      <c r="M54" s="26"/>
+      <c r="N54" s="26"/>
+      <c r="O54" s="26"/>
+      <c r="P54" s="26"/>
     </row>
     <row r="55" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="7">
+      <c r="A55" s="22">
         <v>31</v>
       </c>
-      <c r="B55" s="23" t="s">
+      <c r="B55" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="C55" s="23"/>
-      <c r="D55" s="23"/>
-      <c r="E55" s="23"/>
-      <c r="F55" s="23"/>
-      <c r="G55" s="23"/>
-      <c r="H55" s="23"/>
-      <c r="I55" s="23"/>
-      <c r="J55" s="23"/>
-      <c r="K55" s="23"/>
-      <c r="L55" s="23"/>
-      <c r="M55" s="23"/>
-      <c r="N55" s="23"/>
-      <c r="O55" s="23"/>
-      <c r="P55" s="23"/>
+      <c r="C55" s="29"/>
+      <c r="D55" s="29"/>
+      <c r="E55" s="29"/>
+      <c r="F55" s="29"/>
+      <c r="G55" s="29"/>
+      <c r="H55" s="29"/>
+      <c r="I55" s="29"/>
+      <c r="J55" s="29"/>
+      <c r="K55" s="29"/>
+      <c r="L55" s="29"/>
+      <c r="M55" s="29"/>
+      <c r="N55" s="29"/>
+      <c r="O55" s="29"/>
+      <c r="P55" s="29"/>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>32</v>
       </c>
-      <c r="B56" s="21" t="s">
+      <c r="B56" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="C56" s="21"/>
-      <c r="D56" s="21"/>
-      <c r="E56" s="21"/>
-      <c r="F56" s="21"/>
-      <c r="G56" s="21"/>
-      <c r="H56" s="21"/>
-      <c r="I56" s="21"/>
-      <c r="J56" s="21"/>
-      <c r="K56" s="21"/>
-      <c r="L56" s="21"/>
-      <c r="M56" s="21"/>
-      <c r="N56" s="21"/>
-      <c r="O56" s="21"/>
-      <c r="P56" s="21"/>
-    </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A57">
+      <c r="C56" s="26"/>
+      <c r="D56" s="26"/>
+      <c r="E56" s="26"/>
+      <c r="F56" s="26"/>
+      <c r="G56" s="26"/>
+      <c r="H56" s="26"/>
+      <c r="I56" s="26"/>
+      <c r="J56" s="26"/>
+      <c r="K56" s="26"/>
+      <c r="L56" s="26"/>
+      <c r="M56" s="26"/>
+      <c r="N56" s="26"/>
+      <c r="O56" s="26"/>
+      <c r="P56" s="26"/>
+    </row>
+    <row r="57" spans="1:16" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="7">
         <v>33</v>
       </c>
-      <c r="B57" s="21" t="s">
+      <c r="B57" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="C57" s="21"/>
-      <c r="D57" s="21"/>
-      <c r="E57" s="21"/>
-      <c r="F57" s="21"/>
-      <c r="G57" s="21"/>
-      <c r="H57" s="21"/>
-      <c r="I57" s="21"/>
-      <c r="J57" s="21"/>
-      <c r="K57" s="21"/>
-      <c r="L57" s="21"/>
-      <c r="M57" s="21"/>
-      <c r="N57" s="21"/>
-      <c r="O57" s="21"/>
-      <c r="P57" s="21"/>
+      <c r="C57" s="27"/>
+      <c r="D57" s="27"/>
+      <c r="E57" s="27"/>
+      <c r="F57" s="27"/>
+      <c r="G57" s="27"/>
+      <c r="H57" s="27"/>
+      <c r="I57" s="27"/>
+      <c r="J57" s="27"/>
+      <c r="K57" s="27"/>
+      <c r="L57" s="27"/>
+      <c r="M57" s="27"/>
+      <c r="N57" s="27"/>
+      <c r="O57" s="27"/>
+      <c r="P57" s="27"/>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A58">
+      <c r="A58" s="7">
         <v>34</v>
       </c>
-      <c r="B58" s="21" t="s">
+      <c r="B58" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="C58" s="21"/>
-      <c r="D58" s="21"/>
-      <c r="E58" s="21"/>
-      <c r="F58" s="21"/>
-      <c r="G58" s="21"/>
-      <c r="H58" s="21"/>
-      <c r="I58" s="21"/>
-      <c r="J58" s="21"/>
-      <c r="K58" s="21"/>
-      <c r="L58" s="21"/>
-      <c r="M58" s="21"/>
-      <c r="N58" s="21"/>
-      <c r="O58" s="21"/>
-      <c r="P58" s="21"/>
+      <c r="C58" s="28"/>
+      <c r="D58" s="28"/>
+      <c r="E58" s="28"/>
+      <c r="F58" s="28"/>
+      <c r="G58" s="28"/>
+      <c r="H58" s="28"/>
+      <c r="I58" s="28"/>
+      <c r="J58" s="28"/>
+      <c r="K58" s="28"/>
+      <c r="L58" s="28"/>
+      <c r="M58" s="28"/>
+      <c r="N58" s="28"/>
+      <c r="O58" s="28"/>
+      <c r="P58" s="28"/>
     </row>
     <row r="59" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="26">
+      <c r="A59" s="21">
         <v>35</v>
       </c>
       <c r="B59" s="27" t="s">
@@ -3537,73 +3655,252 @@
       <c r="O59" s="27"/>
       <c r="P59" s="27"/>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A60">
+    <row r="60" spans="1:16" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="35">
         <v>36</v>
       </c>
-      <c r="B60" s="21"/>
-      <c r="C60" s="21"/>
-      <c r="D60" s="21"/>
-      <c r="E60" s="21"/>
-      <c r="F60" s="21"/>
-      <c r="G60" s="21"/>
-      <c r="H60" s="21"/>
-      <c r="I60" s="21"/>
-      <c r="J60" s="21"/>
-      <c r="K60" s="21"/>
-      <c r="L60" s="21"/>
-      <c r="M60" s="21"/>
-      <c r="N60" s="21"/>
-      <c r="O60" s="21"/>
-      <c r="P60" s="21"/>
+      <c r="B60" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="C60" s="36"/>
+      <c r="D60" s="36"/>
+      <c r="E60" s="36"/>
+      <c r="F60" s="36"/>
+      <c r="G60" s="36"/>
+      <c r="H60" s="36"/>
+      <c r="I60" s="36"/>
+      <c r="J60" s="36"/>
+      <c r="K60" s="36"/>
+      <c r="L60" s="36"/>
+      <c r="M60" s="36"/>
+      <c r="N60" s="36"/>
+      <c r="O60" s="36"/>
+      <c r="P60" s="36"/>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A61">
+      <c r="A61" s="7">
         <v>37</v>
       </c>
-      <c r="B61" s="21"/>
-      <c r="C61" s="21"/>
-      <c r="D61" s="21"/>
-      <c r="E61" s="21"/>
-      <c r="F61" s="21"/>
-      <c r="G61" s="21"/>
-      <c r="H61" s="21"/>
-      <c r="I61" s="21"/>
-      <c r="J61" s="21"/>
-      <c r="K61" s="21"/>
-      <c r="L61" s="21"/>
-      <c r="M61" s="21"/>
-      <c r="N61" s="21"/>
-      <c r="O61" s="21"/>
-      <c r="P61" s="21"/>
+      <c r="B61" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="C61" s="28"/>
+      <c r="D61" s="28"/>
+      <c r="E61" s="28"/>
+      <c r="F61" s="28"/>
+      <c r="G61" s="28"/>
+      <c r="H61" s="28"/>
+      <c r="I61" s="28"/>
+      <c r="J61" s="28"/>
+      <c r="K61" s="28"/>
+      <c r="L61" s="28"/>
+      <c r="M61" s="28"/>
+      <c r="N61" s="28"/>
+      <c r="O61" s="28"/>
+      <c r="P61" s="28"/>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A62">
+      <c r="A62" s="7">
         <v>38</v>
       </c>
-      <c r="B62" s="21"/>
-      <c r="C62" s="21"/>
-      <c r="D62" s="21"/>
-      <c r="E62" s="21"/>
-      <c r="F62" s="21"/>
-      <c r="G62" s="21"/>
-      <c r="H62" s="21"/>
-      <c r="I62" s="21"/>
-      <c r="J62" s="21"/>
-      <c r="K62" s="21"/>
-      <c r="L62" s="21"/>
-      <c r="M62" s="21"/>
-      <c r="N62" s="21"/>
-      <c r="O62" s="21"/>
-      <c r="P62" s="21"/>
+      <c r="B62" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="C62" s="28"/>
+      <c r="D62" s="28"/>
+      <c r="E62" s="28"/>
+      <c r="F62" s="28"/>
+      <c r="G62" s="28"/>
+      <c r="H62" s="28"/>
+      <c r="I62" s="28"/>
+      <c r="J62" s="28"/>
+      <c r="K62" s="28"/>
+      <c r="L62" s="28"/>
+      <c r="M62" s="28"/>
+      <c r="N62" s="28"/>
+      <c r="O62" s="28"/>
+      <c r="P62" s="28"/>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A63">
+      <c r="A63" s="7">
         <v>39</v>
       </c>
+      <c r="B63" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="C63" s="32"/>
+      <c r="D63" s="32"/>
+      <c r="E63" s="32"/>
+      <c r="F63" s="32"/>
+      <c r="G63" s="32"/>
+      <c r="H63" s="32"/>
+      <c r="I63" s="32"/>
+      <c r="J63" s="32"/>
+      <c r="K63" s="32"/>
+      <c r="L63" s="32"/>
+      <c r="M63" s="32"/>
+      <c r="N63" s="32"/>
+      <c r="O63" s="32"/>
+      <c r="P63" s="32"/>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A64" s="7">
+        <v>40</v>
+      </c>
+      <c r="B64" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="C64" s="32"/>
+      <c r="D64" s="32"/>
+      <c r="E64" s="32"/>
+      <c r="F64" s="32"/>
+      <c r="G64" s="32"/>
+      <c r="H64" s="32"/>
+      <c r="I64" s="32"/>
+      <c r="J64" s="32"/>
+      <c r="K64" s="32"/>
+      <c r="L64" s="32"/>
+      <c r="M64" s="32"/>
+      <c r="N64" s="32"/>
+      <c r="O64" s="32"/>
+      <c r="P64" s="32"/>
+    </row>
+    <row r="65" spans="1:16" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>41</v>
+      </c>
+      <c r="B65" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="C65" s="25"/>
+      <c r="D65" s="25"/>
+      <c r="E65" s="25"/>
+      <c r="F65" s="25"/>
+      <c r="G65" s="25"/>
+      <c r="H65" s="25"/>
+      <c r="I65" s="25"/>
+      <c r="J65" s="25"/>
+      <c r="K65" s="25"/>
+      <c r="L65" s="25"/>
+      <c r="M65" s="25"/>
+      <c r="N65" s="25"/>
+      <c r="O65" s="25"/>
+      <c r="P65" s="25"/>
+    </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A66" s="7">
+        <v>42</v>
+      </c>
+      <c r="B66" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="C66" s="34"/>
+      <c r="D66" s="34"/>
+      <c r="E66" s="34"/>
+      <c r="F66" s="34"/>
+      <c r="G66" s="34"/>
+      <c r="H66" s="34"/>
+      <c r="I66" s="34"/>
+      <c r="J66" s="34"/>
+      <c r="K66" s="34"/>
+      <c r="L66" s="34"/>
+      <c r="M66" s="34"/>
+      <c r="N66" s="34"/>
+      <c r="O66" s="34"/>
+      <c r="P66" s="34"/>
+    </row>
+    <row r="67" spans="1:16" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="23">
+        <v>43</v>
+      </c>
+      <c r="B67" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="C67" s="25"/>
+      <c r="D67" s="25"/>
+      <c r="E67" s="25"/>
+      <c r="F67" s="25"/>
+      <c r="G67" s="25"/>
+      <c r="H67" s="25"/>
+      <c r="I67" s="25"/>
+      <c r="J67" s="25"/>
+      <c r="K67" s="25"/>
+      <c r="L67" s="25"/>
+      <c r="M67" s="25"/>
+      <c r="N67" s="25"/>
+      <c r="O67" s="25"/>
+      <c r="P67" s="25"/>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A68" s="7">
+        <v>44</v>
+      </c>
+      <c r="B68" s="33" t="s">
+        <v>74</v>
+      </c>
+      <c r="C68" s="33"/>
+      <c r="D68" s="33"/>
+      <c r="E68" s="33"/>
+      <c r="F68" s="33"/>
+      <c r="G68" s="33"/>
+      <c r="H68" s="33"/>
+      <c r="I68" s="33"/>
+      <c r="J68" s="33"/>
+      <c r="K68" s="33"/>
+      <c r="L68" s="33"/>
+      <c r="M68" s="33"/>
+      <c r="N68" s="33"/>
+      <c r="O68" s="33"/>
+      <c r="P68" s="33"/>
+    </row>
+    <row r="69" spans="1:16" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>45</v>
+      </c>
+      <c r="B69" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="C69" s="25"/>
+      <c r="D69" s="25"/>
+      <c r="E69" s="25"/>
+      <c r="F69" s="25"/>
+      <c r="G69" s="25"/>
+      <c r="H69" s="25"/>
+      <c r="I69" s="25"/>
+      <c r="J69" s="25"/>
+      <c r="K69" s="25"/>
+      <c r="L69" s="25"/>
+      <c r="M69" s="25"/>
+      <c r="N69" s="25"/>
+      <c r="O69" s="25"/>
+      <c r="P69" s="25"/>
     </row>
   </sheetData>
-  <mergeCells count="37">
+  <mergeCells count="44">
+    <mergeCell ref="B13:P13"/>
+    <mergeCell ref="B2:P2"/>
+    <mergeCell ref="B3:P3"/>
+    <mergeCell ref="B4:P4"/>
+    <mergeCell ref="B5:P5"/>
+    <mergeCell ref="B6:P6"/>
+    <mergeCell ref="B7:P7"/>
+    <mergeCell ref="B8:P8"/>
+    <mergeCell ref="B9:P9"/>
+    <mergeCell ref="B10:P10"/>
+    <mergeCell ref="B11:P11"/>
+    <mergeCell ref="B12:P12"/>
+    <mergeCell ref="B25:P25"/>
+    <mergeCell ref="B14:P14"/>
+    <mergeCell ref="B15:P15"/>
+    <mergeCell ref="B16:P16"/>
+    <mergeCell ref="B17:P17"/>
+    <mergeCell ref="B18:P18"/>
+    <mergeCell ref="B19:P19"/>
+    <mergeCell ref="B20:P20"/>
+    <mergeCell ref="B21:P21"/>
+    <mergeCell ref="B22:P22"/>
+    <mergeCell ref="B23:P23"/>
+    <mergeCell ref="B24:P24"/>
     <mergeCell ref="B62:P62"/>
     <mergeCell ref="B59:P59"/>
     <mergeCell ref="B60:P60"/>
@@ -3617,32 +3914,16 @@
     <mergeCell ref="B55:P55"/>
     <mergeCell ref="B54:P54"/>
     <mergeCell ref="B53:P53"/>
-    <mergeCell ref="B25:P25"/>
-    <mergeCell ref="B14:P14"/>
-    <mergeCell ref="B15:P15"/>
-    <mergeCell ref="B16:P16"/>
-    <mergeCell ref="B17:P17"/>
-    <mergeCell ref="B18:P18"/>
-    <mergeCell ref="B19:P19"/>
-    <mergeCell ref="B20:P20"/>
-    <mergeCell ref="B21:P21"/>
-    <mergeCell ref="B22:P22"/>
-    <mergeCell ref="B23:P23"/>
-    <mergeCell ref="B24:P24"/>
-    <mergeCell ref="B13:P13"/>
-    <mergeCell ref="B2:P2"/>
-    <mergeCell ref="B3:P3"/>
-    <mergeCell ref="B4:P4"/>
-    <mergeCell ref="B5:P5"/>
-    <mergeCell ref="B6:P6"/>
-    <mergeCell ref="B7:P7"/>
-    <mergeCell ref="B8:P8"/>
-    <mergeCell ref="B9:P9"/>
-    <mergeCell ref="B10:P10"/>
-    <mergeCell ref="B11:P11"/>
-    <mergeCell ref="B12:P12"/>
+    <mergeCell ref="B67:P67"/>
+    <mergeCell ref="B68:P68"/>
+    <mergeCell ref="B69:P69"/>
+    <mergeCell ref="B63:P63"/>
+    <mergeCell ref="B64:P64"/>
+    <mergeCell ref="B65:P65"/>
+    <mergeCell ref="B66:P66"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Chybí jen dongle a validace zelených položek
</commit_message>
<xml_diff>
--- a/MDM/WorkSheet.xlsx
+++ b/MDM/WorkSheet.xlsx
@@ -192,9 +192,6 @@
   </si>
   <si>
     <t>Hypo, žena, 56+ - záměna sudých a lichých hodnot definujících průběhy v segmentu u 1. až 6. procedury (časové intervaly jsou správně)</t>
-  </si>
-  <si>
-    <t>Normo, žena, 56+ - v 9. až 13. proceduře chybí v prvním segmentu hodnoty označení průběhu (vvs) a sweep</t>
   </si>
   <si>
     <t>Obecná (informativní) představa k barvení sloupce v závislosti na hodnotě z registrů (AIN2-AIN1) v rozsahu 38 = zelená / 60 = červená</t>
@@ -360,6 +357,23 @@
         <scheme val="minor"/>
       </rPr>
       <t>(Prověřit!!! Neumím nasimulovat)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Normo, žena, 56+ - v 9. až 13. proceduře chybí v prvním segmentu hodnoty označení průběhu (vvs) a sweep - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>!!! OVĚŘIT !!!</t>
     </r>
   </si>
 </sst>
@@ -549,7 +563,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="47">
+  <fills count="46">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -804,12 +818,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF99FF66"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -974,7 +982,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="3" applyAlignment="1">
@@ -1011,7 +1019,6 @@
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="46" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1024,22 +1031,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="5"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="5"/>
+      <alignment horizontal="left" vertical="center" indent="5"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="5"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1048,23 +1046,29 @@
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="5"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="46" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="5"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="5"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="5"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" wrapText="1" indent="5"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
@@ -1159,7 +1163,7 @@
         <xdr:cNvPr id="2" name="Obrázek 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1053FDDA-A9AC-4562-AAF3-9412BEC8FAC0}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1053FDDA-A9AC-4562-AAF3-9412BEC8FAC0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1475,10 +1479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H112"/>
+  <dimension ref="A1:H113"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="A112" sqref="A112:C112"/>
+      <selection activeCell="A113" sqref="A113:C113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1516,11 +1520,11 @@
       </c>
       <c r="F2" s="4">
         <f>SUM(C:C)</f>
-        <v>484</v>
+        <v>487</v>
       </c>
       <c r="H2" s="5">
         <f>F2*300</f>
-        <v>145200</v>
+        <v>146100</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -2506,6 +2510,14 @@
       </c>
       <c r="C112">
         <v>4</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" s="1">
+        <v>42970</v>
+      </c>
+      <c r="C113">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -2517,8 +2529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:P94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="B91" sqref="B91:P91"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55:P55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2530,592 +2542,592 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="35"/>
-      <c r="N2" s="35"/>
-      <c r="O2" s="35"/>
-      <c r="P2" s="35"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="27"/>
+      <c r="P2" s="27"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>2</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="32"/>
-      <c r="L3" s="32"/>
-      <c r="M3" s="32"/>
-      <c r="N3" s="32"/>
-      <c r="O3" s="32"/>
-      <c r="P3" s="32"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="26"/>
+      <c r="M3" s="26"/>
+      <c r="N3" s="26"/>
+      <c r="O3" s="26"/>
+      <c r="P3" s="26"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>3</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="32"/>
-      <c r="I4" s="32"/>
-      <c r="J4" s="32"/>
-      <c r="K4" s="32"/>
-      <c r="L4" s="32"/>
-      <c r="M4" s="32"/>
-      <c r="N4" s="32"/>
-      <c r="O4" s="32"/>
-      <c r="P4" s="32"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="26"/>
+      <c r="M4" s="26"/>
+      <c r="N4" s="26"/>
+      <c r="O4" s="26"/>
+      <c r="P4" s="26"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>4</v>
       </c>
-      <c r="B5" s="32" t="s">
+      <c r="B5" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="32"/>
-      <c r="I5" s="32"/>
-      <c r="J5" s="32"/>
-      <c r="K5" s="32"/>
-      <c r="L5" s="32"/>
-      <c r="M5" s="32"/>
-      <c r="N5" s="32"/>
-      <c r="O5" s="32"/>
-      <c r="P5" s="32"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="26"/>
+      <c r="N5" s="26"/>
+      <c r="O5" s="26"/>
+      <c r="P5" s="26"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>5</v>
       </c>
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="32"/>
-      <c r="J6" s="32"/>
-      <c r="K6" s="32"/>
-      <c r="L6" s="32"/>
-      <c r="M6" s="32"/>
-      <c r="N6" s="32"/>
-      <c r="O6" s="32"/>
-      <c r="P6" s="32"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="26"/>
+      <c r="M6" s="26"/>
+      <c r="N6" s="26"/>
+      <c r="O6" s="26"/>
+      <c r="P6" s="26"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>6</v>
       </c>
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="C7" s="32"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32"/>
-      <c r="I7" s="32"/>
-      <c r="J7" s="32"/>
-      <c r="K7" s="32"/>
-      <c r="L7" s="32"/>
-      <c r="M7" s="32"/>
-      <c r="N7" s="32"/>
-      <c r="O7" s="32"/>
-      <c r="P7" s="32"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="26"/>
+      <c r="K7" s="26"/>
+      <c r="L7" s="26"/>
+      <c r="M7" s="26"/>
+      <c r="N7" s="26"/>
+      <c r="O7" s="26"/>
+      <c r="P7" s="26"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>7</v>
       </c>
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="32"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="32"/>
-      <c r="H8" s="32"/>
-      <c r="I8" s="32"/>
-      <c r="J8" s="32"/>
-      <c r="K8" s="32"/>
-      <c r="L8" s="32"/>
-      <c r="M8" s="32"/>
-      <c r="N8" s="32"/>
-      <c r="O8" s="32"/>
-      <c r="P8" s="32"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="26"/>
+      <c r="K8" s="26"/>
+      <c r="L8" s="26"/>
+      <c r="M8" s="26"/>
+      <c r="N8" s="26"/>
+      <c r="O8" s="26"/>
+      <c r="P8" s="26"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>8</v>
       </c>
-      <c r="B9" s="32" t="s">
-        <v>63</v>
-      </c>
-      <c r="C9" s="32"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="32"/>
-      <c r="I9" s="32"/>
-      <c r="J9" s="32"/>
-      <c r="K9" s="32"/>
-      <c r="L9" s="32"/>
-      <c r="M9" s="32"/>
-      <c r="N9" s="32"/>
-      <c r="O9" s="32"/>
-      <c r="P9" s="32"/>
+      <c r="B9" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="26"/>
+      <c r="L9" s="26"/>
+      <c r="M9" s="26"/>
+      <c r="N9" s="26"/>
+      <c r="O9" s="26"/>
+      <c r="P9" s="26"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>9</v>
       </c>
-      <c r="B10" s="38" t="s">
+      <c r="B10" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="38"/>
-      <c r="J10" s="38"/>
-      <c r="K10" s="38"/>
-      <c r="L10" s="38"/>
-      <c r="M10" s="38"/>
-      <c r="N10" s="38"/>
-      <c r="O10" s="38"/>
-      <c r="P10" s="38"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="28"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="28"/>
+      <c r="L10" s="28"/>
+      <c r="M10" s="28"/>
+      <c r="N10" s="28"/>
+      <c r="O10" s="28"/>
+      <c r="P10" s="28"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>10</v>
       </c>
-      <c r="B11" s="32" t="s">
+      <c r="B11" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="32"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="32"/>
-      <c r="I11" s="32"/>
-      <c r="J11" s="32"/>
-      <c r="K11" s="32"/>
-      <c r="L11" s="32"/>
-      <c r="M11" s="32"/>
-      <c r="N11" s="32"/>
-      <c r="O11" s="32"/>
-      <c r="P11" s="32"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="26"/>
+      <c r="K11" s="26"/>
+      <c r="L11" s="26"/>
+      <c r="M11" s="26"/>
+      <c r="N11" s="26"/>
+      <c r="O11" s="26"/>
+      <c r="P11" s="26"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>11</v>
       </c>
-      <c r="B12" s="32" t="s">
+      <c r="B12" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="32"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="32"/>
-      <c r="I12" s="32"/>
-      <c r="J12" s="32"/>
-      <c r="K12" s="32"/>
-      <c r="L12" s="32"/>
-      <c r="M12" s="32"/>
-      <c r="N12" s="32"/>
-      <c r="O12" s="32"/>
-      <c r="P12" s="32"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="26"/>
+      <c r="J12" s="26"/>
+      <c r="K12" s="26"/>
+      <c r="L12" s="26"/>
+      <c r="M12" s="26"/>
+      <c r="N12" s="26"/>
+      <c r="O12" s="26"/>
+      <c r="P12" s="26"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>12</v>
       </c>
-      <c r="B13" s="32" t="s">
+      <c r="B13" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="C13" s="32"/>
-      <c r="D13" s="32"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="32"/>
-      <c r="H13" s="32"/>
-      <c r="I13" s="32"/>
-      <c r="J13" s="32"/>
-      <c r="K13" s="32"/>
-      <c r="L13" s="32"/>
-      <c r="M13" s="32"/>
-      <c r="N13" s="32"/>
-      <c r="O13" s="32"/>
-      <c r="P13" s="32"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="26"/>
+      <c r="K13" s="26"/>
+      <c r="L13" s="26"/>
+      <c r="M13" s="26"/>
+      <c r="N13" s="26"/>
+      <c r="O13" s="26"/>
+      <c r="P13" s="26"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>13</v>
       </c>
-      <c r="B14" s="32" t="s">
+      <c r="B14" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="32"/>
-      <c r="D14" s="32"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="32"/>
-      <c r="G14" s="32"/>
-      <c r="H14" s="32"/>
-      <c r="I14" s="32"/>
-      <c r="J14" s="32"/>
-      <c r="K14" s="32"/>
-      <c r="L14" s="32"/>
-      <c r="M14" s="32"/>
-      <c r="N14" s="32"/>
-      <c r="O14" s="32"/>
-      <c r="P14" s="32"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="26"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="26"/>
+      <c r="L14" s="26"/>
+      <c r="M14" s="26"/>
+      <c r="N14" s="26"/>
+      <c r="O14" s="26"/>
+      <c r="P14" s="26"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>14</v>
       </c>
-      <c r="B15" s="38" t="s">
-        <v>65</v>
-      </c>
-      <c r="C15" s="38"/>
-      <c r="D15" s="38"/>
-      <c r="E15" s="38"/>
-      <c r="F15" s="38"/>
-      <c r="G15" s="38"/>
-      <c r="H15" s="38"/>
-      <c r="I15" s="38"/>
-      <c r="J15" s="38"/>
-      <c r="K15" s="38"/>
-      <c r="L15" s="38"/>
-      <c r="M15" s="38"/>
-      <c r="N15" s="38"/>
-      <c r="O15" s="38"/>
-      <c r="P15" s="38"/>
+      <c r="B15" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="28"/>
+      <c r="L15" s="28"/>
+      <c r="M15" s="28"/>
+      <c r="N15" s="28"/>
+      <c r="O15" s="28"/>
+      <c r="P15" s="28"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <v>15</v>
       </c>
-      <c r="B16" s="32" t="s">
+      <c r="B16" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="C16" s="32"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="32"/>
-      <c r="H16" s="32"/>
-      <c r="I16" s="32"/>
-      <c r="J16" s="32"/>
-      <c r="K16" s="32"/>
-      <c r="L16" s="32"/>
-      <c r="M16" s="32"/>
-      <c r="N16" s="32"/>
-      <c r="O16" s="32"/>
-      <c r="P16" s="32"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="26"/>
+      <c r="K16" s="26"/>
+      <c r="L16" s="26"/>
+      <c r="M16" s="26"/>
+      <c r="N16" s="26"/>
+      <c r="O16" s="26"/>
+      <c r="P16" s="26"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>16</v>
       </c>
-      <c r="B17" s="32" t="s">
+      <c r="B17" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="32"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="32"/>
-      <c r="I17" s="32"/>
-      <c r="J17" s="32"/>
-      <c r="K17" s="32"/>
-      <c r="L17" s="32"/>
-      <c r="M17" s="32"/>
-      <c r="N17" s="32"/>
-      <c r="O17" s="32"/>
-      <c r="P17" s="32"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26"/>
+      <c r="K17" s="26"/>
+      <c r="L17" s="26"/>
+      <c r="M17" s="26"/>
+      <c r="N17" s="26"/>
+      <c r="O17" s="26"/>
+      <c r="P17" s="26"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <v>17</v>
       </c>
-      <c r="B18" s="32" t="s">
+      <c r="B18" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="32"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="32"/>
-      <c r="H18" s="32"/>
-      <c r="I18" s="32"/>
-      <c r="J18" s="32"/>
-      <c r="K18" s="32"/>
-      <c r="L18" s="32"/>
-      <c r="M18" s="32"/>
-      <c r="N18" s="32"/>
-      <c r="O18" s="32"/>
-      <c r="P18" s="32"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="26"/>
+      <c r="K18" s="26"/>
+      <c r="L18" s="26"/>
+      <c r="M18" s="26"/>
+      <c r="N18" s="26"/>
+      <c r="O18" s="26"/>
+      <c r="P18" s="26"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>18</v>
       </c>
-      <c r="B19" s="32" t="s">
+      <c r="B19" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="32"/>
-      <c r="D19" s="32"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="32"/>
-      <c r="H19" s="32"/>
-      <c r="I19" s="32"/>
-      <c r="J19" s="32"/>
-      <c r="K19" s="32"/>
-      <c r="L19" s="32"/>
-      <c r="M19" s="32"/>
-      <c r="N19" s="32"/>
-      <c r="O19" s="32"/>
-      <c r="P19" s="32"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="26"/>
+      <c r="I19" s="26"/>
+      <c r="J19" s="26"/>
+      <c r="K19" s="26"/>
+      <c r="L19" s="26"/>
+      <c r="M19" s="26"/>
+      <c r="N19" s="26"/>
+      <c r="O19" s="26"/>
+      <c r="P19" s="26"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
         <v>19</v>
       </c>
-      <c r="B20" s="32" t="s">
+      <c r="B20" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="32"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="32"/>
-      <c r="H20" s="32"/>
-      <c r="I20" s="32"/>
-      <c r="J20" s="32"/>
-      <c r="K20" s="32"/>
-      <c r="L20" s="32"/>
-      <c r="M20" s="32"/>
-      <c r="N20" s="32"/>
-      <c r="O20" s="32"/>
-      <c r="P20" s="32"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="26"/>
+      <c r="H20" s="26"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
+      <c r="K20" s="26"/>
+      <c r="L20" s="26"/>
+      <c r="M20" s="26"/>
+      <c r="N20" s="26"/>
+      <c r="O20" s="26"/>
+      <c r="P20" s="26"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
         <v>20</v>
       </c>
-      <c r="B21" s="32" t="s">
+      <c r="B21" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="C21" s="32"/>
-      <c r="D21" s="32"/>
-      <c r="E21" s="32"/>
-      <c r="F21" s="32"/>
-      <c r="G21" s="32"/>
-      <c r="H21" s="32"/>
-      <c r="I21" s="32"/>
-      <c r="J21" s="32"/>
-      <c r="K21" s="32"/>
-      <c r="L21" s="32"/>
-      <c r="M21" s="32"/>
-      <c r="N21" s="32"/>
-      <c r="O21" s="32"/>
-      <c r="P21" s="32"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="26"/>
+      <c r="J21" s="26"/>
+      <c r="K21" s="26"/>
+      <c r="L21" s="26"/>
+      <c r="M21" s="26"/>
+      <c r="N21" s="26"/>
+      <c r="O21" s="26"/>
+      <c r="P21" s="26"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
         <v>21</v>
       </c>
-      <c r="B22" s="32" t="s">
+      <c r="B22" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="C22" s="32"/>
-      <c r="D22" s="32"/>
-      <c r="E22" s="32"/>
-      <c r="F22" s="32"/>
-      <c r="G22" s="32"/>
-      <c r="H22" s="32"/>
-      <c r="I22" s="32"/>
-      <c r="J22" s="32"/>
-      <c r="K22" s="32"/>
-      <c r="L22" s="32"/>
-      <c r="M22" s="32"/>
-      <c r="N22" s="32"/>
-      <c r="O22" s="32"/>
-      <c r="P22" s="32"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="26"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="26"/>
+      <c r="J22" s="26"/>
+      <c r="K22" s="26"/>
+      <c r="L22" s="26"/>
+      <c r="M22" s="26"/>
+      <c r="N22" s="26"/>
+      <c r="O22" s="26"/>
+      <c r="P22" s="26"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
         <v>22</v>
       </c>
-      <c r="B23" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="C23" s="32"/>
-      <c r="D23" s="32"/>
-      <c r="E23" s="32"/>
-      <c r="F23" s="32"/>
-      <c r="G23" s="32"/>
-      <c r="H23" s="32"/>
-      <c r="I23" s="32"/>
-      <c r="J23" s="32"/>
-      <c r="K23" s="32"/>
-      <c r="L23" s="32"/>
-      <c r="M23" s="32"/>
-      <c r="N23" s="32"/>
-      <c r="O23" s="32"/>
-      <c r="P23" s="32"/>
+      <c r="B23" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="C23" s="26"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="26"/>
+      <c r="I23" s="26"/>
+      <c r="J23" s="26"/>
+      <c r="K23" s="26"/>
+      <c r="L23" s="26"/>
+      <c r="M23" s="26"/>
+      <c r="N23" s="26"/>
+      <c r="O23" s="26"/>
+      <c r="P23" s="26"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
         <v>23</v>
       </c>
-      <c r="B24" s="32" t="s">
+      <c r="B24" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="C24" s="32"/>
-      <c r="D24" s="32"/>
-      <c r="E24" s="32"/>
-      <c r="F24" s="32"/>
-      <c r="G24" s="32"/>
-      <c r="H24" s="32"/>
-      <c r="I24" s="32"/>
-      <c r="J24" s="32"/>
-      <c r="K24" s="32"/>
-      <c r="L24" s="32"/>
-      <c r="M24" s="32"/>
-      <c r="N24" s="32"/>
-      <c r="O24" s="32"/>
-      <c r="P24" s="32"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="26"/>
+      <c r="I24" s="26"/>
+      <c r="J24" s="26"/>
+      <c r="K24" s="26"/>
+      <c r="L24" s="26"/>
+      <c r="M24" s="26"/>
+      <c r="N24" s="26"/>
+      <c r="O24" s="26"/>
+      <c r="P24" s="26"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="9">
         <v>24</v>
       </c>
-      <c r="B25" s="38" t="s">
-        <v>83</v>
-      </c>
-      <c r="C25" s="38"/>
-      <c r="D25" s="38"/>
-      <c r="E25" s="38"/>
-      <c r="F25" s="38"/>
-      <c r="G25" s="38"/>
-      <c r="H25" s="38"/>
-      <c r="I25" s="38"/>
-      <c r="J25" s="38"/>
-      <c r="K25" s="38"/>
-      <c r="L25" s="38"/>
-      <c r="M25" s="38"/>
-      <c r="N25" s="38"/>
-      <c r="O25" s="38"/>
-      <c r="P25" s="38"/>
+      <c r="B25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="C25" s="28"/>
+      <c r="D25" s="28"/>
+      <c r="E25" s="28"/>
+      <c r="F25" s="28"/>
+      <c r="G25" s="28"/>
+      <c r="H25" s="28"/>
+      <c r="I25" s="28"/>
+      <c r="J25" s="28"/>
+      <c r="K25" s="28"/>
+      <c r="L25" s="28"/>
+      <c r="M25" s="28"/>
+      <c r="N25" s="28"/>
+      <c r="O25" s="28"/>
+      <c r="P25" s="28"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
         <v>25</v>
       </c>
-      <c r="B26" s="32" t="s">
+      <c r="B26" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="C26" s="32"/>
-      <c r="D26" s="32"/>
-      <c r="E26" s="32"/>
-      <c r="F26" s="32"/>
-      <c r="G26" s="32"/>
-      <c r="H26" s="32"/>
-      <c r="I26" s="32"/>
-      <c r="J26" s="32"/>
-      <c r="K26" s="32"/>
-      <c r="L26" s="32"/>
-      <c r="M26" s="32"/>
-      <c r="N26" s="32"/>
-      <c r="O26" s="32"/>
-      <c r="P26" s="32"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="26"/>
+      <c r="G26" s="26"/>
+      <c r="H26" s="26"/>
+      <c r="I26" s="26"/>
+      <c r="J26" s="26"/>
+      <c r="K26" s="26"/>
+      <c r="L26" s="26"/>
+      <c r="M26" s="26"/>
+      <c r="N26" s="26"/>
+      <c r="O26" s="26"/>
+      <c r="P26" s="26"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
-      <c r="B27" s="35"/>
-      <c r="C27" s="35"/>
-      <c r="D27" s="35"/>
-      <c r="E27" s="35"/>
-      <c r="F27" s="35"/>
-      <c r="G27" s="35"/>
-      <c r="H27" s="35"/>
-      <c r="I27" s="35"/>
-      <c r="J27" s="35"/>
-      <c r="K27" s="35"/>
-      <c r="L27" s="35"/>
-      <c r="M27" s="35"/>
-      <c r="N27" s="35"/>
-      <c r="O27" s="35"/>
-      <c r="P27" s="35"/>
+      <c r="B27" s="27"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="27"/>
+      <c r="F27" s="27"/>
+      <c r="G27" s="27"/>
+      <c r="H27" s="27"/>
+      <c r="I27" s="27"/>
+      <c r="J27" s="27"/>
+      <c r="K27" s="27"/>
+      <c r="L27" s="27"/>
+      <c r="M27" s="27"/>
+      <c r="N27" s="27"/>
+      <c r="O27" s="27"/>
+      <c r="P27" s="27"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
         <v>27</v>
       </c>
-      <c r="B28" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="C28" s="24"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="24"/>
-      <c r="H28" s="24"/>
-      <c r="I28" s="24"/>
-      <c r="J28" s="24"/>
-      <c r="K28" s="24"/>
-      <c r="L28" s="24"/>
-      <c r="M28" s="24"/>
-      <c r="N28" s="24"/>
-      <c r="O28" s="24"/>
+      <c r="B28" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" s="23"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="23"/>
+      <c r="J28" s="23"/>
+      <c r="K28" s="23"/>
+      <c r="L28" s="23"/>
+      <c r="M28" s="23"/>
+      <c r="N28" s="23"/>
+      <c r="O28" s="23"/>
       <c r="P28" s="8"/>
     </row>
     <row r="29" spans="1:16" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
@@ -3628,402 +3640,402 @@
       <c r="A52">
         <v>28</v>
       </c>
-      <c r="B52" s="35"/>
-      <c r="C52" s="35"/>
-      <c r="D52" s="35"/>
-      <c r="E52" s="35"/>
-      <c r="F52" s="35"/>
-      <c r="G52" s="35"/>
-      <c r="H52" s="35"/>
-      <c r="I52" s="35"/>
-      <c r="J52" s="35"/>
-      <c r="K52" s="35"/>
-      <c r="L52" s="35"/>
-      <c r="M52" s="35"/>
-      <c r="N52" s="35"/>
-      <c r="O52" s="35"/>
-      <c r="P52" s="35"/>
+      <c r="B52" s="27"/>
+      <c r="C52" s="27"/>
+      <c r="D52" s="27"/>
+      <c r="E52" s="27"/>
+      <c r="F52" s="27"/>
+      <c r="G52" s="27"/>
+      <c r="H52" s="27"/>
+      <c r="I52" s="27"/>
+      <c r="J52" s="27"/>
+      <c r="K52" s="27"/>
+      <c r="L52" s="27"/>
+      <c r="M52" s="27"/>
+      <c r="N52" s="27"/>
+      <c r="O52" s="27"/>
+      <c r="P52" s="27"/>
     </row>
     <row r="53" spans="1:16" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="20">
         <v>29</v>
       </c>
-      <c r="B53" s="37" t="s">
-        <v>81</v>
-      </c>
-      <c r="C53" s="37"/>
-      <c r="D53" s="37"/>
-      <c r="E53" s="37"/>
-      <c r="F53" s="37"/>
-      <c r="G53" s="37"/>
-      <c r="H53" s="37"/>
-      <c r="I53" s="37"/>
-      <c r="J53" s="37"/>
-      <c r="K53" s="37"/>
-      <c r="L53" s="37"/>
-      <c r="M53" s="37"/>
-      <c r="N53" s="37"/>
-      <c r="O53" s="37"/>
-      <c r="P53" s="37"/>
+      <c r="B53" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="C53" s="31"/>
+      <c r="D53" s="31"/>
+      <c r="E53" s="31"/>
+      <c r="F53" s="31"/>
+      <c r="G53" s="31"/>
+      <c r="H53" s="31"/>
+      <c r="I53" s="31"/>
+      <c r="J53" s="31"/>
+      <c r="K53" s="31"/>
+      <c r="L53" s="31"/>
+      <c r="M53" s="31"/>
+      <c r="N53" s="31"/>
+      <c r="O53" s="31"/>
+      <c r="P53" s="31"/>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" s="9">
         <v>30</v>
       </c>
-      <c r="B54" s="38" t="s">
-        <v>82</v>
-      </c>
-      <c r="C54" s="38"/>
-      <c r="D54" s="38"/>
-      <c r="E54" s="38"/>
-      <c r="F54" s="38"/>
-      <c r="G54" s="38"/>
-      <c r="H54" s="38"/>
-      <c r="I54" s="38"/>
-      <c r="J54" s="38"/>
-      <c r="K54" s="38"/>
-      <c r="L54" s="38"/>
-      <c r="M54" s="38"/>
-      <c r="N54" s="38"/>
-      <c r="O54" s="38"/>
-      <c r="P54" s="38"/>
+      <c r="B54" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="C54" s="28"/>
+      <c r="D54" s="28"/>
+      <c r="E54" s="28"/>
+      <c r="F54" s="28"/>
+      <c r="G54" s="28"/>
+      <c r="H54" s="28"/>
+      <c r="I54" s="28"/>
+      <c r="J54" s="28"/>
+      <c r="K54" s="28"/>
+      <c r="L54" s="28"/>
+      <c r="M54" s="28"/>
+      <c r="N54" s="28"/>
+      <c r="O54" s="28"/>
+      <c r="P54" s="28"/>
     </row>
     <row r="55" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="22">
+      <c r="A55" s="7">
         <v>31</v>
       </c>
-      <c r="B55" s="36" t="s">
+      <c r="B55" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="C55" s="36"/>
-      <c r="D55" s="36"/>
-      <c r="E55" s="36"/>
-      <c r="F55" s="36"/>
-      <c r="G55" s="36"/>
-      <c r="H55" s="36"/>
-      <c r="I55" s="36"/>
-      <c r="J55" s="36"/>
-      <c r="K55" s="36"/>
-      <c r="L55" s="36"/>
-      <c r="M55" s="36"/>
-      <c r="N55" s="36"/>
-      <c r="O55" s="36"/>
-      <c r="P55" s="36"/>
+      <c r="C55" s="30"/>
+      <c r="D55" s="30"/>
+      <c r="E55" s="30"/>
+      <c r="F55" s="30"/>
+      <c r="G55" s="30"/>
+      <c r="H55" s="30"/>
+      <c r="I55" s="30"/>
+      <c r="J55" s="30"/>
+      <c r="K55" s="30"/>
+      <c r="L55" s="30"/>
+      <c r="M55" s="30"/>
+      <c r="N55" s="30"/>
+      <c r="O55" s="30"/>
+      <c r="P55" s="30"/>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A56">
+      <c r="A56" s="9">
         <v>32</v>
       </c>
-      <c r="B56" s="35" t="s">
-        <v>59</v>
-      </c>
-      <c r="C56" s="35"/>
-      <c r="D56" s="35"/>
-      <c r="E56" s="35"/>
-      <c r="F56" s="35"/>
-      <c r="G56" s="35"/>
-      <c r="H56" s="35"/>
-      <c r="I56" s="35"/>
-      <c r="J56" s="35"/>
-      <c r="K56" s="35"/>
-      <c r="L56" s="35"/>
-      <c r="M56" s="35"/>
-      <c r="N56" s="35"/>
-      <c r="O56" s="35"/>
-      <c r="P56" s="35"/>
+      <c r="B56" s="28" t="s">
+        <v>85</v>
+      </c>
+      <c r="C56" s="28"/>
+      <c r="D56" s="28"/>
+      <c r="E56" s="28"/>
+      <c r="F56" s="28"/>
+      <c r="G56" s="28"/>
+      <c r="H56" s="28"/>
+      <c r="I56" s="28"/>
+      <c r="J56" s="28"/>
+      <c r="K56" s="28"/>
+      <c r="L56" s="28"/>
+      <c r="M56" s="28"/>
+      <c r="N56" s="28"/>
+      <c r="O56" s="28"/>
+      <c r="P56" s="28"/>
     </row>
     <row r="57" spans="1:16" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="7">
         <v>33</v>
       </c>
-      <c r="B57" s="33" t="s">
-        <v>64</v>
-      </c>
-      <c r="C57" s="33"/>
-      <c r="D57" s="33"/>
-      <c r="E57" s="33"/>
-      <c r="F57" s="33"/>
-      <c r="G57" s="33"/>
-      <c r="H57" s="33"/>
-      <c r="I57" s="33"/>
-      <c r="J57" s="33"/>
-      <c r="K57" s="33"/>
-      <c r="L57" s="33"/>
-      <c r="M57" s="33"/>
-      <c r="N57" s="33"/>
-      <c r="O57" s="33"/>
-      <c r="P57" s="33"/>
+      <c r="B57" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="C57" s="29"/>
+      <c r="D57" s="29"/>
+      <c r="E57" s="29"/>
+      <c r="F57" s="29"/>
+      <c r="G57" s="29"/>
+      <c r="H57" s="29"/>
+      <c r="I57" s="29"/>
+      <c r="J57" s="29"/>
+      <c r="K57" s="29"/>
+      <c r="L57" s="29"/>
+      <c r="M57" s="29"/>
+      <c r="N57" s="29"/>
+      <c r="O57" s="29"/>
+      <c r="P57" s="29"/>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
         <v>34</v>
       </c>
-      <c r="B58" s="32" t="s">
-        <v>62</v>
-      </c>
-      <c r="C58" s="32"/>
-      <c r="D58" s="32"/>
-      <c r="E58" s="32"/>
-      <c r="F58" s="32"/>
-      <c r="G58" s="32"/>
-      <c r="H58" s="32"/>
-      <c r="I58" s="32"/>
-      <c r="J58" s="32"/>
-      <c r="K58" s="32"/>
-      <c r="L58" s="32"/>
-      <c r="M58" s="32"/>
-      <c r="N58" s="32"/>
-      <c r="O58" s="32"/>
-      <c r="P58" s="32"/>
+      <c r="B58" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="C58" s="26"/>
+      <c r="D58" s="26"/>
+      <c r="E58" s="26"/>
+      <c r="F58" s="26"/>
+      <c r="G58" s="26"/>
+      <c r="H58" s="26"/>
+      <c r="I58" s="26"/>
+      <c r="J58" s="26"/>
+      <c r="K58" s="26"/>
+      <c r="L58" s="26"/>
+      <c r="M58" s="26"/>
+      <c r="N58" s="26"/>
+      <c r="O58" s="26"/>
+      <c r="P58" s="26"/>
     </row>
     <row r="59" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="21">
         <v>35</v>
       </c>
-      <c r="B59" s="33" t="s">
-        <v>61</v>
-      </c>
-      <c r="C59" s="33"/>
-      <c r="D59" s="33"/>
-      <c r="E59" s="33"/>
-      <c r="F59" s="33"/>
-      <c r="G59" s="33"/>
-      <c r="H59" s="33"/>
-      <c r="I59" s="33"/>
-      <c r="J59" s="33"/>
-      <c r="K59" s="33"/>
-      <c r="L59" s="33"/>
-      <c r="M59" s="33"/>
-      <c r="N59" s="33"/>
-      <c r="O59" s="33"/>
-      <c r="P59" s="33"/>
+      <c r="B59" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="C59" s="29"/>
+      <c r="D59" s="29"/>
+      <c r="E59" s="29"/>
+      <c r="F59" s="29"/>
+      <c r="G59" s="29"/>
+      <c r="H59" s="29"/>
+      <c r="I59" s="29"/>
+      <c r="J59" s="29"/>
+      <c r="K59" s="29"/>
+      <c r="L59" s="29"/>
+      <c r="M59" s="29"/>
+      <c r="N59" s="29"/>
+      <c r="O59" s="29"/>
+      <c r="P59" s="29"/>
     </row>
     <row r="60" spans="1:16" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="25">
+      <c r="A60" s="24">
         <v>36</v>
       </c>
-      <c r="B60" s="34" t="s">
-        <v>75</v>
-      </c>
-      <c r="C60" s="34"/>
-      <c r="D60" s="34"/>
-      <c r="E60" s="34"/>
-      <c r="F60" s="34"/>
-      <c r="G60" s="34"/>
-      <c r="H60" s="34"/>
-      <c r="I60" s="34"/>
-      <c r="J60" s="34"/>
-      <c r="K60" s="34"/>
-      <c r="L60" s="34"/>
-      <c r="M60" s="34"/>
-      <c r="N60" s="34"/>
-      <c r="O60" s="34"/>
-      <c r="P60" s="34"/>
+      <c r="B60" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="C60" s="30"/>
+      <c r="D60" s="30"/>
+      <c r="E60" s="30"/>
+      <c r="F60" s="30"/>
+      <c r="G60" s="30"/>
+      <c r="H60" s="30"/>
+      <c r="I60" s="30"/>
+      <c r="J60" s="30"/>
+      <c r="K60" s="30"/>
+      <c r="L60" s="30"/>
+      <c r="M60" s="30"/>
+      <c r="N60" s="30"/>
+      <c r="O60" s="30"/>
+      <c r="P60" s="30"/>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" s="7">
         <v>37</v>
       </c>
-      <c r="B61" s="32" t="s">
-        <v>66</v>
-      </c>
-      <c r="C61" s="32"/>
-      <c r="D61" s="32"/>
-      <c r="E61" s="32"/>
-      <c r="F61" s="32"/>
-      <c r="G61" s="32"/>
-      <c r="H61" s="32"/>
-      <c r="I61" s="32"/>
-      <c r="J61" s="32"/>
-      <c r="K61" s="32"/>
-      <c r="L61" s="32"/>
-      <c r="M61" s="32"/>
-      <c r="N61" s="32"/>
-      <c r="O61" s="32"/>
-      <c r="P61" s="32"/>
+      <c r="B61" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="C61" s="26"/>
+      <c r="D61" s="26"/>
+      <c r="E61" s="26"/>
+      <c r="F61" s="26"/>
+      <c r="G61" s="26"/>
+      <c r="H61" s="26"/>
+      <c r="I61" s="26"/>
+      <c r="J61" s="26"/>
+      <c r="K61" s="26"/>
+      <c r="L61" s="26"/>
+      <c r="M61" s="26"/>
+      <c r="N61" s="26"/>
+      <c r="O61" s="26"/>
+      <c r="P61" s="26"/>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
         <v>38</v>
       </c>
-      <c r="B62" s="32" t="s">
-        <v>67</v>
-      </c>
-      <c r="C62" s="32"/>
-      <c r="D62" s="32"/>
-      <c r="E62" s="32"/>
-      <c r="F62" s="32"/>
-      <c r="G62" s="32"/>
-      <c r="H62" s="32"/>
-      <c r="I62" s="32"/>
-      <c r="J62" s="32"/>
-      <c r="K62" s="32"/>
-      <c r="L62" s="32"/>
-      <c r="M62" s="32"/>
-      <c r="N62" s="32"/>
-      <c r="O62" s="32"/>
-      <c r="P62" s="32"/>
+      <c r="B62" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="C62" s="26"/>
+      <c r="D62" s="26"/>
+      <c r="E62" s="26"/>
+      <c r="F62" s="26"/>
+      <c r="G62" s="26"/>
+      <c r="H62" s="26"/>
+      <c r="I62" s="26"/>
+      <c r="J62" s="26"/>
+      <c r="K62" s="26"/>
+      <c r="L62" s="26"/>
+      <c r="M62" s="26"/>
+      <c r="N62" s="26"/>
+      <c r="O62" s="26"/>
+      <c r="P62" s="26"/>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" s="7">
         <v>39</v>
       </c>
-      <c r="B63" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="C63" s="30"/>
-      <c r="D63" s="30"/>
-      <c r="E63" s="30"/>
-      <c r="F63" s="30"/>
-      <c r="G63" s="30"/>
-      <c r="H63" s="30"/>
-      <c r="I63" s="30"/>
-      <c r="J63" s="30"/>
-      <c r="K63" s="30"/>
-      <c r="L63" s="30"/>
-      <c r="M63" s="30"/>
-      <c r="N63" s="30"/>
-      <c r="O63" s="30"/>
-      <c r="P63" s="30"/>
+      <c r="B63" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="C63" s="32"/>
+      <c r="D63" s="32"/>
+      <c r="E63" s="32"/>
+      <c r="F63" s="32"/>
+      <c r="G63" s="32"/>
+      <c r="H63" s="32"/>
+      <c r="I63" s="32"/>
+      <c r="J63" s="32"/>
+      <c r="K63" s="32"/>
+      <c r="L63" s="32"/>
+      <c r="M63" s="32"/>
+      <c r="N63" s="32"/>
+      <c r="O63" s="32"/>
+      <c r="P63" s="32"/>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
         <v>40</v>
       </c>
-      <c r="B64" s="30" t="s">
+      <c r="B64" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="C64" s="32"/>
+      <c r="D64" s="32"/>
+      <c r="E64" s="32"/>
+      <c r="F64" s="32"/>
+      <c r="G64" s="32"/>
+      <c r="H64" s="32"/>
+      <c r="I64" s="32"/>
+      <c r="J64" s="32"/>
+      <c r="K64" s="32"/>
+      <c r="L64" s="32"/>
+      <c r="M64" s="32"/>
+      <c r="N64" s="32"/>
+      <c r="O64" s="32"/>
+      <c r="P64" s="32"/>
+    </row>
+    <row r="65" spans="1:16" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="7">
+        <v>41</v>
+      </c>
+      <c r="B65" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="C64" s="30"/>
-      <c r="D64" s="30"/>
-      <c r="E64" s="30"/>
-      <c r="F64" s="30"/>
-      <c r="G64" s="30"/>
-      <c r="H64" s="30"/>
-      <c r="I64" s="30"/>
-      <c r="J64" s="30"/>
-      <c r="K64" s="30"/>
-      <c r="L64" s="30"/>
-      <c r="M64" s="30"/>
-      <c r="N64" s="30"/>
-      <c r="O64" s="30"/>
-      <c r="P64" s="30"/>
-    </row>
-    <row r="65" spans="1:16" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65">
-        <v>41</v>
-      </c>
-      <c r="B65" s="28" t="s">
-        <v>74</v>
-      </c>
-      <c r="C65" s="28"/>
-      <c r="D65" s="28"/>
-      <c r="E65" s="28"/>
-      <c r="F65" s="28"/>
-      <c r="G65" s="28"/>
-      <c r="H65" s="28"/>
-      <c r="I65" s="28"/>
-      <c r="J65" s="28"/>
-      <c r="K65" s="28"/>
-      <c r="L65" s="28"/>
-      <c r="M65" s="28"/>
-      <c r="N65" s="28"/>
-      <c r="O65" s="28"/>
-      <c r="P65" s="28"/>
+      <c r="C65" s="30"/>
+      <c r="D65" s="30"/>
+      <c r="E65" s="30"/>
+      <c r="F65" s="30"/>
+      <c r="G65" s="30"/>
+      <c r="H65" s="30"/>
+      <c r="I65" s="30"/>
+      <c r="J65" s="30"/>
+      <c r="K65" s="30"/>
+      <c r="L65" s="30"/>
+      <c r="M65" s="30"/>
+      <c r="N65" s="30"/>
+      <c r="O65" s="30"/>
+      <c r="P65" s="30"/>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" s="7">
         <v>42</v>
       </c>
-      <c r="B66" s="31" t="s">
+      <c r="B66" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="C66" s="34"/>
+      <c r="D66" s="34"/>
+      <c r="E66" s="34"/>
+      <c r="F66" s="34"/>
+      <c r="G66" s="34"/>
+      <c r="H66" s="34"/>
+      <c r="I66" s="34"/>
+      <c r="J66" s="34"/>
+      <c r="K66" s="34"/>
+      <c r="L66" s="34"/>
+      <c r="M66" s="34"/>
+      <c r="N66" s="34"/>
+      <c r="O66" s="34"/>
+      <c r="P66" s="34"/>
+    </row>
+    <row r="67" spans="1:16" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="22">
+        <v>43</v>
+      </c>
+      <c r="B67" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="C66" s="31"/>
-      <c r="D66" s="31"/>
-      <c r="E66" s="31"/>
-      <c r="F66" s="31"/>
-      <c r="G66" s="31"/>
-      <c r="H66" s="31"/>
-      <c r="I66" s="31"/>
-      <c r="J66" s="31"/>
-      <c r="K66" s="31"/>
-      <c r="L66" s="31"/>
-      <c r="M66" s="31"/>
-      <c r="N66" s="31"/>
-      <c r="O66" s="31"/>
-      <c r="P66" s="31"/>
-    </row>
-    <row r="67" spans="1:16" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="23">
-        <v>43</v>
-      </c>
-      <c r="B67" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="C67" s="28"/>
-      <c r="D67" s="28"/>
-      <c r="E67" s="28"/>
-      <c r="F67" s="28"/>
-      <c r="G67" s="28"/>
-      <c r="H67" s="28"/>
-      <c r="I67" s="28"/>
-      <c r="J67" s="28"/>
-      <c r="K67" s="28"/>
-      <c r="L67" s="28"/>
-      <c r="M67" s="28"/>
-      <c r="N67" s="28"/>
-      <c r="O67" s="28"/>
-      <c r="P67" s="28"/>
+      <c r="C67" s="33"/>
+      <c r="D67" s="33"/>
+      <c r="E67" s="33"/>
+      <c r="F67" s="33"/>
+      <c r="G67" s="33"/>
+      <c r="H67" s="33"/>
+      <c r="I67" s="33"/>
+      <c r="J67" s="33"/>
+      <c r="K67" s="33"/>
+      <c r="L67" s="33"/>
+      <c r="M67" s="33"/>
+      <c r="N67" s="33"/>
+      <c r="O67" s="33"/>
+      <c r="P67" s="33"/>
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68" s="7">
         <v>44</v>
       </c>
-      <c r="B68" s="29" t="s">
+      <c r="B68" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="C68" s="38"/>
+      <c r="D68" s="38"/>
+      <c r="E68" s="38"/>
+      <c r="F68" s="38"/>
+      <c r="G68" s="38"/>
+      <c r="H68" s="38"/>
+      <c r="I68" s="38"/>
+      <c r="J68" s="38"/>
+      <c r="K68" s="38"/>
+      <c r="L68" s="38"/>
+      <c r="M68" s="38"/>
+      <c r="N68" s="38"/>
+      <c r="O68" s="38"/>
+      <c r="P68" s="38"/>
+    </row>
+    <row r="69" spans="1:16" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="24">
+        <v>45</v>
+      </c>
+      <c r="B69" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="C68" s="29"/>
-      <c r="D68" s="29"/>
-      <c r="E68" s="29"/>
-      <c r="F68" s="29"/>
-      <c r="G68" s="29"/>
-      <c r="H68" s="29"/>
-      <c r="I68" s="29"/>
-      <c r="J68" s="29"/>
-      <c r="K68" s="29"/>
-      <c r="L68" s="29"/>
-      <c r="M68" s="29"/>
-      <c r="N68" s="29"/>
-      <c r="O68" s="29"/>
-      <c r="P68" s="29"/>
-    </row>
-    <row r="69" spans="1:16" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="25">
-        <v>45</v>
-      </c>
-      <c r="B69" s="34" t="s">
-        <v>71</v>
-      </c>
-      <c r="C69" s="34"/>
-      <c r="D69" s="34"/>
-      <c r="E69" s="34"/>
-      <c r="F69" s="34"/>
-      <c r="G69" s="34"/>
-      <c r="H69" s="34"/>
-      <c r="I69" s="34"/>
-      <c r="J69" s="34"/>
-      <c r="K69" s="34"/>
-      <c r="L69" s="34"/>
-      <c r="M69" s="34"/>
-      <c r="N69" s="34"/>
-      <c r="O69" s="34"/>
-      <c r="P69" s="34"/>
+      <c r="C69" s="30"/>
+      <c r="D69" s="30"/>
+      <c r="E69" s="30"/>
+      <c r="F69" s="30"/>
+      <c r="G69" s="30"/>
+      <c r="H69" s="30"/>
+      <c r="I69" s="30"/>
+      <c r="J69" s="30"/>
+      <c r="K69" s="30"/>
+      <c r="L69" s="30"/>
+      <c r="M69" s="30"/>
+      <c r="N69" s="30"/>
+      <c r="O69" s="30"/>
+      <c r="P69" s="30"/>
     </row>
     <row r="89" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A89" s="7">
         <v>46</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C89" s="7"/>
       <c r="D89" s="7"/>
@@ -4045,7 +4057,7 @@
         <v>47</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C90" s="7"/>
       <c r="D90" s="7"/>
@@ -4066,92 +4078,128 @@
       <c r="A91" s="9">
         <v>48</v>
       </c>
-      <c r="B91" s="41" t="s">
-        <v>85</v>
-      </c>
-      <c r="C91" s="41"/>
-      <c r="D91" s="41"/>
-      <c r="E91" s="41"/>
-      <c r="F91" s="41"/>
-      <c r="G91" s="41"/>
-      <c r="H91" s="41"/>
-      <c r="I91" s="41"/>
-      <c r="J91" s="41"/>
-      <c r="K91" s="41"/>
-      <c r="L91" s="41"/>
-      <c r="M91" s="41"/>
-      <c r="N91" s="41"/>
-      <c r="O91" s="41"/>
-      <c r="P91" s="41"/>
+      <c r="B91" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="C91" s="39"/>
+      <c r="D91" s="39"/>
+      <c r="E91" s="39"/>
+      <c r="F91" s="39"/>
+      <c r="G91" s="39"/>
+      <c r="H91" s="39"/>
+      <c r="I91" s="39"/>
+      <c r="J91" s="39"/>
+      <c r="K91" s="39"/>
+      <c r="L91" s="39"/>
+      <c r="M91" s="39"/>
+      <c r="N91" s="39"/>
+      <c r="O91" s="39"/>
+      <c r="P91" s="39"/>
     </row>
     <row r="92" spans="1:16" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="25">
+      <c r="A92" s="24">
         <v>49</v>
       </c>
-      <c r="B92" s="40" t="s">
-        <v>79</v>
-      </c>
-      <c r="C92" s="40"/>
-      <c r="D92" s="40"/>
-      <c r="E92" s="40"/>
-      <c r="F92" s="40"/>
-      <c r="G92" s="40"/>
-      <c r="H92" s="40"/>
-      <c r="I92" s="40"/>
-      <c r="J92" s="40"/>
-      <c r="K92" s="40"/>
-      <c r="L92" s="40"/>
-      <c r="M92" s="40"/>
-      <c r="N92" s="40"/>
-      <c r="O92" s="40"/>
-      <c r="P92" s="40"/>
+      <c r="B92" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="C92" s="35"/>
+      <c r="D92" s="35"/>
+      <c r="E92" s="35"/>
+      <c r="F92" s="35"/>
+      <c r="G92" s="35"/>
+      <c r="H92" s="35"/>
+      <c r="I92" s="35"/>
+      <c r="J92" s="35"/>
+      <c r="K92" s="35"/>
+      <c r="L92" s="35"/>
+      <c r="M92" s="35"/>
+      <c r="N92" s="35"/>
+      <c r="O92" s="35"/>
+      <c r="P92" s="35"/>
     </row>
     <row r="93" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="26">
+      <c r="A93" s="25">
         <v>50</v>
       </c>
-      <c r="B93" s="27" t="s">
-        <v>78</v>
-      </c>
-      <c r="C93" s="27"/>
-      <c r="D93" s="27"/>
-      <c r="E93" s="27"/>
-      <c r="F93" s="27"/>
-      <c r="G93" s="27"/>
-      <c r="H93" s="27"/>
-      <c r="I93" s="27"/>
-      <c r="J93" s="27"/>
-      <c r="K93" s="27"/>
-      <c r="L93" s="27"/>
-      <c r="M93" s="27"/>
-      <c r="N93" s="27"/>
-      <c r="O93" s="27"/>
-      <c r="P93" s="27"/>
+      <c r="B93" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="C93" s="36"/>
+      <c r="D93" s="36"/>
+      <c r="E93" s="36"/>
+      <c r="F93" s="36"/>
+      <c r="G93" s="36"/>
+      <c r="H93" s="36"/>
+      <c r="I93" s="36"/>
+      <c r="J93" s="36"/>
+      <c r="K93" s="36"/>
+      <c r="L93" s="36"/>
+      <c r="M93" s="36"/>
+      <c r="N93" s="36"/>
+      <c r="O93" s="36"/>
+      <c r="P93" s="36"/>
     </row>
     <row r="94" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A94" s="7">
         <v>51</v>
       </c>
-      <c r="B94" s="39" t="s">
-        <v>80</v>
-      </c>
-      <c r="C94" s="39"/>
-      <c r="D94" s="39"/>
-      <c r="E94" s="39"/>
-      <c r="F94" s="39"/>
-      <c r="G94" s="39"/>
-      <c r="H94" s="39"/>
-      <c r="I94" s="39"/>
-      <c r="J94" s="39"/>
-      <c r="K94" s="39"/>
-      <c r="L94" s="39"/>
-      <c r="M94" s="39"/>
-      <c r="N94" s="39"/>
-      <c r="O94" s="39"/>
-      <c r="P94" s="39"/>
+      <c r="B94" s="37" t="s">
+        <v>79</v>
+      </c>
+      <c r="C94" s="37"/>
+      <c r="D94" s="37"/>
+      <c r="E94" s="37"/>
+      <c r="F94" s="37"/>
+      <c r="G94" s="37"/>
+      <c r="H94" s="37"/>
+      <c r="I94" s="37"/>
+      <c r="J94" s="37"/>
+      <c r="K94" s="37"/>
+      <c r="L94" s="37"/>
+      <c r="M94" s="37"/>
+      <c r="N94" s="37"/>
+      <c r="O94" s="37"/>
+      <c r="P94" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="48">
+    <mergeCell ref="B92:P92"/>
+    <mergeCell ref="B93:P93"/>
+    <mergeCell ref="B94:P94"/>
+    <mergeCell ref="B67:P67"/>
+    <mergeCell ref="B68:P68"/>
+    <mergeCell ref="B69:P69"/>
+    <mergeCell ref="B91:P91"/>
+    <mergeCell ref="B63:P63"/>
+    <mergeCell ref="B64:P64"/>
+    <mergeCell ref="B65:P65"/>
+    <mergeCell ref="B66:P66"/>
+    <mergeCell ref="B62:P62"/>
+    <mergeCell ref="B59:P59"/>
+    <mergeCell ref="B60:P60"/>
+    <mergeCell ref="B61:P61"/>
+    <mergeCell ref="B26:P26"/>
+    <mergeCell ref="B27:P27"/>
+    <mergeCell ref="B52:P52"/>
+    <mergeCell ref="B58:P58"/>
+    <mergeCell ref="B57:P57"/>
+    <mergeCell ref="B56:P56"/>
+    <mergeCell ref="B55:P55"/>
+    <mergeCell ref="B54:P54"/>
+    <mergeCell ref="B53:P53"/>
+    <mergeCell ref="B25:P25"/>
+    <mergeCell ref="B14:P14"/>
+    <mergeCell ref="B15:P15"/>
+    <mergeCell ref="B16:P16"/>
+    <mergeCell ref="B17:P17"/>
+    <mergeCell ref="B18:P18"/>
+    <mergeCell ref="B19:P19"/>
+    <mergeCell ref="B20:P20"/>
+    <mergeCell ref="B21:P21"/>
+    <mergeCell ref="B22:P22"/>
+    <mergeCell ref="B23:P23"/>
+    <mergeCell ref="B24:P24"/>
     <mergeCell ref="B13:P13"/>
     <mergeCell ref="B2:P2"/>
     <mergeCell ref="B3:P3"/>
@@ -4164,42 +4212,6 @@
     <mergeCell ref="B10:P10"/>
     <mergeCell ref="B11:P11"/>
     <mergeCell ref="B12:P12"/>
-    <mergeCell ref="B25:P25"/>
-    <mergeCell ref="B14:P14"/>
-    <mergeCell ref="B15:P15"/>
-    <mergeCell ref="B16:P16"/>
-    <mergeCell ref="B17:P17"/>
-    <mergeCell ref="B18:P18"/>
-    <mergeCell ref="B19:P19"/>
-    <mergeCell ref="B20:P20"/>
-    <mergeCell ref="B21:P21"/>
-    <mergeCell ref="B22:P22"/>
-    <mergeCell ref="B23:P23"/>
-    <mergeCell ref="B24:P24"/>
-    <mergeCell ref="B59:P59"/>
-    <mergeCell ref="B60:P60"/>
-    <mergeCell ref="B61:P61"/>
-    <mergeCell ref="B26:P26"/>
-    <mergeCell ref="B27:P27"/>
-    <mergeCell ref="B52:P52"/>
-    <mergeCell ref="B58:P58"/>
-    <mergeCell ref="B57:P57"/>
-    <mergeCell ref="B56:P56"/>
-    <mergeCell ref="B55:P55"/>
-    <mergeCell ref="B54:P54"/>
-    <mergeCell ref="B53:P53"/>
-    <mergeCell ref="B63:P63"/>
-    <mergeCell ref="B64:P64"/>
-    <mergeCell ref="B65:P65"/>
-    <mergeCell ref="B66:P66"/>
-    <mergeCell ref="B62:P62"/>
-    <mergeCell ref="B92:P92"/>
-    <mergeCell ref="B93:P93"/>
-    <mergeCell ref="B94:P94"/>
-    <mergeCell ref="B67:P67"/>
-    <mergeCell ref="B68:P68"/>
-    <mergeCell ref="B69:P69"/>
-    <mergeCell ref="B91:P91"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Připomínky kromě 32, 51
</commit_message>
<xml_diff>
--- a/MDM/WorkSheet.xlsx
+++ b/MDM/WorkSheet.xlsx
@@ -10,13 +10,13 @@
     <sheet name="WorkSheet" sheetId="1" r:id="rId1"/>
     <sheet name="Připomínky" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="145621"/>
   <fileRecoveryPr autoRecover="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="92">
   <si>
     <t>Úvodní schůze</t>
   </si>
@@ -127,9 +127,6 @@
   </si>
   <si>
     <t>Opravy připomínek</t>
-  </si>
-  <si>
-    <t>hardwarový klíč</t>
   </si>
   <si>
     <t>při přepínání segmentů se objeví D13 = 1</t>
@@ -424,6 +421,15 @@
   </si>
   <si>
     <t xml:space="preserve">  V tomto okamžiku nelze okno s chybami zavřít. Windows píše:" Neodpovídá". Viz obrázek.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Změní-li uživatel v průběhu procedury jazyk, program spadne a opět se nahodí, avšak procedura se mezitím ukončí a zmizí. </t>
+  </si>
+  <si>
+    <t>hardwarový klíč - dočasne nevyžadovat HW Klíč - (Naplánovat schůzku v příbrami)</t>
+  </si>
+  <si>
+    <t>!!! Ověřit !!!</t>
   </si>
 </sst>
 </file>
@@ -1065,7 +1071,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="3" applyAlignment="1">
@@ -1168,6 +1174,10 @@
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="5"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % – Zvýraznění1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1676,10 +1686,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H113"/>
+  <dimension ref="A1:H116"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="A113" sqref="A113:C113"/>
+    <sheetView showGridLines="0" topLeftCell="A86" workbookViewId="0">
+      <selection activeCell="A116" sqref="A116:C116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1717,11 +1727,11 @@
       </c>
       <c r="F2" s="4">
         <f>SUM(C:C)</f>
-        <v>487</v>
+        <v>495</v>
       </c>
       <c r="H2" s="5">
         <f>F2*300</f>
-        <v>146100</v>
+        <v>148500</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -2715,6 +2725,30 @@
       </c>
       <c r="C113">
         <v>3</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" s="1">
+        <v>42977</v>
+      </c>
+      <c r="C114">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" s="1">
+        <v>42979</v>
+      </c>
+      <c r="C115">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="1">
+        <v>42980</v>
+      </c>
+      <c r="C116">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -2724,10 +2758,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:P99"/>
+  <dimension ref="A2:S119"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:P2"/>
+    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="L100" sqref="L100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2740,7 +2774,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="40" t="s">
-        <v>37</v>
+        <v>90</v>
       </c>
       <c r="C2" s="40"/>
       <c r="D2" s="40"/>
@@ -2762,7 +2796,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="40" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C3" s="40"/>
       <c r="D3" s="40"/>
@@ -2784,7 +2818,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="40" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C4" s="40"/>
       <c r="D4" s="40"/>
@@ -2806,7 +2840,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="40" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C5" s="40"/>
       <c r="D5" s="40"/>
@@ -2828,7 +2862,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="40" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6" s="40"/>
       <c r="D6" s="40"/>
@@ -2850,7 +2884,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="40" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C7" s="40"/>
       <c r="D7" s="40"/>
@@ -2872,7 +2906,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="40" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C8" s="40"/>
       <c r="D8" s="40"/>
@@ -2894,7 +2928,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="40" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C9" s="40"/>
       <c r="D9" s="40"/>
@@ -2916,7 +2950,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="45" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C10" s="45"/>
       <c r="D10" s="45"/>
@@ -2938,7 +2972,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="40" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C11" s="40"/>
       <c r="D11" s="40"/>
@@ -2960,7 +2994,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="40" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" s="40"/>
       <c r="D12" s="40"/>
@@ -2982,7 +3016,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="40" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C13" s="40"/>
       <c r="D13" s="40"/>
@@ -3004,7 +3038,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="40" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C14" s="40"/>
       <c r="D14" s="40"/>
@@ -3026,7 +3060,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="45" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C15" s="45"/>
       <c r="D15" s="45"/>
@@ -3048,7 +3082,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="40" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C16" s="40"/>
       <c r="D16" s="40"/>
@@ -3070,7 +3104,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="40" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C17" s="40"/>
       <c r="D17" s="40"/>
@@ -3092,7 +3126,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="40" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C18" s="40"/>
       <c r="D18" s="40"/>
@@ -3114,7 +3148,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="40" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C19" s="40"/>
       <c r="D19" s="40"/>
@@ -3136,7 +3170,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="40" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C20" s="40"/>
       <c r="D20" s="40"/>
@@ -3158,7 +3192,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="40" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C21" s="40"/>
       <c r="D21" s="40"/>
@@ -3180,7 +3214,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="40" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C22" s="40"/>
       <c r="D22" s="40"/>
@@ -3202,7 +3236,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="40" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C23" s="40"/>
       <c r="D23" s="40"/>
@@ -3224,7 +3258,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="40" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C24" s="40"/>
       <c r="D24" s="40"/>
@@ -3246,7 +3280,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="43" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C25" s="43"/>
       <c r="D25" s="43"/>
@@ -3268,7 +3302,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="40" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C26" s="40"/>
       <c r="D26" s="40"/>
@@ -3310,7 +3344,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C28" s="23"/>
       <c r="D28" s="23"/>
@@ -3858,7 +3892,7 @@
         <v>29</v>
       </c>
       <c r="B53" s="44" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C53" s="44"/>
       <c r="D53" s="44"/>
@@ -3880,7 +3914,7 @@
         <v>30</v>
       </c>
       <c r="B54" s="37" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C54" s="37"/>
       <c r="D54" s="37"/>
@@ -3902,7 +3936,7 @@
         <v>31</v>
       </c>
       <c r="B55" s="37" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C55" s="37"/>
       <c r="D55" s="37"/>
@@ -3924,7 +3958,7 @@
         <v>32</v>
       </c>
       <c r="B56" s="43" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C56" s="43"/>
       <c r="D56" s="43"/>
@@ -3943,7 +3977,7 @@
     </row>
     <row r="57" spans="1:16" s="26" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="28" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C57" s="27"/>
       <c r="D57" s="27"/>
@@ -3983,7 +4017,7 @@
         <v>33</v>
       </c>
       <c r="B59" s="41" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C59" s="41"/>
       <c r="D59" s="41"/>
@@ -4005,7 +4039,7 @@
         <v>34</v>
       </c>
       <c r="B60" s="40" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C60" s="40"/>
       <c r="D60" s="40"/>
@@ -4027,7 +4061,7 @@
         <v>35</v>
       </c>
       <c r="B61" s="41" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C61" s="41"/>
       <c r="D61" s="41"/>
@@ -4049,7 +4083,7 @@
         <v>36</v>
       </c>
       <c r="B62" s="37" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C62" s="37"/>
       <c r="D62" s="37"/>
@@ -4071,7 +4105,7 @@
         <v>37</v>
       </c>
       <c r="B63" s="40" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C63" s="40"/>
       <c r="D63" s="40"/>
@@ -4093,7 +4127,7 @@
         <v>38</v>
       </c>
       <c r="B64" s="40" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C64" s="40"/>
       <c r="D64" s="40"/>
@@ -4115,7 +4149,7 @@
         <v>39</v>
       </c>
       <c r="B65" s="38" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C65" s="38"/>
       <c r="D65" s="38"/>
@@ -4137,7 +4171,7 @@
         <v>40</v>
       </c>
       <c r="B66" s="38" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C66" s="38"/>
       <c r="D66" s="38"/>
@@ -4159,7 +4193,7 @@
         <v>41</v>
       </c>
       <c r="B67" s="37" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C67" s="37"/>
       <c r="D67" s="37"/>
@@ -4181,7 +4215,7 @@
         <v>42</v>
       </c>
       <c r="B68" s="39" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C68" s="39"/>
       <c r="D68" s="39"/>
@@ -4203,7 +4237,7 @@
         <v>43</v>
       </c>
       <c r="B69" s="35" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C69" s="35"/>
       <c r="D69" s="35"/>
@@ -4225,7 +4259,7 @@
         <v>44</v>
       </c>
       <c r="B70" s="36" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C70" s="36"/>
       <c r="D70" s="36"/>
@@ -4247,7 +4281,7 @@
         <v>45</v>
       </c>
       <c r="B71" s="37" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C71" s="37"/>
       <c r="D71" s="37"/>
@@ -4269,7 +4303,7 @@
         <v>46</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C91" s="7"/>
       <c r="D91" s="7"/>
@@ -4291,7 +4325,7 @@
         <v>47</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C92" s="7"/>
       <c r="D92" s="7"/>
@@ -4313,7 +4347,7 @@
         <v>48</v>
       </c>
       <c r="B93" s="32" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C93" s="32"/>
       <c r="D93" s="32"/>
@@ -4335,7 +4369,7 @@
         <v>49</v>
       </c>
       <c r="B94" s="32" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C94" s="32"/>
       <c r="D94" s="32"/>
@@ -4357,7 +4391,7 @@
         <v>50</v>
       </c>
       <c r="B95" s="33" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C95" s="33"/>
       <c r="D95" s="33"/>
@@ -4379,7 +4413,7 @@
         <v>51</v>
       </c>
       <c r="B96" s="34" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C96" s="34"/>
       <c r="D96" s="34"/>
@@ -4396,29 +4430,468 @@
       <c r="O96" s="34"/>
       <c r="P96" s="34"/>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>51</v>
       </c>
       <c r="B97" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="98" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A98" s="7">
         <v>52</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B98" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C98" s="7"/>
+      <c r="D98" s="7"/>
+      <c r="E98" s="7"/>
+      <c r="F98" s="7"/>
+      <c r="G98" s="7"/>
+      <c r="H98" s="7"/>
+      <c r="I98" s="7"/>
+      <c r="J98" s="7"/>
+      <c r="K98" s="7"/>
+      <c r="L98" s="7"/>
+      <c r="M98" s="7"/>
+      <c r="N98" s="7"/>
+      <c r="O98" s="7"/>
+      <c r="P98" s="7"/>
+      <c r="Q98" s="7"/>
+      <c r="R98" s="7"/>
+      <c r="S98" s="7"/>
+    </row>
+    <row r="99" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A99" s="7"/>
+      <c r="B99" s="7" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B99" t="s">
+      <c r="C99" s="7"/>
+      <c r="D99" s="7"/>
+      <c r="E99" s="7"/>
+      <c r="F99" s="7"/>
+      <c r="G99" s="7"/>
+      <c r="H99" s="7"/>
+      <c r="I99" s="7"/>
+      <c r="J99" s="7"/>
+      <c r="K99" s="47" t="s">
+        <v>91</v>
+      </c>
+      <c r="L99" s="7"/>
+      <c r="M99" s="7"/>
+      <c r="N99" s="7"/>
+      <c r="O99" s="7"/>
+      <c r="P99" s="7"/>
+      <c r="Q99" s="7"/>
+      <c r="R99" s="7"/>
+      <c r="S99" s="7"/>
+    </row>
+    <row r="100" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A100" s="7"/>
+      <c r="B100" s="7"/>
+      <c r="C100" s="7"/>
+      <c r="D100" s="7"/>
+      <c r="E100" s="7"/>
+      <c r="F100" s="7"/>
+      <c r="G100" s="7"/>
+      <c r="H100" s="7"/>
+      <c r="I100" s="7"/>
+      <c r="J100" s="7"/>
+      <c r="K100" s="7"/>
+      <c r="L100" s="7"/>
+      <c r="M100" s="7"/>
+      <c r="N100" s="7"/>
+      <c r="O100" s="7"/>
+      <c r="P100" s="7"/>
+      <c r="Q100" s="7"/>
+      <c r="R100" s="7"/>
+      <c r="S100" s="7"/>
+    </row>
+    <row r="101" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A101" s="7"/>
+      <c r="B101" s="7"/>
+      <c r="C101" s="7"/>
+      <c r="D101" s="7"/>
+      <c r="E101" s="7"/>
+      <c r="F101" s="7"/>
+      <c r="G101" s="7"/>
+      <c r="H101" s="7"/>
+      <c r="I101" s="7"/>
+      <c r="J101" s="7"/>
+      <c r="K101" s="7"/>
+      <c r="L101" s="7"/>
+      <c r="M101" s="7"/>
+      <c r="N101" s="7"/>
+      <c r="O101" s="7"/>
+      <c r="P101" s="7"/>
+      <c r="Q101" s="7"/>
+      <c r="R101" s="7"/>
+      <c r="S101" s="7"/>
+    </row>
+    <row r="102" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A102" s="7"/>
+      <c r="B102" s="7"/>
+      <c r="C102" s="7"/>
+      <c r="D102" s="7"/>
+      <c r="E102" s="7"/>
+      <c r="F102" s="7"/>
+      <c r="G102" s="7"/>
+      <c r="H102" s="7"/>
+      <c r="I102" s="7"/>
+      <c r="J102" s="7"/>
+      <c r="K102" s="7"/>
+      <c r="L102" s="7"/>
+      <c r="M102" s="7"/>
+      <c r="N102" s="7"/>
+      <c r="O102" s="7"/>
+      <c r="P102" s="7"/>
+      <c r="Q102" s="7"/>
+      <c r="R102" s="7"/>
+      <c r="S102" s="7"/>
+    </row>
+    <row r="103" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A103" s="7"/>
+      <c r="B103" s="7"/>
+      <c r="C103" s="7"/>
+      <c r="D103" s="7"/>
+      <c r="E103" s="7"/>
+      <c r="F103" s="7"/>
+      <c r="G103" s="7"/>
+      <c r="H103" s="7"/>
+      <c r="I103" s="7"/>
+      <c r="J103" s="7"/>
+      <c r="K103" s="7"/>
+      <c r="L103" s="7"/>
+      <c r="M103" s="7"/>
+      <c r="N103" s="7"/>
+      <c r="O103" s="7"/>
+      <c r="P103" s="7"/>
+      <c r="Q103" s="7"/>
+      <c r="R103" s="7"/>
+      <c r="S103" s="7"/>
+    </row>
+    <row r="104" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A104" s="7"/>
+      <c r="B104" s="7"/>
+      <c r="C104" s="7"/>
+      <c r="D104" s="7"/>
+      <c r="E104" s="7"/>
+      <c r="F104" s="7"/>
+      <c r="G104" s="7"/>
+      <c r="H104" s="7"/>
+      <c r="I104" s="7"/>
+      <c r="J104" s="7"/>
+      <c r="K104" s="7"/>
+      <c r="L104" s="7"/>
+      <c r="M104" s="7"/>
+      <c r="N104" s="7"/>
+      <c r="O104" s="7"/>
+      <c r="P104" s="7"/>
+      <c r="Q104" s="7"/>
+      <c r="R104" s="7"/>
+      <c r="S104" s="7"/>
+    </row>
+    <row r="105" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A105" s="7"/>
+      <c r="B105" s="7"/>
+      <c r="C105" s="7"/>
+      <c r="D105" s="7"/>
+      <c r="E105" s="7"/>
+      <c r="F105" s="7"/>
+      <c r="G105" s="7"/>
+      <c r="H105" s="7"/>
+      <c r="I105" s="7"/>
+      <c r="J105" s="7"/>
+      <c r="K105" s="7"/>
+      <c r="L105" s="7"/>
+      <c r="M105" s="7"/>
+      <c r="N105" s="7"/>
+      <c r="O105" s="7"/>
+      <c r="P105" s="7"/>
+      <c r="Q105" s="7"/>
+      <c r="R105" s="7"/>
+      <c r="S105" s="7"/>
+    </row>
+    <row r="106" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A106" s="7"/>
+      <c r="B106" s="7"/>
+      <c r="C106" s="7"/>
+      <c r="D106" s="7"/>
+      <c r="E106" s="7"/>
+      <c r="F106" s="7"/>
+      <c r="G106" s="7"/>
+      <c r="H106" s="7"/>
+      <c r="I106" s="7"/>
+      <c r="J106" s="7"/>
+      <c r="K106" s="7"/>
+      <c r="L106" s="7"/>
+      <c r="M106" s="7"/>
+      <c r="N106" s="7"/>
+      <c r="O106" s="7"/>
+      <c r="P106" s="7"/>
+      <c r="Q106" s="7"/>
+      <c r="R106" s="7"/>
+      <c r="S106" s="7"/>
+    </row>
+    <row r="107" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A107" s="7"/>
+      <c r="B107" s="7"/>
+      <c r="C107" s="7"/>
+      <c r="D107" s="7"/>
+      <c r="E107" s="7"/>
+      <c r="F107" s="7"/>
+      <c r="G107" s="7"/>
+      <c r="H107" s="7"/>
+      <c r="I107" s="7"/>
+      <c r="J107" s="7"/>
+      <c r="K107" s="7"/>
+      <c r="L107" s="7"/>
+      <c r="M107" s="7"/>
+      <c r="N107" s="7"/>
+      <c r="O107" s="7"/>
+      <c r="P107" s="7"/>
+      <c r="Q107" s="7"/>
+      <c r="R107" s="7"/>
+      <c r="S107" s="7"/>
+    </row>
+    <row r="108" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A108" s="7"/>
+      <c r="B108" s="7"/>
+      <c r="C108" s="7"/>
+      <c r="D108" s="7"/>
+      <c r="E108" s="7"/>
+      <c r="F108" s="7"/>
+      <c r="G108" s="7"/>
+      <c r="H108" s="7"/>
+      <c r="I108" s="7"/>
+      <c r="J108" s="7"/>
+      <c r="K108" s="7"/>
+      <c r="L108" s="7"/>
+      <c r="M108" s="7"/>
+      <c r="N108" s="7"/>
+      <c r="O108" s="7"/>
+      <c r="P108" s="7"/>
+      <c r="Q108" s="7"/>
+      <c r="R108" s="7"/>
+      <c r="S108" s="7"/>
+    </row>
+    <row r="109" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A109" s="7"/>
+      <c r="B109" s="7"/>
+      <c r="C109" s="7"/>
+      <c r="D109" s="7"/>
+      <c r="E109" s="7"/>
+      <c r="F109" s="7"/>
+      <c r="G109" s="7"/>
+      <c r="H109" s="7"/>
+      <c r="I109" s="7"/>
+      <c r="J109" s="7"/>
+      <c r="K109" s="7"/>
+      <c r="L109" s="7"/>
+      <c r="M109" s="7"/>
+      <c r="N109" s="7"/>
+      <c r="O109" s="7"/>
+      <c r="P109" s="7"/>
+      <c r="Q109" s="7"/>
+      <c r="R109" s="7"/>
+      <c r="S109" s="7"/>
+    </row>
+    <row r="110" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A110" s="7"/>
+      <c r="B110" s="7"/>
+      <c r="C110" s="7"/>
+      <c r="D110" s="7"/>
+      <c r="E110" s="7"/>
+      <c r="F110" s="7"/>
+      <c r="G110" s="7"/>
+      <c r="H110" s="7"/>
+      <c r="I110" s="7"/>
+      <c r="J110" s="7"/>
+      <c r="K110" s="7"/>
+      <c r="L110" s="7"/>
+      <c r="M110" s="7"/>
+      <c r="N110" s="7"/>
+      <c r="O110" s="7"/>
+      <c r="P110" s="7"/>
+      <c r="Q110" s="7"/>
+      <c r="R110" s="7"/>
+      <c r="S110" s="7"/>
+    </row>
+    <row r="111" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A111" s="7"/>
+      <c r="B111" s="7"/>
+      <c r="C111" s="7"/>
+      <c r="D111" s="7"/>
+      <c r="E111" s="7"/>
+      <c r="F111" s="7"/>
+      <c r="G111" s="7"/>
+      <c r="H111" s="7"/>
+      <c r="I111" s="7"/>
+      <c r="J111" s="7"/>
+      <c r="K111" s="7"/>
+      <c r="L111" s="7"/>
+      <c r="M111" s="7"/>
+      <c r="N111" s="7"/>
+      <c r="O111" s="7"/>
+      <c r="P111" s="7"/>
+      <c r="Q111" s="7"/>
+      <c r="R111" s="7"/>
+      <c r="S111" s="7"/>
+    </row>
+    <row r="112" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A112" s="7"/>
+      <c r="B112" s="7"/>
+      <c r="C112" s="7"/>
+      <c r="D112" s="7"/>
+      <c r="E112" s="7"/>
+      <c r="F112" s="7"/>
+      <c r="G112" s="7"/>
+      <c r="H112" s="7"/>
+      <c r="I112" s="7"/>
+      <c r="J112" s="7"/>
+      <c r="K112" s="7"/>
+      <c r="L112" s="7"/>
+      <c r="M112" s="7"/>
+      <c r="N112" s="7"/>
+      <c r="O112" s="7"/>
+      <c r="P112" s="7"/>
+      <c r="Q112" s="7"/>
+      <c r="R112" s="7"/>
+      <c r="S112" s="7"/>
+    </row>
+    <row r="113" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A113" s="7"/>
+      <c r="B113" s="7"/>
+      <c r="C113" s="7"/>
+      <c r="D113" s="7"/>
+      <c r="E113" s="7"/>
+      <c r="F113" s="7"/>
+      <c r="G113" s="7"/>
+      <c r="H113" s="7"/>
+      <c r="I113" s="7"/>
+      <c r="J113" s="7"/>
+      <c r="K113" s="7"/>
+      <c r="L113" s="7"/>
+      <c r="M113" s="7"/>
+      <c r="N113" s="7"/>
+      <c r="O113" s="7"/>
+      <c r="P113" s="7"/>
+      <c r="Q113" s="7"/>
+      <c r="R113" s="7"/>
+      <c r="S113" s="7"/>
+    </row>
+    <row r="114" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A114" s="7"/>
+      <c r="B114" s="7"/>
+      <c r="C114" s="7"/>
+      <c r="D114" s="7"/>
+      <c r="E114" s="7"/>
+      <c r="F114" s="7"/>
+      <c r="G114" s="7"/>
+      <c r="H114" s="7"/>
+      <c r="I114" s="7"/>
+      <c r="J114" s="7"/>
+      <c r="K114" s="7"/>
+      <c r="L114" s="7"/>
+      <c r="M114" s="7"/>
+      <c r="N114" s="7"/>
+      <c r="O114" s="7"/>
+      <c r="P114" s="7"/>
+      <c r="Q114" s="7"/>
+      <c r="R114" s="7"/>
+      <c r="S114" s="7"/>
+    </row>
+    <row r="115" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A115" s="7"/>
+      <c r="B115" s="7"/>
+      <c r="C115" s="7"/>
+      <c r="D115" s="7"/>
+      <c r="E115" s="7"/>
+      <c r="F115" s="7"/>
+      <c r="G115" s="7"/>
+      <c r="H115" s="7"/>
+      <c r="I115" s="7"/>
+      <c r="J115" s="7"/>
+      <c r="K115" s="7"/>
+      <c r="L115" s="7"/>
+      <c r="M115" s="7"/>
+      <c r="N115" s="7"/>
+      <c r="O115" s="7"/>
+      <c r="P115" s="7"/>
+      <c r="Q115" s="7"/>
+      <c r="R115" s="7"/>
+      <c r="S115" s="7"/>
+    </row>
+    <row r="116" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A116" s="7"/>
+      <c r="B116" s="7"/>
+      <c r="C116" s="7"/>
+      <c r="D116" s="7"/>
+      <c r="E116" s="7"/>
+      <c r="F116" s="7"/>
+      <c r="G116" s="7"/>
+      <c r="H116" s="7"/>
+      <c r="I116" s="7"/>
+      <c r="J116" s="7"/>
+      <c r="K116" s="7"/>
+      <c r="L116" s="7"/>
+      <c r="M116" s="7"/>
+      <c r="N116" s="7"/>
+      <c r="O116" s="7"/>
+      <c r="P116" s="7"/>
+      <c r="Q116" s="7"/>
+      <c r="R116" s="7"/>
+      <c r="S116" s="7"/>
+    </row>
+    <row r="117" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A117" s="7"/>
+      <c r="B117" s="7"/>
+      <c r="C117" s="7"/>
+      <c r="D117" s="7"/>
+      <c r="E117" s="7"/>
+      <c r="F117" s="7"/>
+      <c r="G117" s="7"/>
+      <c r="H117" s="7"/>
+      <c r="I117" s="7"/>
+      <c r="J117" s="7"/>
+      <c r="K117" s="7"/>
+      <c r="L117" s="7"/>
+      <c r="M117" s="7"/>
+      <c r="N117" s="7"/>
+      <c r="O117" s="7"/>
+      <c r="P117" s="7"/>
+      <c r="Q117" s="7"/>
+      <c r="R117" s="7"/>
+      <c r="S117" s="7"/>
+    </row>
+    <row r="118" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A118" s="7">
+        <v>53</v>
+      </c>
+      <c r="B118" s="46" t="s">
         <v>89</v>
       </c>
+      <c r="C118" s="46"/>
+      <c r="D118" s="46"/>
+      <c r="E118" s="46"/>
+      <c r="F118" s="46"/>
+      <c r="G118" s="46"/>
+      <c r="H118" s="46"/>
+      <c r="I118" s="46"/>
+      <c r="J118" s="46"/>
+      <c r="K118" s="46"/>
+      <c r="L118" s="46"/>
+      <c r="M118" s="46"/>
+    </row>
+    <row r="119" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>54</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="48">
+  <mergeCells count="49">
     <mergeCell ref="B13:P13"/>
     <mergeCell ref="B2:P2"/>
     <mergeCell ref="B3:P3"/>
@@ -4460,6 +4933,7 @@
     <mergeCell ref="B67:P67"/>
     <mergeCell ref="B68:P68"/>
     <mergeCell ref="B64:P64"/>
+    <mergeCell ref="B118:M118"/>
     <mergeCell ref="B94:P94"/>
     <mergeCell ref="B95:P95"/>
     <mergeCell ref="B96:P96"/>

</xml_diff>

<commit_message>
Výsledek návštěvy v Příbrami
</commit_message>
<xml_diff>
--- a/MDM/WorkSheet.xlsx
+++ b/MDM/WorkSheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="96">
   <si>
     <t>Úvodní schůze</t>
   </si>
@@ -420,16 +420,42 @@
     <t>Po obnovení komunikace (odpojení a znovu připojení LAN kabelu k Desce LAN) proběhne Autotest s validními chybami.Před zahájením procedury byl funkční poze kanál č. 1 (ostatní nejsou připojené)</t>
   </si>
   <si>
-    <t xml:space="preserve">  V tomto okamžiku nelze okno s chybami zavřít. Windows píše:" Neodpovídá". Viz obrázek.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Změní-li uživatel v průběhu procedury jazyk, program spadne a opět se nahodí, avšak procedura se mezitím ukončí a zmizí. </t>
   </si>
   <si>
     <t>hardwarový klíč - dočasne nevyžadovat HW Klíč - (Naplánovat schůzku v příbrami)</t>
   </si>
   <si>
-    <t>!!! Ověřit !!!</t>
+    <r>
+      <t xml:space="preserve">  V tomto okamžiku nelze okno s chybami zavřít. Windows píše:" Neodpovídá". Viz obrázek. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>!!! Ověřit !!! Stále přetrvává</t>
+    </r>
+  </si>
+  <si>
+    <t>Informace (pole) "Zdravotní pojišťovna" úplně odstranit (v praxi se nikdy nevyužije)</t>
+  </si>
+  <si>
+    <t>Pro test vodivosti přidat neutrální odlišné krátké potvzující pípnutí (přechod mezi "Připojte elektrody" a "Kanál připraven"), aby sestra otočená zády k přístroji slyšela, že pacient už je připojen.</t>
+  </si>
+  <si>
+    <t>Pro Superadmina dát info, že tam není zastrčená flashka</t>
+  </si>
+  <si>
+    <t>Bílé číslice do monitoru, upravit opacity, světlejší zelená do sloupce</t>
+  </si>
+  <si>
+    <t>Z monitoru vyhodit DOUT, přidat rozdíl AIN2-AIN1</t>
   </si>
 </sst>
 </file>
@@ -652,7 +678,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="46">
+  <fills count="47">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -910,6 +936,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1071,7 +1103,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="3" applyAlignment="1">
@@ -1132,6 +1164,11 @@
       <alignment horizontal="left" vertical="center" indent="5"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="46" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="46" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1174,10 +1211,7 @@
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="5"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % – Zvýraznění1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2758,10 +2792,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:S119"/>
+  <dimension ref="A2:S123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="L100" sqref="L100"/>
+    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="B123" sqref="B123:S123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2773,571 +2807,571 @@
       <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="40" t="s">
-        <v>90</v>
-      </c>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40"/>
-      <c r="N2" s="40"/>
-      <c r="O2" s="40"/>
-      <c r="P2" s="40"/>
+      <c r="B2" s="43" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="43"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="43"/>
+      <c r="N2" s="43"/>
+      <c r="O2" s="43"/>
+      <c r="P2" s="43"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>2</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="40"/>
-      <c r="J3" s="40"/>
-      <c r="K3" s="40"/>
-      <c r="L3" s="40"/>
-      <c r="M3" s="40"/>
-      <c r="N3" s="40"/>
-      <c r="O3" s="40"/>
-      <c r="P3" s="40"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
+      <c r="K3" s="43"/>
+      <c r="L3" s="43"/>
+      <c r="M3" s="43"/>
+      <c r="N3" s="43"/>
+      <c r="O3" s="43"/>
+      <c r="P3" s="43"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>3</v>
       </c>
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="43" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
-      <c r="K4" s="40"/>
-      <c r="L4" s="40"/>
-      <c r="M4" s="40"/>
-      <c r="N4" s="40"/>
-      <c r="O4" s="40"/>
-      <c r="P4" s="40"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="43"/>
+      <c r="J4" s="43"/>
+      <c r="K4" s="43"/>
+      <c r="L4" s="43"/>
+      <c r="M4" s="43"/>
+      <c r="N4" s="43"/>
+      <c r="O4" s="43"/>
+      <c r="P4" s="43"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>4</v>
       </c>
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="40"/>
-      <c r="I5" s="40"/>
-      <c r="J5" s="40"/>
-      <c r="K5" s="40"/>
-      <c r="L5" s="40"/>
-      <c r="M5" s="40"/>
-      <c r="N5" s="40"/>
-      <c r="O5" s="40"/>
-      <c r="P5" s="40"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="43"/>
+      <c r="I5" s="43"/>
+      <c r="J5" s="43"/>
+      <c r="K5" s="43"/>
+      <c r="L5" s="43"/>
+      <c r="M5" s="43"/>
+      <c r="N5" s="43"/>
+      <c r="O5" s="43"/>
+      <c r="P5" s="43"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>5</v>
       </c>
-      <c r="B6" s="40" t="s">
+      <c r="B6" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="40"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="40"/>
-      <c r="H6" s="40"/>
-      <c r="I6" s="40"/>
-      <c r="J6" s="40"/>
-      <c r="K6" s="40"/>
-      <c r="L6" s="40"/>
-      <c r="M6" s="40"/>
-      <c r="N6" s="40"/>
-      <c r="O6" s="40"/>
-      <c r="P6" s="40"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43"/>
+      <c r="J6" s="43"/>
+      <c r="K6" s="43"/>
+      <c r="L6" s="43"/>
+      <c r="M6" s="43"/>
+      <c r="N6" s="43"/>
+      <c r="O6" s="43"/>
+      <c r="P6" s="43"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>6</v>
       </c>
-      <c r="B7" s="40" t="s">
+      <c r="B7" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="40"/>
-      <c r="D7" s="40"/>
-      <c r="E7" s="40"/>
-      <c r="F7" s="40"/>
-      <c r="G7" s="40"/>
-      <c r="H7" s="40"/>
-      <c r="I7" s="40"/>
-      <c r="J7" s="40"/>
-      <c r="K7" s="40"/>
-      <c r="L7" s="40"/>
-      <c r="M7" s="40"/>
-      <c r="N7" s="40"/>
-      <c r="O7" s="40"/>
-      <c r="P7" s="40"/>
+      <c r="C7" s="43"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
+      <c r="I7" s="43"/>
+      <c r="J7" s="43"/>
+      <c r="K7" s="43"/>
+      <c r="L7" s="43"/>
+      <c r="M7" s="43"/>
+      <c r="N7" s="43"/>
+      <c r="O7" s="43"/>
+      <c r="P7" s="43"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>7</v>
       </c>
-      <c r="B8" s="40" t="s">
+      <c r="B8" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="40"/>
-      <c r="D8" s="40"/>
-      <c r="E8" s="40"/>
-      <c r="F8" s="40"/>
-      <c r="G8" s="40"/>
-      <c r="H8" s="40"/>
-      <c r="I8" s="40"/>
-      <c r="J8" s="40"/>
-      <c r="K8" s="40"/>
-      <c r="L8" s="40"/>
-      <c r="M8" s="40"/>
-      <c r="N8" s="40"/>
-      <c r="O8" s="40"/>
-      <c r="P8" s="40"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="43"/>
+      <c r="I8" s="43"/>
+      <c r="J8" s="43"/>
+      <c r="K8" s="43"/>
+      <c r="L8" s="43"/>
+      <c r="M8" s="43"/>
+      <c r="N8" s="43"/>
+      <c r="O8" s="43"/>
+      <c r="P8" s="43"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>8</v>
       </c>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="40"/>
-      <c r="G9" s="40"/>
-      <c r="H9" s="40"/>
-      <c r="I9" s="40"/>
-      <c r="J9" s="40"/>
-      <c r="K9" s="40"/>
-      <c r="L9" s="40"/>
-      <c r="M9" s="40"/>
-      <c r="N9" s="40"/>
-      <c r="O9" s="40"/>
-      <c r="P9" s="40"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="43"/>
+      <c r="I9" s="43"/>
+      <c r="J9" s="43"/>
+      <c r="K9" s="43"/>
+      <c r="L9" s="43"/>
+      <c r="M9" s="43"/>
+      <c r="N9" s="43"/>
+      <c r="O9" s="43"/>
+      <c r="P9" s="43"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>9</v>
       </c>
-      <c r="B10" s="45" t="s">
+      <c r="B10" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="C10" s="45"/>
-      <c r="D10" s="45"/>
-      <c r="E10" s="45"/>
-      <c r="F10" s="45"/>
-      <c r="G10" s="45"/>
-      <c r="H10" s="45"/>
-      <c r="I10" s="45"/>
-      <c r="J10" s="45"/>
-      <c r="K10" s="45"/>
-      <c r="L10" s="45"/>
-      <c r="M10" s="45"/>
-      <c r="N10" s="45"/>
-      <c r="O10" s="45"/>
-      <c r="P10" s="45"/>
+      <c r="C10" s="48"/>
+      <c r="D10" s="48"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="48"/>
+      <c r="H10" s="48"/>
+      <c r="I10" s="48"/>
+      <c r="J10" s="48"/>
+      <c r="K10" s="48"/>
+      <c r="L10" s="48"/>
+      <c r="M10" s="48"/>
+      <c r="N10" s="48"/>
+      <c r="O10" s="48"/>
+      <c r="P10" s="48"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>10</v>
       </c>
-      <c r="B11" s="40" t="s">
+      <c r="B11" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="40"/>
-      <c r="J11" s="40"/>
-      <c r="K11" s="40"/>
-      <c r="L11" s="40"/>
-      <c r="M11" s="40"/>
-      <c r="N11" s="40"/>
-      <c r="O11" s="40"/>
-      <c r="P11" s="40"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="43"/>
+      <c r="I11" s="43"/>
+      <c r="J11" s="43"/>
+      <c r="K11" s="43"/>
+      <c r="L11" s="43"/>
+      <c r="M11" s="43"/>
+      <c r="N11" s="43"/>
+      <c r="O11" s="43"/>
+      <c r="P11" s="43"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>11</v>
       </c>
-      <c r="B12" s="40" t="s">
+      <c r="B12" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="40"/>
-      <c r="D12" s="40"/>
-      <c r="E12" s="40"/>
-      <c r="F12" s="40"/>
-      <c r="G12" s="40"/>
-      <c r="H12" s="40"/>
-      <c r="I12" s="40"/>
-      <c r="J12" s="40"/>
-      <c r="K12" s="40"/>
-      <c r="L12" s="40"/>
-      <c r="M12" s="40"/>
-      <c r="N12" s="40"/>
-      <c r="O12" s="40"/>
-      <c r="P12" s="40"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="43"/>
+      <c r="I12" s="43"/>
+      <c r="J12" s="43"/>
+      <c r="K12" s="43"/>
+      <c r="L12" s="43"/>
+      <c r="M12" s="43"/>
+      <c r="N12" s="43"/>
+      <c r="O12" s="43"/>
+      <c r="P12" s="43"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>12</v>
       </c>
-      <c r="B13" s="40" t="s">
+      <c r="B13" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="40"/>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="40"/>
-      <c r="J13" s="40"/>
-      <c r="K13" s="40"/>
-      <c r="L13" s="40"/>
-      <c r="M13" s="40"/>
-      <c r="N13" s="40"/>
-      <c r="O13" s="40"/>
-      <c r="P13" s="40"/>
+      <c r="C13" s="43"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="43"/>
+      <c r="I13" s="43"/>
+      <c r="J13" s="43"/>
+      <c r="K13" s="43"/>
+      <c r="L13" s="43"/>
+      <c r="M13" s="43"/>
+      <c r="N13" s="43"/>
+      <c r="O13" s="43"/>
+      <c r="P13" s="43"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>13</v>
       </c>
-      <c r="B14" s="40" t="s">
+      <c r="B14" s="43" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="40"/>
-      <c r="D14" s="40"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="40"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="40"/>
-      <c r="I14" s="40"/>
-      <c r="J14" s="40"/>
-      <c r="K14" s="40"/>
-      <c r="L14" s="40"/>
-      <c r="M14" s="40"/>
-      <c r="N14" s="40"/>
-      <c r="O14" s="40"/>
-      <c r="P14" s="40"/>
+      <c r="C14" s="43"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="43"/>
+      <c r="H14" s="43"/>
+      <c r="I14" s="43"/>
+      <c r="J14" s="43"/>
+      <c r="K14" s="43"/>
+      <c r="L14" s="43"/>
+      <c r="M14" s="43"/>
+      <c r="N14" s="43"/>
+      <c r="O14" s="43"/>
+      <c r="P14" s="43"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>14</v>
       </c>
-      <c r="B15" s="45" t="s">
+      <c r="B15" s="48" t="s">
         <v>63</v>
       </c>
-      <c r="C15" s="45"/>
-      <c r="D15" s="45"/>
-      <c r="E15" s="45"/>
-      <c r="F15" s="45"/>
-      <c r="G15" s="45"/>
-      <c r="H15" s="45"/>
-      <c r="I15" s="45"/>
-      <c r="J15" s="45"/>
-      <c r="K15" s="45"/>
-      <c r="L15" s="45"/>
-      <c r="M15" s="45"/>
-      <c r="N15" s="45"/>
-      <c r="O15" s="45"/>
-      <c r="P15" s="45"/>
+      <c r="C15" s="48"/>
+      <c r="D15" s="48"/>
+      <c r="E15" s="48"/>
+      <c r="F15" s="48"/>
+      <c r="G15" s="48"/>
+      <c r="H15" s="48"/>
+      <c r="I15" s="48"/>
+      <c r="J15" s="48"/>
+      <c r="K15" s="48"/>
+      <c r="L15" s="48"/>
+      <c r="M15" s="48"/>
+      <c r="N15" s="48"/>
+      <c r="O15" s="48"/>
+      <c r="P15" s="48"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <v>15</v>
       </c>
-      <c r="B16" s="40" t="s">
+      <c r="B16" s="43" t="s">
         <v>45</v>
       </c>
-      <c r="C16" s="40"/>
-      <c r="D16" s="40"/>
-      <c r="E16" s="40"/>
-      <c r="F16" s="40"/>
-      <c r="G16" s="40"/>
-      <c r="H16" s="40"/>
-      <c r="I16" s="40"/>
-      <c r="J16" s="40"/>
-      <c r="K16" s="40"/>
-      <c r="L16" s="40"/>
-      <c r="M16" s="40"/>
-      <c r="N16" s="40"/>
-      <c r="O16" s="40"/>
-      <c r="P16" s="40"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="43"/>
+      <c r="E16" s="43"/>
+      <c r="F16" s="43"/>
+      <c r="G16" s="43"/>
+      <c r="H16" s="43"/>
+      <c r="I16" s="43"/>
+      <c r="J16" s="43"/>
+      <c r="K16" s="43"/>
+      <c r="L16" s="43"/>
+      <c r="M16" s="43"/>
+      <c r="N16" s="43"/>
+      <c r="O16" s="43"/>
+      <c r="P16" s="43"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>16</v>
       </c>
-      <c r="B17" s="40" t="s">
+      <c r="B17" s="43" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="40"/>
-      <c r="D17" s="40"/>
-      <c r="E17" s="40"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="40"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="40"/>
-      <c r="K17" s="40"/>
-      <c r="L17" s="40"/>
-      <c r="M17" s="40"/>
-      <c r="N17" s="40"/>
-      <c r="O17" s="40"/>
-      <c r="P17" s="40"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="43"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="43"/>
+      <c r="G17" s="43"/>
+      <c r="H17" s="43"/>
+      <c r="I17" s="43"/>
+      <c r="J17" s="43"/>
+      <c r="K17" s="43"/>
+      <c r="L17" s="43"/>
+      <c r="M17" s="43"/>
+      <c r="N17" s="43"/>
+      <c r="O17" s="43"/>
+      <c r="P17" s="43"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <v>17</v>
       </c>
-      <c r="B18" s="40" t="s">
+      <c r="B18" s="43" t="s">
         <v>47</v>
       </c>
-      <c r="C18" s="40"/>
-      <c r="D18" s="40"/>
-      <c r="E18" s="40"/>
-      <c r="F18" s="40"/>
-      <c r="G18" s="40"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="40"/>
-      <c r="K18" s="40"/>
-      <c r="L18" s="40"/>
-      <c r="M18" s="40"/>
-      <c r="N18" s="40"/>
-      <c r="O18" s="40"/>
-      <c r="P18" s="40"/>
+      <c r="C18" s="43"/>
+      <c r="D18" s="43"/>
+      <c r="E18" s="43"/>
+      <c r="F18" s="43"/>
+      <c r="G18" s="43"/>
+      <c r="H18" s="43"/>
+      <c r="I18" s="43"/>
+      <c r="J18" s="43"/>
+      <c r="K18" s="43"/>
+      <c r="L18" s="43"/>
+      <c r="M18" s="43"/>
+      <c r="N18" s="43"/>
+      <c r="O18" s="43"/>
+      <c r="P18" s="43"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>18</v>
       </c>
-      <c r="B19" s="40" t="s">
+      <c r="B19" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="C19" s="40"/>
-      <c r="D19" s="40"/>
-      <c r="E19" s="40"/>
-      <c r="F19" s="40"/>
-      <c r="G19" s="40"/>
-      <c r="H19" s="40"/>
-      <c r="I19" s="40"/>
-      <c r="J19" s="40"/>
-      <c r="K19" s="40"/>
-      <c r="L19" s="40"/>
-      <c r="M19" s="40"/>
-      <c r="N19" s="40"/>
-      <c r="O19" s="40"/>
-      <c r="P19" s="40"/>
+      <c r="C19" s="43"/>
+      <c r="D19" s="43"/>
+      <c r="E19" s="43"/>
+      <c r="F19" s="43"/>
+      <c r="G19" s="43"/>
+      <c r="H19" s="43"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
+      <c r="K19" s="43"/>
+      <c r="L19" s="43"/>
+      <c r="M19" s="43"/>
+      <c r="N19" s="43"/>
+      <c r="O19" s="43"/>
+      <c r="P19" s="43"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
         <v>19</v>
       </c>
-      <c r="B20" s="40" t="s">
+      <c r="B20" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="40"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="40"/>
-      <c r="F20" s="40"/>
-      <c r="G20" s="40"/>
-      <c r="H20" s="40"/>
-      <c r="I20" s="40"/>
-      <c r="J20" s="40"/>
-      <c r="K20" s="40"/>
-      <c r="L20" s="40"/>
-      <c r="M20" s="40"/>
-      <c r="N20" s="40"/>
-      <c r="O20" s="40"/>
-      <c r="P20" s="40"/>
+      <c r="C20" s="43"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="43"/>
+      <c r="G20" s="43"/>
+      <c r="H20" s="43"/>
+      <c r="I20" s="43"/>
+      <c r="J20" s="43"/>
+      <c r="K20" s="43"/>
+      <c r="L20" s="43"/>
+      <c r="M20" s="43"/>
+      <c r="N20" s="43"/>
+      <c r="O20" s="43"/>
+      <c r="P20" s="43"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
         <v>20</v>
       </c>
-      <c r="B21" s="40" t="s">
+      <c r="B21" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="C21" s="40"/>
-      <c r="D21" s="40"/>
-      <c r="E21" s="40"/>
-      <c r="F21" s="40"/>
-      <c r="G21" s="40"/>
-      <c r="H21" s="40"/>
-      <c r="I21" s="40"/>
-      <c r="J21" s="40"/>
-      <c r="K21" s="40"/>
-      <c r="L21" s="40"/>
-      <c r="M21" s="40"/>
-      <c r="N21" s="40"/>
-      <c r="O21" s="40"/>
-      <c r="P21" s="40"/>
+      <c r="C21" s="43"/>
+      <c r="D21" s="43"/>
+      <c r="E21" s="43"/>
+      <c r="F21" s="43"/>
+      <c r="G21" s="43"/>
+      <c r="H21" s="43"/>
+      <c r="I21" s="43"/>
+      <c r="J21" s="43"/>
+      <c r="K21" s="43"/>
+      <c r="L21" s="43"/>
+      <c r="M21" s="43"/>
+      <c r="N21" s="43"/>
+      <c r="O21" s="43"/>
+      <c r="P21" s="43"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
         <v>21</v>
       </c>
-      <c r="B22" s="40" t="s">
+      <c r="B22" s="43" t="s">
         <v>53</v>
       </c>
-      <c r="C22" s="40"/>
-      <c r="D22" s="40"/>
-      <c r="E22" s="40"/>
-      <c r="F22" s="40"/>
-      <c r="G22" s="40"/>
-      <c r="H22" s="40"/>
-      <c r="I22" s="40"/>
-      <c r="J22" s="40"/>
-      <c r="K22" s="40"/>
-      <c r="L22" s="40"/>
-      <c r="M22" s="40"/>
-      <c r="N22" s="40"/>
-      <c r="O22" s="40"/>
-      <c r="P22" s="40"/>
+      <c r="C22" s="43"/>
+      <c r="D22" s="43"/>
+      <c r="E22" s="43"/>
+      <c r="F22" s="43"/>
+      <c r="G22" s="43"/>
+      <c r="H22" s="43"/>
+      <c r="I22" s="43"/>
+      <c r="J22" s="43"/>
+      <c r="K22" s="43"/>
+      <c r="L22" s="43"/>
+      <c r="M22" s="43"/>
+      <c r="N22" s="43"/>
+      <c r="O22" s="43"/>
+      <c r="P22" s="43"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
         <v>22</v>
       </c>
-      <c r="B23" s="40" t="s">
+      <c r="B23" s="43" t="s">
         <v>80</v>
       </c>
-      <c r="C23" s="40"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="40"/>
-      <c r="F23" s="40"/>
-      <c r="G23" s="40"/>
-      <c r="H23" s="40"/>
-      <c r="I23" s="40"/>
-      <c r="J23" s="40"/>
-      <c r="K23" s="40"/>
-      <c r="L23" s="40"/>
-      <c r="M23" s="40"/>
-      <c r="N23" s="40"/>
-      <c r="O23" s="40"/>
-      <c r="P23" s="40"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="43"/>
+      <c r="E23" s="43"/>
+      <c r="F23" s="43"/>
+      <c r="G23" s="43"/>
+      <c r="H23" s="43"/>
+      <c r="I23" s="43"/>
+      <c r="J23" s="43"/>
+      <c r="K23" s="43"/>
+      <c r="L23" s="43"/>
+      <c r="M23" s="43"/>
+      <c r="N23" s="43"/>
+      <c r="O23" s="43"/>
+      <c r="P23" s="43"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
         <v>23</v>
       </c>
-      <c r="B24" s="40" t="s">
+      <c r="B24" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="C24" s="40"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="40"/>
-      <c r="F24" s="40"/>
-      <c r="G24" s="40"/>
-      <c r="H24" s="40"/>
-      <c r="I24" s="40"/>
-      <c r="J24" s="40"/>
-      <c r="K24" s="40"/>
-      <c r="L24" s="40"/>
-      <c r="M24" s="40"/>
-      <c r="N24" s="40"/>
-      <c r="O24" s="40"/>
-      <c r="P24" s="40"/>
+      <c r="C24" s="43"/>
+      <c r="D24" s="43"/>
+      <c r="E24" s="43"/>
+      <c r="F24" s="43"/>
+      <c r="G24" s="43"/>
+      <c r="H24" s="43"/>
+      <c r="I24" s="43"/>
+      <c r="J24" s="43"/>
+      <c r="K24" s="43"/>
+      <c r="L24" s="43"/>
+      <c r="M24" s="43"/>
+      <c r="N24" s="43"/>
+      <c r="O24" s="43"/>
+      <c r="P24" s="43"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="9">
         <v>24</v>
       </c>
-      <c r="B25" s="43" t="s">
+      <c r="B25" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="C25" s="43"/>
-      <c r="D25" s="43"/>
-      <c r="E25" s="43"/>
-      <c r="F25" s="43"/>
-      <c r="G25" s="43"/>
-      <c r="H25" s="43"/>
-      <c r="I25" s="43"/>
-      <c r="J25" s="43"/>
-      <c r="K25" s="43"/>
-      <c r="L25" s="43"/>
-      <c r="M25" s="43"/>
-      <c r="N25" s="43"/>
-      <c r="O25" s="43"/>
-      <c r="P25" s="43"/>
+      <c r="C25" s="46"/>
+      <c r="D25" s="46"/>
+      <c r="E25" s="46"/>
+      <c r="F25" s="46"/>
+      <c r="G25" s="46"/>
+      <c r="H25" s="46"/>
+      <c r="I25" s="46"/>
+      <c r="J25" s="46"/>
+      <c r="K25" s="46"/>
+      <c r="L25" s="46"/>
+      <c r="M25" s="46"/>
+      <c r="N25" s="46"/>
+      <c r="O25" s="46"/>
+      <c r="P25" s="46"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
         <v>25</v>
       </c>
-      <c r="B26" s="40" t="s">
+      <c r="B26" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="C26" s="40"/>
-      <c r="D26" s="40"/>
-      <c r="E26" s="40"/>
-      <c r="F26" s="40"/>
-      <c r="G26" s="40"/>
-      <c r="H26" s="40"/>
-      <c r="I26" s="40"/>
-      <c r="J26" s="40"/>
-      <c r="K26" s="40"/>
-      <c r="L26" s="40"/>
-      <c r="M26" s="40"/>
-      <c r="N26" s="40"/>
-      <c r="O26" s="40"/>
-      <c r="P26" s="40"/>
+      <c r="C26" s="43"/>
+      <c r="D26" s="43"/>
+      <c r="E26" s="43"/>
+      <c r="F26" s="43"/>
+      <c r="G26" s="43"/>
+      <c r="H26" s="43"/>
+      <c r="I26" s="43"/>
+      <c r="J26" s="43"/>
+      <c r="K26" s="43"/>
+      <c r="L26" s="43"/>
+      <c r="M26" s="43"/>
+      <c r="N26" s="43"/>
+      <c r="O26" s="43"/>
+      <c r="P26" s="43"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
-      <c r="B27" s="42"/>
-      <c r="C27" s="42"/>
-      <c r="D27" s="42"/>
-      <c r="E27" s="42"/>
-      <c r="F27" s="42"/>
-      <c r="G27" s="42"/>
-      <c r="H27" s="42"/>
-      <c r="I27" s="42"/>
-      <c r="J27" s="42"/>
-      <c r="K27" s="42"/>
-      <c r="L27" s="42"/>
-      <c r="M27" s="42"/>
-      <c r="N27" s="42"/>
-      <c r="O27" s="42"/>
-      <c r="P27" s="42"/>
+      <c r="B27" s="45"/>
+      <c r="C27" s="45"/>
+      <c r="D27" s="45"/>
+      <c r="E27" s="45"/>
+      <c r="F27" s="45"/>
+      <c r="G27" s="45"/>
+      <c r="H27" s="45"/>
+      <c r="I27" s="45"/>
+      <c r="J27" s="45"/>
+      <c r="K27" s="45"/>
+      <c r="L27" s="45"/>
+      <c r="M27" s="45"/>
+      <c r="N27" s="45"/>
+      <c r="O27" s="45"/>
+      <c r="P27" s="45"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
@@ -3871,109 +3905,109 @@
       <c r="A52">
         <v>28</v>
       </c>
-      <c r="B52" s="42"/>
-      <c r="C52" s="42"/>
-      <c r="D52" s="42"/>
-      <c r="E52" s="42"/>
-      <c r="F52" s="42"/>
-      <c r="G52" s="42"/>
-      <c r="H52" s="42"/>
-      <c r="I52" s="42"/>
-      <c r="J52" s="42"/>
-      <c r="K52" s="42"/>
-      <c r="L52" s="42"/>
-      <c r="M52" s="42"/>
-      <c r="N52" s="42"/>
-      <c r="O52" s="42"/>
-      <c r="P52" s="42"/>
+      <c r="B52" s="45"/>
+      <c r="C52" s="45"/>
+      <c r="D52" s="45"/>
+      <c r="E52" s="45"/>
+      <c r="F52" s="45"/>
+      <c r="G52" s="45"/>
+      <c r="H52" s="45"/>
+      <c r="I52" s="45"/>
+      <c r="J52" s="45"/>
+      <c r="K52" s="45"/>
+      <c r="L52" s="45"/>
+      <c r="M52" s="45"/>
+      <c r="N52" s="45"/>
+      <c r="O52" s="45"/>
+      <c r="P52" s="45"/>
     </row>
     <row r="53" spans="1:16" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="20">
         <v>29</v>
       </c>
-      <c r="B53" s="44" t="s">
+      <c r="B53" s="47" t="s">
         <v>79</v>
       </c>
-      <c r="C53" s="44"/>
-      <c r="D53" s="44"/>
-      <c r="E53" s="44"/>
-      <c r="F53" s="44"/>
-      <c r="G53" s="44"/>
-      <c r="H53" s="44"/>
-      <c r="I53" s="44"/>
-      <c r="J53" s="44"/>
-      <c r="K53" s="44"/>
-      <c r="L53" s="44"/>
-      <c r="M53" s="44"/>
-      <c r="N53" s="44"/>
-      <c r="O53" s="44"/>
-      <c r="P53" s="44"/>
+      <c r="C53" s="47"/>
+      <c r="D53" s="47"/>
+      <c r="E53" s="47"/>
+      <c r="F53" s="47"/>
+      <c r="G53" s="47"/>
+      <c r="H53" s="47"/>
+      <c r="I53" s="47"/>
+      <c r="J53" s="47"/>
+      <c r="K53" s="47"/>
+      <c r="L53" s="47"/>
+      <c r="M53" s="47"/>
+      <c r="N53" s="47"/>
+      <c r="O53" s="47"/>
+      <c r="P53" s="47"/>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
         <v>30</v>
       </c>
-      <c r="B54" s="37" t="s">
+      <c r="B54" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="C54" s="37"/>
-      <c r="D54" s="37"/>
-      <c r="E54" s="37"/>
-      <c r="F54" s="37"/>
-      <c r="G54" s="37"/>
-      <c r="H54" s="37"/>
-      <c r="I54" s="37"/>
-      <c r="J54" s="37"/>
-      <c r="K54" s="37"/>
-      <c r="L54" s="37"/>
-      <c r="M54" s="37"/>
-      <c r="N54" s="37"/>
-      <c r="O54" s="37"/>
-      <c r="P54" s="37"/>
+      <c r="C54" s="40"/>
+      <c r="D54" s="40"/>
+      <c r="E54" s="40"/>
+      <c r="F54" s="40"/>
+      <c r="G54" s="40"/>
+      <c r="H54" s="40"/>
+      <c r="I54" s="40"/>
+      <c r="J54" s="40"/>
+      <c r="K54" s="40"/>
+      <c r="L54" s="40"/>
+      <c r="M54" s="40"/>
+      <c r="N54" s="40"/>
+      <c r="O54" s="40"/>
+      <c r="P54" s="40"/>
     </row>
     <row r="55" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="7">
         <v>31</v>
       </c>
-      <c r="B55" s="37" t="s">
+      <c r="B55" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="C55" s="37"/>
-      <c r="D55" s="37"/>
-      <c r="E55" s="37"/>
-      <c r="F55" s="37"/>
-      <c r="G55" s="37"/>
-      <c r="H55" s="37"/>
-      <c r="I55" s="37"/>
-      <c r="J55" s="37"/>
-      <c r="K55" s="37"/>
-      <c r="L55" s="37"/>
-      <c r="M55" s="37"/>
-      <c r="N55" s="37"/>
-      <c r="O55" s="37"/>
-      <c r="P55" s="37"/>
+      <c r="C55" s="40"/>
+      <c r="D55" s="40"/>
+      <c r="E55" s="40"/>
+      <c r="F55" s="40"/>
+      <c r="G55" s="40"/>
+      <c r="H55" s="40"/>
+      <c r="I55" s="40"/>
+      <c r="J55" s="40"/>
+      <c r="K55" s="40"/>
+      <c r="L55" s="40"/>
+      <c r="M55" s="40"/>
+      <c r="N55" s="40"/>
+      <c r="O55" s="40"/>
+      <c r="P55" s="40"/>
     </row>
     <row r="56" spans="1:16" s="26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="26">
         <v>32</v>
       </c>
-      <c r="B56" s="43" t="s">
+      <c r="B56" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="C56" s="43"/>
-      <c r="D56" s="43"/>
-      <c r="E56" s="43"/>
-      <c r="F56" s="43"/>
-      <c r="G56" s="43"/>
-      <c r="H56" s="43"/>
-      <c r="I56" s="43"/>
-      <c r="J56" s="43"/>
-      <c r="K56" s="43"/>
-      <c r="L56" s="43"/>
-      <c r="M56" s="43"/>
-      <c r="N56" s="43"/>
-      <c r="O56" s="43"/>
-      <c r="P56" s="43"/>
+      <c r="C56" s="46"/>
+      <c r="D56" s="46"/>
+      <c r="E56" s="46"/>
+      <c r="F56" s="46"/>
+      <c r="G56" s="46"/>
+      <c r="H56" s="46"/>
+      <c r="I56" s="46"/>
+      <c r="J56" s="46"/>
+      <c r="K56" s="46"/>
+      <c r="L56" s="46"/>
+      <c r="M56" s="46"/>
+      <c r="N56" s="46"/>
+      <c r="O56" s="46"/>
+      <c r="P56" s="46"/>
     </row>
     <row r="57" spans="1:16" s="26" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="28" t="s">
@@ -4016,287 +4050,287 @@
       <c r="A59" s="7">
         <v>33</v>
       </c>
-      <c r="B59" s="41" t="s">
+      <c r="B59" s="44" t="s">
         <v>62</v>
       </c>
-      <c r="C59" s="41"/>
-      <c r="D59" s="41"/>
-      <c r="E59" s="41"/>
-      <c r="F59" s="41"/>
-      <c r="G59" s="41"/>
-      <c r="H59" s="41"/>
-      <c r="I59" s="41"/>
-      <c r="J59" s="41"/>
-      <c r="K59" s="41"/>
-      <c r="L59" s="41"/>
-      <c r="M59" s="41"/>
-      <c r="N59" s="41"/>
-      <c r="O59" s="41"/>
-      <c r="P59" s="41"/>
+      <c r="C59" s="44"/>
+      <c r="D59" s="44"/>
+      <c r="E59" s="44"/>
+      <c r="F59" s="44"/>
+      <c r="G59" s="44"/>
+      <c r="H59" s="44"/>
+      <c r="I59" s="44"/>
+      <c r="J59" s="44"/>
+      <c r="K59" s="44"/>
+      <c r="L59" s="44"/>
+      <c r="M59" s="44"/>
+      <c r="N59" s="44"/>
+      <c r="O59" s="44"/>
+      <c r="P59" s="44"/>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
         <v>34</v>
       </c>
-      <c r="B60" s="40" t="s">
+      <c r="B60" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="C60" s="40"/>
-      <c r="D60" s="40"/>
-      <c r="E60" s="40"/>
-      <c r="F60" s="40"/>
-      <c r="G60" s="40"/>
-      <c r="H60" s="40"/>
-      <c r="I60" s="40"/>
-      <c r="J60" s="40"/>
-      <c r="K60" s="40"/>
-      <c r="L60" s="40"/>
-      <c r="M60" s="40"/>
-      <c r="N60" s="40"/>
-      <c r="O60" s="40"/>
-      <c r="P60" s="40"/>
+      <c r="C60" s="43"/>
+      <c r="D60" s="43"/>
+      <c r="E60" s="43"/>
+      <c r="F60" s="43"/>
+      <c r="G60" s="43"/>
+      <c r="H60" s="43"/>
+      <c r="I60" s="43"/>
+      <c r="J60" s="43"/>
+      <c r="K60" s="43"/>
+      <c r="L60" s="43"/>
+      <c r="M60" s="43"/>
+      <c r="N60" s="43"/>
+      <c r="O60" s="43"/>
+      <c r="P60" s="43"/>
     </row>
     <row r="61" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="21">
         <v>35</v>
       </c>
-      <c r="B61" s="41" t="s">
+      <c r="B61" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="C61" s="41"/>
-      <c r="D61" s="41"/>
-      <c r="E61" s="41"/>
-      <c r="F61" s="41"/>
-      <c r="G61" s="41"/>
-      <c r="H61" s="41"/>
-      <c r="I61" s="41"/>
-      <c r="J61" s="41"/>
-      <c r="K61" s="41"/>
-      <c r="L61" s="41"/>
-      <c r="M61" s="41"/>
-      <c r="N61" s="41"/>
-      <c r="O61" s="41"/>
-      <c r="P61" s="41"/>
+      <c r="C61" s="44"/>
+      <c r="D61" s="44"/>
+      <c r="E61" s="44"/>
+      <c r="F61" s="44"/>
+      <c r="G61" s="44"/>
+      <c r="H61" s="44"/>
+      <c r="I61" s="44"/>
+      <c r="J61" s="44"/>
+      <c r="K61" s="44"/>
+      <c r="L61" s="44"/>
+      <c r="M61" s="44"/>
+      <c r="N61" s="44"/>
+      <c r="O61" s="44"/>
+      <c r="P61" s="44"/>
     </row>
     <row r="62" spans="1:16" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="24">
         <v>36</v>
       </c>
-      <c r="B62" s="37" t="s">
+      <c r="B62" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="C62" s="37"/>
-      <c r="D62" s="37"/>
-      <c r="E62" s="37"/>
-      <c r="F62" s="37"/>
-      <c r="G62" s="37"/>
-      <c r="H62" s="37"/>
-      <c r="I62" s="37"/>
-      <c r="J62" s="37"/>
-      <c r="K62" s="37"/>
-      <c r="L62" s="37"/>
-      <c r="M62" s="37"/>
-      <c r="N62" s="37"/>
-      <c r="O62" s="37"/>
-      <c r="P62" s="37"/>
+      <c r="C62" s="40"/>
+      <c r="D62" s="40"/>
+      <c r="E62" s="40"/>
+      <c r="F62" s="40"/>
+      <c r="G62" s="40"/>
+      <c r="H62" s="40"/>
+      <c r="I62" s="40"/>
+      <c r="J62" s="40"/>
+      <c r="K62" s="40"/>
+      <c r="L62" s="40"/>
+      <c r="M62" s="40"/>
+      <c r="N62" s="40"/>
+      <c r="O62" s="40"/>
+      <c r="P62" s="40"/>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" s="7">
         <v>37</v>
       </c>
-      <c r="B63" s="40" t="s">
+      <c r="B63" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="C63" s="40"/>
-      <c r="D63" s="40"/>
-      <c r="E63" s="40"/>
-      <c r="F63" s="40"/>
-      <c r="G63" s="40"/>
-      <c r="H63" s="40"/>
-      <c r="I63" s="40"/>
-      <c r="J63" s="40"/>
-      <c r="K63" s="40"/>
-      <c r="L63" s="40"/>
-      <c r="M63" s="40"/>
-      <c r="N63" s="40"/>
-      <c r="O63" s="40"/>
-      <c r="P63" s="40"/>
+      <c r="C63" s="43"/>
+      <c r="D63" s="43"/>
+      <c r="E63" s="43"/>
+      <c r="F63" s="43"/>
+      <c r="G63" s="43"/>
+      <c r="H63" s="43"/>
+      <c r="I63" s="43"/>
+      <c r="J63" s="43"/>
+      <c r="K63" s="43"/>
+      <c r="L63" s="43"/>
+      <c r="M63" s="43"/>
+      <c r="N63" s="43"/>
+      <c r="O63" s="43"/>
+      <c r="P63" s="43"/>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
         <v>38</v>
       </c>
-      <c r="B64" s="40" t="s">
+      <c r="B64" s="43" t="s">
         <v>65</v>
       </c>
-      <c r="C64" s="40"/>
-      <c r="D64" s="40"/>
-      <c r="E64" s="40"/>
-      <c r="F64" s="40"/>
-      <c r="G64" s="40"/>
-      <c r="H64" s="40"/>
-      <c r="I64" s="40"/>
-      <c r="J64" s="40"/>
-      <c r="K64" s="40"/>
-      <c r="L64" s="40"/>
-      <c r="M64" s="40"/>
-      <c r="N64" s="40"/>
-      <c r="O64" s="40"/>
-      <c r="P64" s="40"/>
+      <c r="C64" s="43"/>
+      <c r="D64" s="43"/>
+      <c r="E64" s="43"/>
+      <c r="F64" s="43"/>
+      <c r="G64" s="43"/>
+      <c r="H64" s="43"/>
+      <c r="I64" s="43"/>
+      <c r="J64" s="43"/>
+      <c r="K64" s="43"/>
+      <c r="L64" s="43"/>
+      <c r="M64" s="43"/>
+      <c r="N64" s="43"/>
+      <c r="O64" s="43"/>
+      <c r="P64" s="43"/>
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65" s="7">
         <v>39</v>
       </c>
-      <c r="B65" s="38" t="s">
+      <c r="B65" s="41" t="s">
         <v>70</v>
       </c>
-      <c r="C65" s="38"/>
-      <c r="D65" s="38"/>
-      <c r="E65" s="38"/>
-      <c r="F65" s="38"/>
-      <c r="G65" s="38"/>
-      <c r="H65" s="38"/>
-      <c r="I65" s="38"/>
-      <c r="J65" s="38"/>
-      <c r="K65" s="38"/>
-      <c r="L65" s="38"/>
-      <c r="M65" s="38"/>
-      <c r="N65" s="38"/>
-      <c r="O65" s="38"/>
-      <c r="P65" s="38"/>
+      <c r="C65" s="41"/>
+      <c r="D65" s="41"/>
+      <c r="E65" s="41"/>
+      <c r="F65" s="41"/>
+      <c r="G65" s="41"/>
+      <c r="H65" s="41"/>
+      <c r="I65" s="41"/>
+      <c r="J65" s="41"/>
+      <c r="K65" s="41"/>
+      <c r="L65" s="41"/>
+      <c r="M65" s="41"/>
+      <c r="N65" s="41"/>
+      <c r="O65" s="41"/>
+      <c r="P65" s="41"/>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" s="7">
         <v>40</v>
       </c>
-      <c r="B66" s="38" t="s">
+      <c r="B66" s="41" t="s">
         <v>71</v>
       </c>
-      <c r="C66" s="38"/>
-      <c r="D66" s="38"/>
-      <c r="E66" s="38"/>
-      <c r="F66" s="38"/>
-      <c r="G66" s="38"/>
-      <c r="H66" s="38"/>
-      <c r="I66" s="38"/>
-      <c r="J66" s="38"/>
-      <c r="K66" s="38"/>
-      <c r="L66" s="38"/>
-      <c r="M66" s="38"/>
-      <c r="N66" s="38"/>
-      <c r="O66" s="38"/>
-      <c r="P66" s="38"/>
+      <c r="C66" s="41"/>
+      <c r="D66" s="41"/>
+      <c r="E66" s="41"/>
+      <c r="F66" s="41"/>
+      <c r="G66" s="41"/>
+      <c r="H66" s="41"/>
+      <c r="I66" s="41"/>
+      <c r="J66" s="41"/>
+      <c r="K66" s="41"/>
+      <c r="L66" s="41"/>
+      <c r="M66" s="41"/>
+      <c r="N66" s="41"/>
+      <c r="O66" s="41"/>
+      <c r="P66" s="41"/>
     </row>
     <row r="67" spans="1:16" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="7">
         <v>41</v>
       </c>
-      <c r="B67" s="37" t="s">
+      <c r="B67" s="40" t="s">
         <v>72</v>
       </c>
-      <c r="C67" s="37"/>
-      <c r="D67" s="37"/>
-      <c r="E67" s="37"/>
-      <c r="F67" s="37"/>
-      <c r="G67" s="37"/>
-      <c r="H67" s="37"/>
-      <c r="I67" s="37"/>
-      <c r="J67" s="37"/>
-      <c r="K67" s="37"/>
-      <c r="L67" s="37"/>
-      <c r="M67" s="37"/>
-      <c r="N67" s="37"/>
-      <c r="O67" s="37"/>
-      <c r="P67" s="37"/>
+      <c r="C67" s="40"/>
+      <c r="D67" s="40"/>
+      <c r="E67" s="40"/>
+      <c r="F67" s="40"/>
+      <c r="G67" s="40"/>
+      <c r="H67" s="40"/>
+      <c r="I67" s="40"/>
+      <c r="J67" s="40"/>
+      <c r="K67" s="40"/>
+      <c r="L67" s="40"/>
+      <c r="M67" s="40"/>
+      <c r="N67" s="40"/>
+      <c r="O67" s="40"/>
+      <c r="P67" s="40"/>
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68" s="7">
         <v>42</v>
       </c>
-      <c r="B68" s="39" t="s">
+      <c r="B68" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="C68" s="39"/>
-      <c r="D68" s="39"/>
-      <c r="E68" s="39"/>
-      <c r="F68" s="39"/>
-      <c r="G68" s="39"/>
-      <c r="H68" s="39"/>
-      <c r="I68" s="39"/>
-      <c r="J68" s="39"/>
-      <c r="K68" s="39"/>
-      <c r="L68" s="39"/>
-      <c r="M68" s="39"/>
-      <c r="N68" s="39"/>
-      <c r="O68" s="39"/>
-      <c r="P68" s="39"/>
+      <c r="C68" s="42"/>
+      <c r="D68" s="42"/>
+      <c r="E68" s="42"/>
+      <c r="F68" s="42"/>
+      <c r="G68" s="42"/>
+      <c r="H68" s="42"/>
+      <c r="I68" s="42"/>
+      <c r="J68" s="42"/>
+      <c r="K68" s="42"/>
+      <c r="L68" s="42"/>
+      <c r="M68" s="42"/>
+      <c r="N68" s="42"/>
+      <c r="O68" s="42"/>
+      <c r="P68" s="42"/>
     </row>
     <row r="69" spans="1:16" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="22">
         <v>43</v>
       </c>
-      <c r="B69" s="35" t="s">
+      <c r="B69" s="38" t="s">
         <v>67</v>
       </c>
-      <c r="C69" s="35"/>
-      <c r="D69" s="35"/>
-      <c r="E69" s="35"/>
-      <c r="F69" s="35"/>
-      <c r="G69" s="35"/>
-      <c r="H69" s="35"/>
-      <c r="I69" s="35"/>
-      <c r="J69" s="35"/>
-      <c r="K69" s="35"/>
-      <c r="L69" s="35"/>
-      <c r="M69" s="35"/>
-      <c r="N69" s="35"/>
-      <c r="O69" s="35"/>
-      <c r="P69" s="35"/>
+      <c r="C69" s="38"/>
+      <c r="D69" s="38"/>
+      <c r="E69" s="38"/>
+      <c r="F69" s="38"/>
+      <c r="G69" s="38"/>
+      <c r="H69" s="38"/>
+      <c r="I69" s="38"/>
+      <c r="J69" s="38"/>
+      <c r="K69" s="38"/>
+      <c r="L69" s="38"/>
+      <c r="M69" s="38"/>
+      <c r="N69" s="38"/>
+      <c r="O69" s="38"/>
+      <c r="P69" s="38"/>
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70" s="7">
         <v>44</v>
       </c>
-      <c r="B70" s="36" t="s">
+      <c r="B70" s="39" t="s">
         <v>68</v>
       </c>
-      <c r="C70" s="36"/>
-      <c r="D70" s="36"/>
-      <c r="E70" s="36"/>
-      <c r="F70" s="36"/>
-      <c r="G70" s="36"/>
-      <c r="H70" s="36"/>
-      <c r="I70" s="36"/>
-      <c r="J70" s="36"/>
-      <c r="K70" s="36"/>
-      <c r="L70" s="36"/>
-      <c r="M70" s="36"/>
-      <c r="N70" s="36"/>
-      <c r="O70" s="36"/>
-      <c r="P70" s="36"/>
+      <c r="C70" s="39"/>
+      <c r="D70" s="39"/>
+      <c r="E70" s="39"/>
+      <c r="F70" s="39"/>
+      <c r="G70" s="39"/>
+      <c r="H70" s="39"/>
+      <c r="I70" s="39"/>
+      <c r="J70" s="39"/>
+      <c r="K70" s="39"/>
+      <c r="L70" s="39"/>
+      <c r="M70" s="39"/>
+      <c r="N70" s="39"/>
+      <c r="O70" s="39"/>
+      <c r="P70" s="39"/>
     </row>
     <row r="71" spans="1:16" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="24">
         <v>45</v>
       </c>
-      <c r="B71" s="37" t="s">
+      <c r="B71" s="40" t="s">
         <v>69</v>
       </c>
-      <c r="C71" s="37"/>
-      <c r="D71" s="37"/>
-      <c r="E71" s="37"/>
-      <c r="F71" s="37"/>
-      <c r="G71" s="37"/>
-      <c r="H71" s="37"/>
-      <c r="I71" s="37"/>
-      <c r="J71" s="37"/>
-      <c r="K71" s="37"/>
-      <c r="L71" s="37"/>
-      <c r="M71" s="37"/>
-      <c r="N71" s="37"/>
-      <c r="O71" s="37"/>
-      <c r="P71" s="37"/>
+      <c r="C71" s="40"/>
+      <c r="D71" s="40"/>
+      <c r="E71" s="40"/>
+      <c r="F71" s="40"/>
+      <c r="G71" s="40"/>
+      <c r="H71" s="40"/>
+      <c r="I71" s="40"/>
+      <c r="J71" s="40"/>
+      <c r="K71" s="40"/>
+      <c r="L71" s="40"/>
+      <c r="M71" s="40"/>
+      <c r="N71" s="40"/>
+      <c r="O71" s="40"/>
+      <c r="P71" s="40"/>
     </row>
     <row r="91" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A91" s="7">
@@ -4346,89 +4380,89 @@
       <c r="A93" s="24">
         <v>48</v>
       </c>
-      <c r="B93" s="32" t="s">
+      <c r="B93" s="35" t="s">
         <v>82</v>
       </c>
-      <c r="C93" s="32"/>
-      <c r="D93" s="32"/>
-      <c r="E93" s="32"/>
-      <c r="F93" s="32"/>
-      <c r="G93" s="32"/>
-      <c r="H93" s="32"/>
-      <c r="I93" s="32"/>
-      <c r="J93" s="32"/>
-      <c r="K93" s="32"/>
-      <c r="L93" s="32"/>
-      <c r="M93" s="32"/>
-      <c r="N93" s="32"/>
-      <c r="O93" s="32"/>
-      <c r="P93" s="32"/>
+      <c r="C93" s="35"/>
+      <c r="D93" s="35"/>
+      <c r="E93" s="35"/>
+      <c r="F93" s="35"/>
+      <c r="G93" s="35"/>
+      <c r="H93" s="35"/>
+      <c r="I93" s="35"/>
+      <c r="J93" s="35"/>
+      <c r="K93" s="35"/>
+      <c r="L93" s="35"/>
+      <c r="M93" s="35"/>
+      <c r="N93" s="35"/>
+      <c r="O93" s="35"/>
+      <c r="P93" s="35"/>
     </row>
     <row r="94" spans="1:16" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="24">
         <v>49</v>
       </c>
-      <c r="B94" s="32" t="s">
+      <c r="B94" s="35" t="s">
         <v>77</v>
       </c>
-      <c r="C94" s="32"/>
-      <c r="D94" s="32"/>
-      <c r="E94" s="32"/>
-      <c r="F94" s="32"/>
-      <c r="G94" s="32"/>
-      <c r="H94" s="32"/>
-      <c r="I94" s="32"/>
-      <c r="J94" s="32"/>
-      <c r="K94" s="32"/>
-      <c r="L94" s="32"/>
-      <c r="M94" s="32"/>
-      <c r="N94" s="32"/>
-      <c r="O94" s="32"/>
-      <c r="P94" s="32"/>
+      <c r="C94" s="35"/>
+      <c r="D94" s="35"/>
+      <c r="E94" s="35"/>
+      <c r="F94" s="35"/>
+      <c r="G94" s="35"/>
+      <c r="H94" s="35"/>
+      <c r="I94" s="35"/>
+      <c r="J94" s="35"/>
+      <c r="K94" s="35"/>
+      <c r="L94" s="35"/>
+      <c r="M94" s="35"/>
+      <c r="N94" s="35"/>
+      <c r="O94" s="35"/>
+      <c r="P94" s="35"/>
     </row>
     <row r="95" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="25">
         <v>50</v>
       </c>
-      <c r="B95" s="33" t="s">
+      <c r="B95" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="C95" s="33"/>
-      <c r="D95" s="33"/>
-      <c r="E95" s="33"/>
-      <c r="F95" s="33"/>
-      <c r="G95" s="33"/>
-      <c r="H95" s="33"/>
-      <c r="I95" s="33"/>
-      <c r="J95" s="33"/>
-      <c r="K95" s="33"/>
-      <c r="L95" s="33"/>
-      <c r="M95" s="33"/>
-      <c r="N95" s="33"/>
-      <c r="O95" s="33"/>
-      <c r="P95" s="33"/>
+      <c r="C95" s="36"/>
+      <c r="D95" s="36"/>
+      <c r="E95" s="36"/>
+      <c r="F95" s="36"/>
+      <c r="G95" s="36"/>
+      <c r="H95" s="36"/>
+      <c r="I95" s="36"/>
+      <c r="J95" s="36"/>
+      <c r="K95" s="36"/>
+      <c r="L95" s="36"/>
+      <c r="M95" s="36"/>
+      <c r="N95" s="36"/>
+      <c r="O95" s="36"/>
+      <c r="P95" s="36"/>
     </row>
     <row r="96" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A96" s="7">
         <v>51</v>
       </c>
-      <c r="B96" s="34" t="s">
+      <c r="B96" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="C96" s="34"/>
-      <c r="D96" s="34"/>
-      <c r="E96" s="34"/>
-      <c r="F96" s="34"/>
-      <c r="G96" s="34"/>
-      <c r="H96" s="34"/>
-      <c r="I96" s="34"/>
-      <c r="J96" s="34"/>
-      <c r="K96" s="34"/>
-      <c r="L96" s="34"/>
-      <c r="M96" s="34"/>
-      <c r="N96" s="34"/>
-      <c r="O96" s="34"/>
-      <c r="P96" s="34"/>
+      <c r="C96" s="37"/>
+      <c r="D96" s="37"/>
+      <c r="E96" s="37"/>
+      <c r="F96" s="37"/>
+      <c r="G96" s="37"/>
+      <c r="H96" s="37"/>
+      <c r="I96" s="37"/>
+      <c r="J96" s="37"/>
+      <c r="K96" s="37"/>
+      <c r="L96" s="37"/>
+      <c r="M96" s="37"/>
+      <c r="N96" s="37"/>
+      <c r="O96" s="37"/>
+      <c r="P96" s="37"/>
     </row>
     <row r="97" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A97">
@@ -4438,55 +4472,19 @@
         <v>81</v>
       </c>
     </row>
-    <row r="98" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A98" s="7">
+    <row r="98" spans="1:19" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="32">
         <v>52</v>
       </c>
-      <c r="B98" s="7" t="s">
+      <c r="B98" s="32" t="s">
         <v>87</v>
       </c>
-      <c r="C98" s="7"/>
-      <c r="D98" s="7"/>
-      <c r="E98" s="7"/>
-      <c r="F98" s="7"/>
-      <c r="G98" s="7"/>
-      <c r="H98" s="7"/>
-      <c r="I98" s="7"/>
-      <c r="J98" s="7"/>
-      <c r="K98" s="7"/>
-      <c r="L98" s="7"/>
-      <c r="M98" s="7"/>
-      <c r="N98" s="7"/>
-      <c r="O98" s="7"/>
-      <c r="P98" s="7"/>
-      <c r="Q98" s="7"/>
-      <c r="R98" s="7"/>
-      <c r="S98" s="7"/>
-    </row>
-    <row r="99" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A99" s="7"/>
-      <c r="B99" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="C99" s="7"/>
-      <c r="D99" s="7"/>
-      <c r="E99" s="7"/>
-      <c r="F99" s="7"/>
-      <c r="G99" s="7"/>
-      <c r="H99" s="7"/>
-      <c r="I99" s="7"/>
-      <c r="J99" s="7"/>
-      <c r="K99" s="47" t="s">
-        <v>91</v>
-      </c>
-      <c r="L99" s="7"/>
-      <c r="M99" s="7"/>
-      <c r="N99" s="7"/>
-      <c r="O99" s="7"/>
-      <c r="P99" s="7"/>
-      <c r="Q99" s="7"/>
-      <c r="R99" s="7"/>
-      <c r="S99" s="7"/>
+    </row>
+    <row r="99" spans="1:19" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B99" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="K99" s="33"/>
     </row>
     <row r="100" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A100" s="7"/>
@@ -4870,28 +4868,117 @@
       <c r="A118" s="7">
         <v>53</v>
       </c>
-      <c r="B118" s="46" t="s">
-        <v>89</v>
-      </c>
-      <c r="C118" s="46"/>
-      <c r="D118" s="46"/>
-      <c r="E118" s="46"/>
-      <c r="F118" s="46"/>
-      <c r="G118" s="46"/>
-      <c r="H118" s="46"/>
-      <c r="I118" s="46"/>
-      <c r="J118" s="46"/>
-      <c r="K118" s="46"/>
-      <c r="L118" s="46"/>
-      <c r="M118" s="46"/>
+      <c r="B118" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="C118" s="34"/>
+      <c r="D118" s="34"/>
+      <c r="E118" s="34"/>
+      <c r="F118" s="34"/>
+      <c r="G118" s="34"/>
+      <c r="H118" s="34"/>
+      <c r="I118" s="34"/>
+      <c r="J118" s="34"/>
+      <c r="K118" s="34"/>
+      <c r="L118" s="34"/>
+      <c r="M118" s="34"/>
     </row>
     <row r="119" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>54</v>
       </c>
+      <c r="B119" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="120" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>55</v>
+      </c>
+      <c r="B120" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="121" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A121" s="32">
+        <v>56</v>
+      </c>
+      <c r="B121" s="49" t="s">
+        <v>93</v>
+      </c>
+      <c r="C121" s="49"/>
+      <c r="D121" s="49"/>
+      <c r="E121" s="49"/>
+      <c r="F121" s="49"/>
+      <c r="G121" s="49"/>
+      <c r="H121" s="49"/>
+      <c r="I121" s="49"/>
+      <c r="J121" s="49"/>
+      <c r="K121" s="49"/>
+      <c r="L121" s="49"/>
+      <c r="M121" s="49"/>
+      <c r="N121" s="49"/>
+      <c r="O121" s="49"/>
+      <c r="P121" s="49"/>
+      <c r="Q121" s="49"/>
+      <c r="R121" s="49"/>
+      <c r="S121" s="49"/>
+    </row>
+    <row r="122" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A122" s="32">
+        <v>57</v>
+      </c>
+      <c r="B122" s="49" t="s">
+        <v>94</v>
+      </c>
+      <c r="C122" s="49"/>
+      <c r="D122" s="49"/>
+      <c r="E122" s="49"/>
+      <c r="F122" s="49"/>
+      <c r="G122" s="49"/>
+      <c r="H122" s="49"/>
+      <c r="I122" s="49"/>
+      <c r="J122" s="49"/>
+      <c r="K122" s="49"/>
+      <c r="L122" s="49"/>
+      <c r="M122" s="49"/>
+      <c r="N122" s="49"/>
+      <c r="O122" s="49"/>
+      <c r="P122" s="49"/>
+      <c r="Q122" s="49"/>
+      <c r="R122" s="49"/>
+      <c r="S122" s="49"/>
+    </row>
+    <row r="123" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A123" s="32">
+        <v>58</v>
+      </c>
+      <c r="B123" s="49" t="s">
+        <v>95</v>
+      </c>
+      <c r="C123" s="49"/>
+      <c r="D123" s="49"/>
+      <c r="E123" s="49"/>
+      <c r="F123" s="49"/>
+      <c r="G123" s="49"/>
+      <c r="H123" s="49"/>
+      <c r="I123" s="49"/>
+      <c r="J123" s="49"/>
+      <c r="K123" s="49"/>
+      <c r="L123" s="49"/>
+      <c r="M123" s="49"/>
+      <c r="N123" s="49"/>
+      <c r="O123" s="49"/>
+      <c r="P123" s="49"/>
+      <c r="Q123" s="49"/>
+      <c r="R123" s="49"/>
+      <c r="S123" s="49"/>
     </row>
   </sheetData>
-  <mergeCells count="49">
+  <mergeCells count="52">
+    <mergeCell ref="B121:S121"/>
+    <mergeCell ref="B122:S122"/>
+    <mergeCell ref="B123:S123"/>
     <mergeCell ref="B13:P13"/>
     <mergeCell ref="B2:P2"/>
     <mergeCell ref="B3:P3"/>

</xml_diff>

<commit_message>
Chybí 17 a 84
</commit_message>
<xml_diff>
--- a/MDM/WorkSheet.xlsx
+++ b/MDM/WorkSheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="139">
   <si>
     <t>Úvodní schůze</t>
   </si>
@@ -508,6 +508,69 @@
   </si>
   <si>
     <t>Opraveno. Pokud nastane stav "vysoké impedance" ve stavu "nastavení proudu", musí se nastavení proudu přerušit, podobně jako 72.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pokud se opakovaně klikne myší na stejnou ikonu "Procedury" nebo "Seznam pacientů", tak dochází zbytečně k opakovanému vykreslení okna a obrazovka jakoby problikne </t>
+  </si>
+  <si>
+    <t>Administrátor může během procesu léčení vymazat pacienty, kteří se zrovna léčí a vyvolat tak neošetřenou chybu viz. obrázek:</t>
+  </si>
+  <si>
+    <t>Pokud tohoto zašedlého pacienta obsluha přesto vybere, tak se zobrazí stávající upozornění "Tento pacient je již připojen na jiný kanál"</t>
+  </si>
+  <si>
+    <t>Pokud se pro určitý kanál vybere konkrétní pacient, tak není žádoucí aby se pro jiný kanál nabízel stejný pacient , který už se léčí na jiném kanálu (pro větší přehlednost by měl být v tuto chvíli řádek s pacientem zašedlý,)</t>
+  </si>
+  <si>
+    <t>V okně "Seznam pacientů" zvětšit řádek s nabídkou ikon "První"; Předchozí"; Aktuální řádek";… stejně jako v bodu 69</t>
+  </si>
+  <si>
+    <t>V okně "Seznam pacientů" zvětšit řádky jednotlivých pacientů viz. bod 77</t>
+  </si>
+  <si>
+    <t>Je na zvážení , jestli by během léčení :</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> a) neměla být databáze úplně nepřístupná,</t>
+  </si>
+  <si>
+    <t>Preferujeme řešení dle bodu b)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> b) nebo během léčení nepůjdou mazat řádky s (konkrétními) pacienty (kteří se zrovna léčí).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2) došlo k založení nového pacienta </t>
+  </si>
+  <si>
+    <t>Záloha databáze (pacientů a uživatelů- resp. komprimace do" .enc" souboru) se musí vždy provést při následujícíh úkonech:</t>
+  </si>
+  <si>
+    <t>3) došlo k inkrementaci "Čísla procedury" pacienta</t>
+  </si>
+  <si>
+    <t>zabrání se tak strátě informací při úmyslném i nechtěném výpadku proudu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Na konci procedury (po uplynutí 30 min intervalu) je nutné výrazně snížit rychlost poklesu proudu do nuly. </t>
+  </si>
+  <si>
+    <t>do té doby, dokud nedojde k prvnímu čtení z desky generátoru</t>
+  </si>
+  <si>
+    <t>Je nutné se zaměřit se na skutečnost, že při zapnutí napájení desky generátoru je ihned aktivní informace o restartu desky</t>
+  </si>
+  <si>
+    <t>Při opakovaném postupném výběru více kanálů (pěti a více) se někdy ještě stane že se nesprávně vyhodnotí stav : "Došlo k restartu desky"</t>
+  </si>
+  <si>
+    <t>Se zvětšením řádků s výběrem pacienta viz. bod 70 je vhodné zvětšit úměřně i písmo, aby obsluha mohla přečíst lépe text (třeba i bez brýlí)</t>
+  </si>
+  <si>
+    <t>V seznamech je navíc jeden prázdný řádek</t>
+  </si>
+  <si>
+    <t>1) došlo k založení nového uživatele</t>
   </si>
 </sst>
 </file>
@@ -1161,7 +1224,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="3" applyAlignment="1">
@@ -1212,11 +1275,18 @@
     </xf>
     <xf numFmtId="0" fontId="22" fillId="46" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="22" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="46" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="22" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="5"/>
     </xf>
@@ -1226,14 +1296,14 @@
     <xf numFmtId="0" fontId="22" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="5"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="5"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="5"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="5"/>
@@ -1253,14 +1323,11 @@
     <xf numFmtId="0" fontId="22" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="5"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" xfId="6" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % – Zvýraznění1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1739,6 +1806,106 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>6803</xdr:colOff>
+      <xdr:row>255</xdr:row>
+      <xdr:rowOff>122464</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>554725</xdr:colOff>
+      <xdr:row>271</xdr:row>
+      <xdr:rowOff>138546</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Obrázek 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1DF164B-89EE-4A2D-B3BC-3A25C3B53EB1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="612939" y="49886259"/>
+          <a:ext cx="5397013" cy="3064082"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>286</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>244186</xdr:colOff>
+      <xdr:row>297</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Obrázek 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{141051D1-422D-4BA3-A12F-D667A9A6C3D7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="606136" y="55669295"/>
+          <a:ext cx="6305550" cy="2247900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2029,10 +2196,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H124"/>
+  <dimension ref="A1:H126"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="A124" sqref="A124:C124"/>
+    <sheetView showGridLines="0" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="A126" sqref="A126:C126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2070,11 +2237,11 @@
       </c>
       <c r="F2" s="4">
         <f>SUM(C:C)</f>
-        <v>535</v>
+        <v>541</v>
       </c>
       <c r="H2" s="5">
         <f>F2*300</f>
-        <v>160500</v>
+        <v>162300</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -3162,6 +3329,22 @@
       </c>
       <c r="C124">
         <v>4</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" s="1">
+        <v>43025</v>
+      </c>
+      <c r="C125">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" s="1">
+        <v>43027</v>
+      </c>
+      <c r="C126">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -3171,10 +3354,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:X254"/>
+  <dimension ref="A2:X299"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A209" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B220" sqref="B220:P220"/>
+    <sheetView tabSelected="1" topLeftCell="A272" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="M288" sqref="M288"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3190,571 +3373,571 @@
       <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="38" t="s">
         <v>88</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
-      <c r="O2" s="33"/>
-      <c r="P2" s="33"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="38"/>
+      <c r="P2" s="38"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>2</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="33"/>
-      <c r="J3" s="33"/>
-      <c r="K3" s="33"/>
-      <c r="L3" s="33"/>
-      <c r="M3" s="33"/>
-      <c r="N3" s="33"/>
-      <c r="O3" s="33"/>
-      <c r="P3" s="33"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="38"/>
+      <c r="M3" s="38"/>
+      <c r="N3" s="38"/>
+      <c r="O3" s="38"/>
+      <c r="P3" s="38"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>3</v>
       </c>
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
-      <c r="K4" s="33"/>
-      <c r="L4" s="33"/>
-      <c r="M4" s="33"/>
-      <c r="N4" s="33"/>
-      <c r="O4" s="33"/>
-      <c r="P4" s="33"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
+      <c r="K4" s="38"/>
+      <c r="L4" s="38"/>
+      <c r="M4" s="38"/>
+      <c r="N4" s="38"/>
+      <c r="O4" s="38"/>
+      <c r="P4" s="38"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>4</v>
       </c>
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
-      <c r="I5" s="33"/>
-      <c r="J5" s="33"/>
-      <c r="K5" s="33"/>
-      <c r="L5" s="33"/>
-      <c r="M5" s="33"/>
-      <c r="N5" s="33"/>
-      <c r="O5" s="33"/>
-      <c r="P5" s="33"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="38"/>
+      <c r="J5" s="38"/>
+      <c r="K5" s="38"/>
+      <c r="L5" s="38"/>
+      <c r="M5" s="38"/>
+      <c r="N5" s="38"/>
+      <c r="O5" s="38"/>
+      <c r="P5" s="38"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>5</v>
       </c>
-      <c r="B6" s="33" t="s">
+      <c r="B6" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="33"/>
-      <c r="J6" s="33"/>
-      <c r="K6" s="33"/>
-      <c r="L6" s="33"/>
-      <c r="M6" s="33"/>
-      <c r="N6" s="33"/>
-      <c r="O6" s="33"/>
-      <c r="P6" s="33"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="38"/>
+      <c r="J6" s="38"/>
+      <c r="K6" s="38"/>
+      <c r="L6" s="38"/>
+      <c r="M6" s="38"/>
+      <c r="N6" s="38"/>
+      <c r="O6" s="38"/>
+      <c r="P6" s="38"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>6</v>
       </c>
-      <c r="B7" s="33" t="s">
+      <c r="B7" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="33"/>
-      <c r="I7" s="33"/>
-      <c r="J7" s="33"/>
-      <c r="K7" s="33"/>
-      <c r="L7" s="33"/>
-      <c r="M7" s="33"/>
-      <c r="N7" s="33"/>
-      <c r="O7" s="33"/>
-      <c r="P7" s="33"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="38"/>
+      <c r="J7" s="38"/>
+      <c r="K7" s="38"/>
+      <c r="L7" s="38"/>
+      <c r="M7" s="38"/>
+      <c r="N7" s="38"/>
+      <c r="O7" s="38"/>
+      <c r="P7" s="38"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>7</v>
       </c>
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="33"/>
-      <c r="I8" s="33"/>
-      <c r="J8" s="33"/>
-      <c r="K8" s="33"/>
-      <c r="L8" s="33"/>
-      <c r="M8" s="33"/>
-      <c r="N8" s="33"/>
-      <c r="O8" s="33"/>
-      <c r="P8" s="33"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="38"/>
+      <c r="J8" s="38"/>
+      <c r="K8" s="38"/>
+      <c r="L8" s="38"/>
+      <c r="M8" s="38"/>
+      <c r="N8" s="38"/>
+      <c r="O8" s="38"/>
+      <c r="P8" s="38"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>8</v>
       </c>
-      <c r="B9" s="33" t="s">
+      <c r="B9" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="33"/>
-      <c r="I9" s="33"/>
-      <c r="J9" s="33"/>
-      <c r="K9" s="33"/>
-      <c r="L9" s="33"/>
-      <c r="M9" s="33"/>
-      <c r="N9" s="33"/>
-      <c r="O9" s="33"/>
-      <c r="P9" s="33"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="38"/>
+      <c r="K9" s="38"/>
+      <c r="L9" s="38"/>
+      <c r="M9" s="38"/>
+      <c r="N9" s="38"/>
+      <c r="O9" s="38"/>
+      <c r="P9" s="38"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>9</v>
       </c>
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="34"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="34"/>
-      <c r="J10" s="34"/>
-      <c r="K10" s="34"/>
-      <c r="L10" s="34"/>
-      <c r="M10" s="34"/>
-      <c r="N10" s="34"/>
-      <c r="O10" s="34"/>
-      <c r="P10" s="34"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="39"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="39"/>
+      <c r="K10" s="39"/>
+      <c r="L10" s="39"/>
+      <c r="M10" s="39"/>
+      <c r="N10" s="39"/>
+      <c r="O10" s="39"/>
+      <c r="P10" s="39"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>10</v>
       </c>
-      <c r="B11" s="33" t="s">
+      <c r="B11" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="33"/>
-      <c r="J11" s="33"/>
-      <c r="K11" s="33"/>
-      <c r="L11" s="33"/>
-      <c r="M11" s="33"/>
-      <c r="N11" s="33"/>
-      <c r="O11" s="33"/>
-      <c r="P11" s="33"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="38"/>
+      <c r="J11" s="38"/>
+      <c r="K11" s="38"/>
+      <c r="L11" s="38"/>
+      <c r="M11" s="38"/>
+      <c r="N11" s="38"/>
+      <c r="O11" s="38"/>
+      <c r="P11" s="38"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>11</v>
       </c>
-      <c r="B12" s="33" t="s">
+      <c r="B12" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="33"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="33"/>
-      <c r="G12" s="33"/>
-      <c r="H12" s="33"/>
-      <c r="I12" s="33"/>
-      <c r="J12" s="33"/>
-      <c r="K12" s="33"/>
-      <c r="L12" s="33"/>
-      <c r="M12" s="33"/>
-      <c r="N12" s="33"/>
-      <c r="O12" s="33"/>
-      <c r="P12" s="33"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="38"/>
+      <c r="L12" s="38"/>
+      <c r="M12" s="38"/>
+      <c r="N12" s="38"/>
+      <c r="O12" s="38"/>
+      <c r="P12" s="38"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>12</v>
       </c>
-      <c r="B13" s="33" t="s">
+      <c r="B13" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="33"/>
-      <c r="I13" s="33"/>
-      <c r="J13" s="33"/>
-      <c r="K13" s="33"/>
-      <c r="L13" s="33"/>
-      <c r="M13" s="33"/>
-      <c r="N13" s="33"/>
-      <c r="O13" s="33"/>
-      <c r="P13" s="33"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="38"/>
+      <c r="J13" s="38"/>
+      <c r="K13" s="38"/>
+      <c r="L13" s="38"/>
+      <c r="M13" s="38"/>
+      <c r="N13" s="38"/>
+      <c r="O13" s="38"/>
+      <c r="P13" s="38"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>13</v>
       </c>
-      <c r="B14" s="33" t="s">
+      <c r="B14" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="33"/>
-      <c r="D14" s="33"/>
-      <c r="E14" s="33"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="33"/>
-      <c r="H14" s="33"/>
-      <c r="I14" s="33"/>
-      <c r="J14" s="33"/>
-      <c r="K14" s="33"/>
-      <c r="L14" s="33"/>
-      <c r="M14" s="33"/>
-      <c r="N14" s="33"/>
-      <c r="O14" s="33"/>
-      <c r="P14" s="33"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
+      <c r="J14" s="38"/>
+      <c r="K14" s="38"/>
+      <c r="L14" s="38"/>
+      <c r="M14" s="38"/>
+      <c r="N14" s="38"/>
+      <c r="O14" s="38"/>
+      <c r="P14" s="38"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>14</v>
       </c>
-      <c r="B15" s="34" t="s">
+      <c r="B15" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="C15" s="34"/>
-      <c r="D15" s="34"/>
-      <c r="E15" s="34"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="34"/>
-      <c r="H15" s="34"/>
-      <c r="I15" s="34"/>
-      <c r="J15" s="34"/>
-      <c r="K15" s="34"/>
-      <c r="L15" s="34"/>
-      <c r="M15" s="34"/>
-      <c r="N15" s="34"/>
-      <c r="O15" s="34"/>
-      <c r="P15" s="34"/>
+      <c r="C15" s="39"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="39"/>
+      <c r="G15" s="39"/>
+      <c r="H15" s="39"/>
+      <c r="I15" s="39"/>
+      <c r="J15" s="39"/>
+      <c r="K15" s="39"/>
+      <c r="L15" s="39"/>
+      <c r="M15" s="39"/>
+      <c r="N15" s="39"/>
+      <c r="O15" s="39"/>
+      <c r="P15" s="39"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <v>15</v>
       </c>
-      <c r="B16" s="33" t="s">
+      <c r="B16" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="C16" s="33"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="33"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="33"/>
-      <c r="J16" s="33"/>
-      <c r="K16" s="33"/>
-      <c r="L16" s="33"/>
-      <c r="M16" s="33"/>
-      <c r="N16" s="33"/>
-      <c r="O16" s="33"/>
-      <c r="P16" s="33"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="38"/>
+      <c r="J16" s="38"/>
+      <c r="K16" s="38"/>
+      <c r="L16" s="38"/>
+      <c r="M16" s="38"/>
+      <c r="N16" s="38"/>
+      <c r="O16" s="38"/>
+      <c r="P16" s="38"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>16</v>
       </c>
-      <c r="B17" s="33" t="s">
+      <c r="B17" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="33"/>
-      <c r="D17" s="33"/>
-      <c r="E17" s="33"/>
-      <c r="F17" s="33"/>
-      <c r="G17" s="33"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="33"/>
-      <c r="J17" s="33"/>
-      <c r="K17" s="33"/>
-      <c r="L17" s="33"/>
-      <c r="M17" s="33"/>
-      <c r="N17" s="33"/>
-      <c r="O17" s="33"/>
-      <c r="P17" s="33"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="38"/>
+      <c r="I17" s="38"/>
+      <c r="J17" s="38"/>
+      <c r="K17" s="38"/>
+      <c r="L17" s="38"/>
+      <c r="M17" s="38"/>
+      <c r="N17" s="38"/>
+      <c r="O17" s="38"/>
+      <c r="P17" s="38"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18" s="7">
+      <c r="A18" s="8">
         <v>17</v>
       </c>
-      <c r="B18" s="33" t="s">
+      <c r="B18" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="C18" s="33"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="33"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
-      <c r="J18" s="33"/>
-      <c r="K18" s="33"/>
-      <c r="L18" s="33"/>
-      <c r="M18" s="33"/>
-      <c r="N18" s="33"/>
-      <c r="O18" s="33"/>
-      <c r="P18" s="33"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="41"/>
+      <c r="I18" s="41"/>
+      <c r="J18" s="41"/>
+      <c r="K18" s="41"/>
+      <c r="L18" s="41"/>
+      <c r="M18" s="41"/>
+      <c r="N18" s="41"/>
+      <c r="O18" s="41"/>
+      <c r="P18" s="41"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>18</v>
       </c>
-      <c r="B19" s="33" t="s">
+      <c r="B19" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="C19" s="33"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="33"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="33"/>
-      <c r="H19" s="33"/>
-      <c r="I19" s="33"/>
-      <c r="J19" s="33"/>
-      <c r="K19" s="33"/>
-      <c r="L19" s="33"/>
-      <c r="M19" s="33"/>
-      <c r="N19" s="33"/>
-      <c r="O19" s="33"/>
-      <c r="P19" s="33"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="38"/>
+      <c r="I19" s="38"/>
+      <c r="J19" s="38"/>
+      <c r="K19" s="38"/>
+      <c r="L19" s="38"/>
+      <c r="M19" s="38"/>
+      <c r="N19" s="38"/>
+      <c r="O19" s="38"/>
+      <c r="P19" s="38"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
         <v>19</v>
       </c>
-      <c r="B20" s="33" t="s">
+      <c r="B20" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="33"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="33"/>
-      <c r="F20" s="33"/>
-      <c r="G20" s="33"/>
-      <c r="H20" s="33"/>
-      <c r="I20" s="33"/>
-      <c r="J20" s="33"/>
-      <c r="K20" s="33"/>
-      <c r="L20" s="33"/>
-      <c r="M20" s="33"/>
-      <c r="N20" s="33"/>
-      <c r="O20" s="33"/>
-      <c r="P20" s="33"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="38"/>
+      <c r="F20" s="38"/>
+      <c r="G20" s="38"/>
+      <c r="H20" s="38"/>
+      <c r="I20" s="38"/>
+      <c r="J20" s="38"/>
+      <c r="K20" s="38"/>
+      <c r="L20" s="38"/>
+      <c r="M20" s="38"/>
+      <c r="N20" s="38"/>
+      <c r="O20" s="38"/>
+      <c r="P20" s="38"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
         <v>20</v>
       </c>
-      <c r="B21" s="33" t="s">
+      <c r="B21" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="C21" s="33"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="33"/>
-      <c r="F21" s="33"/>
-      <c r="G21" s="33"/>
-      <c r="H21" s="33"/>
-      <c r="I21" s="33"/>
-      <c r="J21" s="33"/>
-      <c r="K21" s="33"/>
-      <c r="L21" s="33"/>
-      <c r="M21" s="33"/>
-      <c r="N21" s="33"/>
-      <c r="O21" s="33"/>
-      <c r="P21" s="33"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="38"/>
+      <c r="H21" s="38"/>
+      <c r="I21" s="38"/>
+      <c r="J21" s="38"/>
+      <c r="K21" s="38"/>
+      <c r="L21" s="38"/>
+      <c r="M21" s="38"/>
+      <c r="N21" s="38"/>
+      <c r="O21" s="38"/>
+      <c r="P21" s="38"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
         <v>21</v>
       </c>
-      <c r="B22" s="33" t="s">
+      <c r="B22" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="C22" s="33"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="33"/>
-      <c r="G22" s="33"/>
-      <c r="H22" s="33"/>
-      <c r="I22" s="33"/>
-      <c r="J22" s="33"/>
-      <c r="K22" s="33"/>
-      <c r="L22" s="33"/>
-      <c r="M22" s="33"/>
-      <c r="N22" s="33"/>
-      <c r="O22" s="33"/>
-      <c r="P22" s="33"/>
+      <c r="C22" s="38"/>
+      <c r="D22" s="38"/>
+      <c r="E22" s="38"/>
+      <c r="F22" s="38"/>
+      <c r="G22" s="38"/>
+      <c r="H22" s="38"/>
+      <c r="I22" s="38"/>
+      <c r="J22" s="38"/>
+      <c r="K22" s="38"/>
+      <c r="L22" s="38"/>
+      <c r="M22" s="38"/>
+      <c r="N22" s="38"/>
+      <c r="O22" s="38"/>
+      <c r="P22" s="38"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
         <v>22</v>
       </c>
-      <c r="B23" s="33" t="s">
+      <c r="B23" s="38" t="s">
         <v>79</v>
       </c>
-      <c r="C23" s="33"/>
-      <c r="D23" s="33"/>
-      <c r="E23" s="33"/>
-      <c r="F23" s="33"/>
-      <c r="G23" s="33"/>
-      <c r="H23" s="33"/>
-      <c r="I23" s="33"/>
-      <c r="J23" s="33"/>
-      <c r="K23" s="33"/>
-      <c r="L23" s="33"/>
-      <c r="M23" s="33"/>
-      <c r="N23" s="33"/>
-      <c r="O23" s="33"/>
-      <c r="P23" s="33"/>
+      <c r="C23" s="38"/>
+      <c r="D23" s="38"/>
+      <c r="E23" s="38"/>
+      <c r="F23" s="38"/>
+      <c r="G23" s="38"/>
+      <c r="H23" s="38"/>
+      <c r="I23" s="38"/>
+      <c r="J23" s="38"/>
+      <c r="K23" s="38"/>
+      <c r="L23" s="38"/>
+      <c r="M23" s="38"/>
+      <c r="N23" s="38"/>
+      <c r="O23" s="38"/>
+      <c r="P23" s="38"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
         <v>23</v>
       </c>
-      <c r="B24" s="33" t="s">
+      <c r="B24" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="C24" s="33"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="33"/>
-      <c r="G24" s="33"/>
-      <c r="H24" s="33"/>
-      <c r="I24" s="33"/>
-      <c r="J24" s="33"/>
-      <c r="K24" s="33"/>
-      <c r="L24" s="33"/>
-      <c r="M24" s="33"/>
-      <c r="N24" s="33"/>
-      <c r="O24" s="33"/>
-      <c r="P24" s="33"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="38"/>
+      <c r="G24" s="38"/>
+      <c r="H24" s="38"/>
+      <c r="I24" s="38"/>
+      <c r="J24" s="38"/>
+      <c r="K24" s="38"/>
+      <c r="L24" s="38"/>
+      <c r="M24" s="38"/>
+      <c r="N24" s="38"/>
+      <c r="O24" s="38"/>
+      <c r="P24" s="38"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="9">
         <v>24</v>
       </c>
-      <c r="B25" s="35" t="s">
+      <c r="B25" s="40" t="s">
         <v>85</v>
       </c>
-      <c r="C25" s="35"/>
-      <c r="D25" s="35"/>
-      <c r="E25" s="35"/>
-      <c r="F25" s="35"/>
-      <c r="G25" s="35"/>
-      <c r="H25" s="35"/>
-      <c r="I25" s="35"/>
-      <c r="J25" s="35"/>
-      <c r="K25" s="35"/>
-      <c r="L25" s="35"/>
-      <c r="M25" s="35"/>
-      <c r="N25" s="35"/>
-      <c r="O25" s="35"/>
-      <c r="P25" s="35"/>
+      <c r="C25" s="40"/>
+      <c r="D25" s="40"/>
+      <c r="E25" s="40"/>
+      <c r="F25" s="40"/>
+      <c r="G25" s="40"/>
+      <c r="H25" s="40"/>
+      <c r="I25" s="40"/>
+      <c r="J25" s="40"/>
+      <c r="K25" s="40"/>
+      <c r="L25" s="40"/>
+      <c r="M25" s="40"/>
+      <c r="N25" s="40"/>
+      <c r="O25" s="40"/>
+      <c r="P25" s="40"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
         <v>25</v>
       </c>
-      <c r="B26" s="33" t="s">
+      <c r="B26" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="C26" s="33"/>
-      <c r="D26" s="33"/>
-      <c r="E26" s="33"/>
-      <c r="F26" s="33"/>
-      <c r="G26" s="33"/>
-      <c r="H26" s="33"/>
-      <c r="I26" s="33"/>
-      <c r="J26" s="33"/>
-      <c r="K26" s="33"/>
-      <c r="L26" s="33"/>
-      <c r="M26" s="33"/>
-      <c r="N26" s="33"/>
-      <c r="O26" s="33"/>
-      <c r="P26" s="33"/>
+      <c r="C26" s="38"/>
+      <c r="D26" s="38"/>
+      <c r="E26" s="38"/>
+      <c r="F26" s="38"/>
+      <c r="G26" s="38"/>
+      <c r="H26" s="38"/>
+      <c r="I26" s="38"/>
+      <c r="J26" s="38"/>
+      <c r="K26" s="38"/>
+      <c r="L26" s="38"/>
+      <c r="M26" s="38"/>
+      <c r="N26" s="38"/>
+      <c r="O26" s="38"/>
+      <c r="P26" s="38"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="8">
         <v>26</v>
       </c>
-      <c r="B27" s="38"/>
-      <c r="C27" s="38"/>
-      <c r="D27" s="38"/>
-      <c r="E27" s="38"/>
-      <c r="F27" s="38"/>
-      <c r="G27" s="38"/>
-      <c r="H27" s="38"/>
-      <c r="I27" s="38"/>
-      <c r="J27" s="38"/>
-      <c r="K27" s="38"/>
-      <c r="L27" s="38"/>
-      <c r="M27" s="38"/>
-      <c r="N27" s="38"/>
-      <c r="O27" s="38"/>
-      <c r="P27" s="38"/>
+      <c r="B27" s="41"/>
+      <c r="C27" s="41"/>
+      <c r="D27" s="41"/>
+      <c r="E27" s="41"/>
+      <c r="F27" s="41"/>
+      <c r="G27" s="41"/>
+      <c r="H27" s="41"/>
+      <c r="I27" s="41"/>
+      <c r="J27" s="41"/>
+      <c r="K27" s="41"/>
+      <c r="L27" s="41"/>
+      <c r="M27" s="41"/>
+      <c r="N27" s="41"/>
+      <c r="O27" s="41"/>
+      <c r="P27" s="41"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
@@ -4288,433 +4471,433 @@
       <c r="A52" s="8">
         <v>28</v>
       </c>
-      <c r="B52" s="38"/>
-      <c r="C52" s="38"/>
-      <c r="D52" s="38"/>
-      <c r="E52" s="38"/>
-      <c r="F52" s="38"/>
-      <c r="G52" s="38"/>
-      <c r="H52" s="38"/>
-      <c r="I52" s="38"/>
-      <c r="J52" s="38"/>
-      <c r="K52" s="38"/>
-      <c r="L52" s="38"/>
-      <c r="M52" s="38"/>
-      <c r="N52" s="38"/>
-      <c r="O52" s="38"/>
-      <c r="P52" s="38"/>
+      <c r="B52" s="41"/>
+      <c r="C52" s="41"/>
+      <c r="D52" s="41"/>
+      <c r="E52" s="41"/>
+      <c r="F52" s="41"/>
+      <c r="G52" s="41"/>
+      <c r="H52" s="41"/>
+      <c r="I52" s="41"/>
+      <c r="J52" s="41"/>
+      <c r="K52" s="41"/>
+      <c r="L52" s="41"/>
+      <c r="M52" s="41"/>
+      <c r="N52" s="41"/>
+      <c r="O52" s="41"/>
+      <c r="P52" s="41"/>
     </row>
     <row r="53" spans="1:16" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="22">
         <v>29</v>
       </c>
-      <c r="B53" s="39" t="s">
+      <c r="B53" s="44" t="s">
         <v>78</v>
       </c>
-      <c r="C53" s="39"/>
-      <c r="D53" s="39"/>
-      <c r="E53" s="39"/>
-      <c r="F53" s="39"/>
-      <c r="G53" s="39"/>
-      <c r="H53" s="39"/>
-      <c r="I53" s="39"/>
-      <c r="J53" s="39"/>
-      <c r="K53" s="39"/>
-      <c r="L53" s="39"/>
-      <c r="M53" s="39"/>
-      <c r="N53" s="39"/>
-      <c r="O53" s="39"/>
-      <c r="P53" s="39"/>
+      <c r="C53" s="44"/>
+      <c r="D53" s="44"/>
+      <c r="E53" s="44"/>
+      <c r="F53" s="44"/>
+      <c r="G53" s="44"/>
+      <c r="H53" s="44"/>
+      <c r="I53" s="44"/>
+      <c r="J53" s="44"/>
+      <c r="K53" s="44"/>
+      <c r="L53" s="44"/>
+      <c r="M53" s="44"/>
+      <c r="N53" s="44"/>
+      <c r="O53" s="44"/>
+      <c r="P53" s="44"/>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
         <v>30</v>
       </c>
-      <c r="B54" s="37" t="s">
+      <c r="B54" s="43" t="s">
         <v>82</v>
       </c>
-      <c r="C54" s="37"/>
-      <c r="D54" s="37"/>
-      <c r="E54" s="37"/>
-      <c r="F54" s="37"/>
-      <c r="G54" s="37"/>
-      <c r="H54" s="37"/>
-      <c r="I54" s="37"/>
-      <c r="J54" s="37"/>
-      <c r="K54" s="37"/>
-      <c r="L54" s="37"/>
-      <c r="M54" s="37"/>
-      <c r="N54" s="37"/>
-      <c r="O54" s="37"/>
-      <c r="P54" s="37"/>
+      <c r="C54" s="43"/>
+      <c r="D54" s="43"/>
+      <c r="E54" s="43"/>
+      <c r="F54" s="43"/>
+      <c r="G54" s="43"/>
+      <c r="H54" s="43"/>
+      <c r="I54" s="43"/>
+      <c r="J54" s="43"/>
+      <c r="K54" s="43"/>
+      <c r="L54" s="43"/>
+      <c r="M54" s="43"/>
+      <c r="N54" s="43"/>
+      <c r="O54" s="43"/>
+      <c r="P54" s="43"/>
     </row>
     <row r="55" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="7">
         <v>31</v>
       </c>
-      <c r="B55" s="37" t="s">
+      <c r="B55" s="43" t="s">
         <v>57</v>
       </c>
-      <c r="C55" s="37"/>
-      <c r="D55" s="37"/>
-      <c r="E55" s="37"/>
-      <c r="F55" s="37"/>
-      <c r="G55" s="37"/>
-      <c r="H55" s="37"/>
-      <c r="I55" s="37"/>
-      <c r="J55" s="37"/>
-      <c r="K55" s="37"/>
-      <c r="L55" s="37"/>
-      <c r="M55" s="37"/>
-      <c r="N55" s="37"/>
-      <c r="O55" s="37"/>
-      <c r="P55" s="37"/>
+      <c r="C55" s="43"/>
+      <c r="D55" s="43"/>
+      <c r="E55" s="43"/>
+      <c r="F55" s="43"/>
+      <c r="G55" s="43"/>
+      <c r="H55" s="43"/>
+      <c r="I55" s="43"/>
+      <c r="J55" s="43"/>
+      <c r="K55" s="43"/>
+      <c r="L55" s="43"/>
+      <c r="M55" s="43"/>
+      <c r="N55" s="43"/>
+      <c r="O55" s="43"/>
+      <c r="P55" s="43"/>
     </row>
     <row r="56" spans="1:16" s="23" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
         <v>32</v>
       </c>
-      <c r="B56" s="37" t="s">
+      <c r="B56" s="43" t="s">
         <v>83</v>
       </c>
-      <c r="C56" s="37"/>
-      <c r="D56" s="37"/>
-      <c r="E56" s="37"/>
-      <c r="F56" s="37"/>
-      <c r="G56" s="37"/>
-      <c r="H56" s="37"/>
-      <c r="I56" s="37"/>
-      <c r="J56" s="37"/>
-      <c r="K56" s="37"/>
-      <c r="L56" s="37"/>
-      <c r="M56" s="37"/>
-      <c r="N56" s="37"/>
-      <c r="O56" s="37"/>
-      <c r="P56" s="37"/>
+      <c r="C56" s="43"/>
+      <c r="D56" s="43"/>
+      <c r="E56" s="43"/>
+      <c r="F56" s="43"/>
+      <c r="G56" s="43"/>
+      <c r="H56" s="43"/>
+      <c r="I56" s="43"/>
+      <c r="J56" s="43"/>
+      <c r="K56" s="43"/>
+      <c r="L56" s="43"/>
+      <c r="M56" s="43"/>
+      <c r="N56" s="43"/>
+      <c r="O56" s="43"/>
+      <c r="P56" s="43"/>
     </row>
     <row r="57" spans="1:16" s="23" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="7"/>
-      <c r="B57" s="37" t="s">
+      <c r="B57" s="43" t="s">
         <v>84</v>
       </c>
-      <c r="C57" s="37"/>
-      <c r="D57" s="37"/>
-      <c r="E57" s="37"/>
-      <c r="F57" s="37"/>
-      <c r="G57" s="37"/>
-      <c r="H57" s="37"/>
-      <c r="I57" s="37"/>
-      <c r="J57" s="37"/>
-      <c r="K57" s="37"/>
-      <c r="L57" s="37"/>
-      <c r="M57" s="37"/>
-      <c r="N57" s="37"/>
-      <c r="O57" s="37"/>
-      <c r="P57" s="37"/>
+      <c r="C57" s="43"/>
+      <c r="D57" s="43"/>
+      <c r="E57" s="43"/>
+      <c r="F57" s="43"/>
+      <c r="G57" s="43"/>
+      <c r="H57" s="43"/>
+      <c r="I57" s="43"/>
+      <c r="J57" s="43"/>
+      <c r="K57" s="43"/>
+      <c r="L57" s="43"/>
+      <c r="M57" s="43"/>
+      <c r="N57" s="43"/>
+      <c r="O57" s="43"/>
+      <c r="P57" s="43"/>
     </row>
     <row r="58" spans="1:16" s="24" customFormat="1" ht="249.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="7"/>
-      <c r="B58" s="37"/>
-      <c r="C58" s="37"/>
-      <c r="D58" s="37"/>
-      <c r="E58" s="37"/>
-      <c r="F58" s="37"/>
-      <c r="G58" s="37"/>
-      <c r="H58" s="37"/>
-      <c r="I58" s="37"/>
-      <c r="J58" s="37"/>
-      <c r="K58" s="37"/>
-      <c r="L58" s="37"/>
-      <c r="M58" s="37"/>
-      <c r="N58" s="37"/>
-      <c r="O58" s="37"/>
-      <c r="P58" s="37"/>
+      <c r="B58" s="43"/>
+      <c r="C58" s="43"/>
+      <c r="D58" s="43"/>
+      <c r="E58" s="43"/>
+      <c r="F58" s="43"/>
+      <c r="G58" s="43"/>
+      <c r="H58" s="43"/>
+      <c r="I58" s="43"/>
+      <c r="J58" s="43"/>
+      <c r="K58" s="43"/>
+      <c r="L58" s="43"/>
+      <c r="M58" s="43"/>
+      <c r="N58" s="43"/>
+      <c r="O58" s="43"/>
+      <c r="P58" s="43"/>
     </row>
     <row r="59" spans="1:16" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="7">
         <v>33</v>
       </c>
-      <c r="B59" s="36" t="s">
+      <c r="B59" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="C59" s="36"/>
-      <c r="D59" s="36"/>
-      <c r="E59" s="36"/>
-      <c r="F59" s="36"/>
-      <c r="G59" s="36"/>
-      <c r="H59" s="36"/>
-      <c r="I59" s="36"/>
-      <c r="J59" s="36"/>
-      <c r="K59" s="36"/>
-      <c r="L59" s="36"/>
-      <c r="M59" s="36"/>
-      <c r="N59" s="36"/>
-      <c r="O59" s="36"/>
-      <c r="P59" s="36"/>
+      <c r="C59" s="42"/>
+      <c r="D59" s="42"/>
+      <c r="E59" s="42"/>
+      <c r="F59" s="42"/>
+      <c r="G59" s="42"/>
+      <c r="H59" s="42"/>
+      <c r="I59" s="42"/>
+      <c r="J59" s="42"/>
+      <c r="K59" s="42"/>
+      <c r="L59" s="42"/>
+      <c r="M59" s="42"/>
+      <c r="N59" s="42"/>
+      <c r="O59" s="42"/>
+      <c r="P59" s="42"/>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
         <v>34</v>
       </c>
-      <c r="B60" s="33" t="s">
+      <c r="B60" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="C60" s="33"/>
-      <c r="D60" s="33"/>
-      <c r="E60" s="33"/>
-      <c r="F60" s="33"/>
-      <c r="G60" s="33"/>
-      <c r="H60" s="33"/>
-      <c r="I60" s="33"/>
-      <c r="J60" s="33"/>
-      <c r="K60" s="33"/>
-      <c r="L60" s="33"/>
-      <c r="M60" s="33"/>
-      <c r="N60" s="33"/>
-      <c r="O60" s="33"/>
-      <c r="P60" s="33"/>
+      <c r="C60" s="38"/>
+      <c r="D60" s="38"/>
+      <c r="E60" s="38"/>
+      <c r="F60" s="38"/>
+      <c r="G60" s="38"/>
+      <c r="H60" s="38"/>
+      <c r="I60" s="38"/>
+      <c r="J60" s="38"/>
+      <c r="K60" s="38"/>
+      <c r="L60" s="38"/>
+      <c r="M60" s="38"/>
+      <c r="N60" s="38"/>
+      <c r="O60" s="38"/>
+      <c r="P60" s="38"/>
     </row>
     <row r="61" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="25">
         <v>35</v>
       </c>
-      <c r="B61" s="36" t="s">
+      <c r="B61" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="C61" s="36"/>
-      <c r="D61" s="36"/>
-      <c r="E61" s="36"/>
-      <c r="F61" s="36"/>
-      <c r="G61" s="36"/>
-      <c r="H61" s="36"/>
-      <c r="I61" s="36"/>
-      <c r="J61" s="36"/>
-      <c r="K61" s="36"/>
-      <c r="L61" s="36"/>
-      <c r="M61" s="36"/>
-      <c r="N61" s="36"/>
-      <c r="O61" s="36"/>
-      <c r="P61" s="36"/>
+      <c r="C61" s="42"/>
+      <c r="D61" s="42"/>
+      <c r="E61" s="42"/>
+      <c r="F61" s="42"/>
+      <c r="G61" s="42"/>
+      <c r="H61" s="42"/>
+      <c r="I61" s="42"/>
+      <c r="J61" s="42"/>
+      <c r="K61" s="42"/>
+      <c r="L61" s="42"/>
+      <c r="M61" s="42"/>
+      <c r="N61" s="42"/>
+      <c r="O61" s="42"/>
+      <c r="P61" s="42"/>
     </row>
     <row r="62" spans="1:16" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="26">
         <v>36</v>
       </c>
-      <c r="B62" s="37" t="s">
+      <c r="B62" s="43" t="s">
         <v>72</v>
       </c>
-      <c r="C62" s="37"/>
-      <c r="D62" s="37"/>
-      <c r="E62" s="37"/>
-      <c r="F62" s="37"/>
-      <c r="G62" s="37"/>
-      <c r="H62" s="37"/>
-      <c r="I62" s="37"/>
-      <c r="J62" s="37"/>
-      <c r="K62" s="37"/>
-      <c r="L62" s="37"/>
-      <c r="M62" s="37"/>
-      <c r="N62" s="37"/>
-      <c r="O62" s="37"/>
-      <c r="P62" s="37"/>
+      <c r="C62" s="43"/>
+      <c r="D62" s="43"/>
+      <c r="E62" s="43"/>
+      <c r="F62" s="43"/>
+      <c r="G62" s="43"/>
+      <c r="H62" s="43"/>
+      <c r="I62" s="43"/>
+      <c r="J62" s="43"/>
+      <c r="K62" s="43"/>
+      <c r="L62" s="43"/>
+      <c r="M62" s="43"/>
+      <c r="N62" s="43"/>
+      <c r="O62" s="43"/>
+      <c r="P62" s="43"/>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" s="7">
         <v>37</v>
       </c>
-      <c r="B63" s="33" t="s">
+      <c r="B63" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="C63" s="33"/>
-      <c r="D63" s="33"/>
-      <c r="E63" s="33"/>
-      <c r="F63" s="33"/>
-      <c r="G63" s="33"/>
-      <c r="H63" s="33"/>
-      <c r="I63" s="33"/>
-      <c r="J63" s="33"/>
-      <c r="K63" s="33"/>
-      <c r="L63" s="33"/>
-      <c r="M63" s="33"/>
-      <c r="N63" s="33"/>
-      <c r="O63" s="33"/>
-      <c r="P63" s="33"/>
+      <c r="C63" s="38"/>
+      <c r="D63" s="38"/>
+      <c r="E63" s="38"/>
+      <c r="F63" s="38"/>
+      <c r="G63" s="38"/>
+      <c r="H63" s="38"/>
+      <c r="I63" s="38"/>
+      <c r="J63" s="38"/>
+      <c r="K63" s="38"/>
+      <c r="L63" s="38"/>
+      <c r="M63" s="38"/>
+      <c r="N63" s="38"/>
+      <c r="O63" s="38"/>
+      <c r="P63" s="38"/>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
         <v>38</v>
       </c>
-      <c r="B64" s="33" t="s">
+      <c r="B64" s="38" t="s">
         <v>65</v>
       </c>
-      <c r="C64" s="33"/>
-      <c r="D64" s="33"/>
-      <c r="E64" s="33"/>
-      <c r="F64" s="33"/>
-      <c r="G64" s="33"/>
-      <c r="H64" s="33"/>
-      <c r="I64" s="33"/>
-      <c r="J64" s="33"/>
-      <c r="K64" s="33"/>
-      <c r="L64" s="33"/>
-      <c r="M64" s="33"/>
-      <c r="N64" s="33"/>
-      <c r="O64" s="33"/>
-      <c r="P64" s="33"/>
+      <c r="C64" s="38"/>
+      <c r="D64" s="38"/>
+      <c r="E64" s="38"/>
+      <c r="F64" s="38"/>
+      <c r="G64" s="38"/>
+      <c r="H64" s="38"/>
+      <c r="I64" s="38"/>
+      <c r="J64" s="38"/>
+      <c r="K64" s="38"/>
+      <c r="L64" s="38"/>
+      <c r="M64" s="38"/>
+      <c r="N64" s="38"/>
+      <c r="O64" s="38"/>
+      <c r="P64" s="38"/>
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65" s="7">
         <v>39</v>
       </c>
-      <c r="B65" s="43" t="s">
+      <c r="B65" s="48" t="s">
         <v>69</v>
       </c>
-      <c r="C65" s="43"/>
-      <c r="D65" s="43"/>
-      <c r="E65" s="43"/>
-      <c r="F65" s="43"/>
-      <c r="G65" s="43"/>
-      <c r="H65" s="43"/>
-      <c r="I65" s="43"/>
-      <c r="J65" s="43"/>
-      <c r="K65" s="43"/>
-      <c r="L65" s="43"/>
-      <c r="M65" s="43"/>
-      <c r="N65" s="43"/>
-      <c r="O65" s="43"/>
-      <c r="P65" s="43"/>
+      <c r="C65" s="48"/>
+      <c r="D65" s="48"/>
+      <c r="E65" s="48"/>
+      <c r="F65" s="48"/>
+      <c r="G65" s="48"/>
+      <c r="H65" s="48"/>
+      <c r="I65" s="48"/>
+      <c r="J65" s="48"/>
+      <c r="K65" s="48"/>
+      <c r="L65" s="48"/>
+      <c r="M65" s="48"/>
+      <c r="N65" s="48"/>
+      <c r="O65" s="48"/>
+      <c r="P65" s="48"/>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" s="7">
         <v>40</v>
       </c>
-      <c r="B66" s="43" t="s">
+      <c r="B66" s="48" t="s">
         <v>70</v>
       </c>
-      <c r="C66" s="43"/>
-      <c r="D66" s="43"/>
-      <c r="E66" s="43"/>
-      <c r="F66" s="43"/>
-      <c r="G66" s="43"/>
-      <c r="H66" s="43"/>
-      <c r="I66" s="43"/>
-      <c r="J66" s="43"/>
-      <c r="K66" s="43"/>
-      <c r="L66" s="43"/>
-      <c r="M66" s="43"/>
-      <c r="N66" s="43"/>
-      <c r="O66" s="43"/>
-      <c r="P66" s="43"/>
+      <c r="C66" s="48"/>
+      <c r="D66" s="48"/>
+      <c r="E66" s="48"/>
+      <c r="F66" s="48"/>
+      <c r="G66" s="48"/>
+      <c r="H66" s="48"/>
+      <c r="I66" s="48"/>
+      <c r="J66" s="48"/>
+      <c r="K66" s="48"/>
+      <c r="L66" s="48"/>
+      <c r="M66" s="48"/>
+      <c r="N66" s="48"/>
+      <c r="O66" s="48"/>
+      <c r="P66" s="48"/>
     </row>
     <row r="67" spans="1:16" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="7">
         <v>41</v>
       </c>
-      <c r="B67" s="37" t="s">
+      <c r="B67" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="C67" s="37"/>
-      <c r="D67" s="37"/>
-      <c r="E67" s="37"/>
-      <c r="F67" s="37"/>
-      <c r="G67" s="37"/>
-      <c r="H67" s="37"/>
-      <c r="I67" s="37"/>
-      <c r="J67" s="37"/>
-      <c r="K67" s="37"/>
-      <c r="L67" s="37"/>
-      <c r="M67" s="37"/>
-      <c r="N67" s="37"/>
-      <c r="O67" s="37"/>
-      <c r="P67" s="37"/>
+      <c r="C67" s="43"/>
+      <c r="D67" s="43"/>
+      <c r="E67" s="43"/>
+      <c r="F67" s="43"/>
+      <c r="G67" s="43"/>
+      <c r="H67" s="43"/>
+      <c r="I67" s="43"/>
+      <c r="J67" s="43"/>
+      <c r="K67" s="43"/>
+      <c r="L67" s="43"/>
+      <c r="M67" s="43"/>
+      <c r="N67" s="43"/>
+      <c r="O67" s="43"/>
+      <c r="P67" s="43"/>
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68" s="7">
         <v>42</v>
       </c>
-      <c r="B68" s="44" t="s">
+      <c r="B68" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="C68" s="44"/>
-      <c r="D68" s="44"/>
-      <c r="E68" s="44"/>
-      <c r="F68" s="44"/>
-      <c r="G68" s="44"/>
-      <c r="H68" s="44"/>
-      <c r="I68" s="44"/>
-      <c r="J68" s="44"/>
-      <c r="K68" s="44"/>
-      <c r="L68" s="44"/>
-      <c r="M68" s="44"/>
-      <c r="N68" s="44"/>
-      <c r="O68" s="44"/>
-      <c r="P68" s="44"/>
+      <c r="C68" s="49"/>
+      <c r="D68" s="49"/>
+      <c r="E68" s="49"/>
+      <c r="F68" s="49"/>
+      <c r="G68" s="49"/>
+      <c r="H68" s="49"/>
+      <c r="I68" s="49"/>
+      <c r="J68" s="49"/>
+      <c r="K68" s="49"/>
+      <c r="L68" s="49"/>
+      <c r="M68" s="49"/>
+      <c r="N68" s="49"/>
+      <c r="O68" s="49"/>
+      <c r="P68" s="49"/>
     </row>
     <row r="69" spans="1:16" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="27">
         <v>43</v>
       </c>
-      <c r="B69" s="40" t="s">
+      <c r="B69" s="45" t="s">
         <v>102</v>
       </c>
-      <c r="C69" s="40"/>
-      <c r="D69" s="40"/>
-      <c r="E69" s="40"/>
-      <c r="F69" s="40"/>
-      <c r="G69" s="40"/>
-      <c r="H69" s="40"/>
-      <c r="I69" s="40"/>
-      <c r="J69" s="40"/>
-      <c r="K69" s="40"/>
-      <c r="L69" s="40"/>
-      <c r="M69" s="40"/>
-      <c r="N69" s="40"/>
-      <c r="O69" s="40"/>
-      <c r="P69" s="40"/>
+      <c r="C69" s="45"/>
+      <c r="D69" s="45"/>
+      <c r="E69" s="45"/>
+      <c r="F69" s="45"/>
+      <c r="G69" s="45"/>
+      <c r="H69" s="45"/>
+      <c r="I69" s="45"/>
+      <c r="J69" s="45"/>
+      <c r="K69" s="45"/>
+      <c r="L69" s="45"/>
+      <c r="M69" s="45"/>
+      <c r="N69" s="45"/>
+      <c r="O69" s="45"/>
+      <c r="P69" s="45"/>
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70" s="7">
         <v>44</v>
       </c>
-      <c r="B70" s="41" t="s">
+      <c r="B70" s="46" t="s">
         <v>67</v>
       </c>
-      <c r="C70" s="41"/>
-      <c r="D70" s="41"/>
-      <c r="E70" s="41"/>
-      <c r="F70" s="41"/>
-      <c r="G70" s="41"/>
-      <c r="H70" s="41"/>
-      <c r="I70" s="41"/>
-      <c r="J70" s="41"/>
-      <c r="K70" s="41"/>
-      <c r="L70" s="41"/>
-      <c r="M70" s="41"/>
-      <c r="N70" s="41"/>
-      <c r="O70" s="41"/>
-      <c r="P70" s="41"/>
+      <c r="C70" s="46"/>
+      <c r="D70" s="46"/>
+      <c r="E70" s="46"/>
+      <c r="F70" s="46"/>
+      <c r="G70" s="46"/>
+      <c r="H70" s="46"/>
+      <c r="I70" s="46"/>
+      <c r="J70" s="46"/>
+      <c r="K70" s="46"/>
+      <c r="L70" s="46"/>
+      <c r="M70" s="46"/>
+      <c r="N70" s="46"/>
+      <c r="O70" s="46"/>
+      <c r="P70" s="46"/>
     </row>
     <row r="71" spans="1:16" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="26">
         <v>45</v>
       </c>
-      <c r="B71" s="37" t="s">
+      <c r="B71" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="C71" s="37"/>
-      <c r="D71" s="37"/>
-      <c r="E71" s="37"/>
-      <c r="F71" s="37"/>
-      <c r="G71" s="37"/>
-      <c r="H71" s="37"/>
-      <c r="I71" s="37"/>
-      <c r="J71" s="37"/>
-      <c r="K71" s="37"/>
-      <c r="L71" s="37"/>
-      <c r="M71" s="37"/>
-      <c r="N71" s="37"/>
-      <c r="O71" s="37"/>
-      <c r="P71" s="37"/>
+      <c r="C71" s="43"/>
+      <c r="D71" s="43"/>
+      <c r="E71" s="43"/>
+      <c r="F71" s="43"/>
+      <c r="G71" s="43"/>
+      <c r="H71" s="43"/>
+      <c r="I71" s="43"/>
+      <c r="J71" s="43"/>
+      <c r="K71" s="43"/>
+      <c r="L71" s="43"/>
+      <c r="M71" s="43"/>
+      <c r="N71" s="43"/>
+      <c r="O71" s="43"/>
+      <c r="P71" s="43"/>
     </row>
     <row r="91" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A91" s="7">
@@ -4764,156 +4947,156 @@
       <c r="A93" s="26">
         <v>48</v>
       </c>
-      <c r="B93" s="42" t="s">
+      <c r="B93" s="47" t="s">
         <v>81</v>
       </c>
-      <c r="C93" s="42"/>
-      <c r="D93" s="42"/>
-      <c r="E93" s="42"/>
-      <c r="F93" s="42"/>
-      <c r="G93" s="42"/>
-      <c r="H93" s="42"/>
-      <c r="I93" s="42"/>
-      <c r="J93" s="42"/>
-      <c r="K93" s="42"/>
-      <c r="L93" s="42"/>
-      <c r="M93" s="42"/>
-      <c r="N93" s="42"/>
-      <c r="O93" s="42"/>
-      <c r="P93" s="42"/>
+      <c r="C93" s="47"/>
+      <c r="D93" s="47"/>
+      <c r="E93" s="47"/>
+      <c r="F93" s="47"/>
+      <c r="G93" s="47"/>
+      <c r="H93" s="47"/>
+      <c r="I93" s="47"/>
+      <c r="J93" s="47"/>
+      <c r="K93" s="47"/>
+      <c r="L93" s="47"/>
+      <c r="M93" s="47"/>
+      <c r="N93" s="47"/>
+      <c r="O93" s="47"/>
+      <c r="P93" s="47"/>
     </row>
     <row r="94" spans="1:16" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="26">
         <v>49</v>
       </c>
-      <c r="B94" s="42" t="s">
+      <c r="B94" s="47" t="s">
         <v>76</v>
       </c>
-      <c r="C94" s="42"/>
-      <c r="D94" s="42"/>
-      <c r="E94" s="42"/>
-      <c r="F94" s="42"/>
-      <c r="G94" s="42"/>
-      <c r="H94" s="42"/>
-      <c r="I94" s="42"/>
-      <c r="J94" s="42"/>
-      <c r="K94" s="42"/>
-      <c r="L94" s="42"/>
-      <c r="M94" s="42"/>
-      <c r="N94" s="42"/>
-      <c r="O94" s="42"/>
-      <c r="P94" s="42"/>
+      <c r="C94" s="47"/>
+      <c r="D94" s="47"/>
+      <c r="E94" s="47"/>
+      <c r="F94" s="47"/>
+      <c r="G94" s="47"/>
+      <c r="H94" s="47"/>
+      <c r="I94" s="47"/>
+      <c r="J94" s="47"/>
+      <c r="K94" s="47"/>
+      <c r="L94" s="47"/>
+      <c r="M94" s="47"/>
+      <c r="N94" s="47"/>
+      <c r="O94" s="47"/>
+      <c r="P94" s="47"/>
     </row>
     <row r="95" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="26">
         <v>50</v>
       </c>
-      <c r="B95" s="45" t="s">
+      <c r="B95" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="C95" s="45"/>
-      <c r="D95" s="45"/>
-      <c r="E95" s="45"/>
-      <c r="F95" s="45"/>
-      <c r="G95" s="45"/>
-      <c r="H95" s="45"/>
-      <c r="I95" s="45"/>
-      <c r="J95" s="45"/>
-      <c r="K95" s="45"/>
-      <c r="L95" s="45"/>
-      <c r="M95" s="45"/>
-      <c r="N95" s="45"/>
-      <c r="O95" s="45"/>
-      <c r="P95" s="45"/>
+      <c r="C95" s="35"/>
+      <c r="D95" s="35"/>
+      <c r="E95" s="35"/>
+      <c r="F95" s="35"/>
+      <c r="G95" s="35"/>
+      <c r="H95" s="35"/>
+      <c r="I95" s="35"/>
+      <c r="J95" s="35"/>
+      <c r="K95" s="35"/>
+      <c r="L95" s="35"/>
+      <c r="M95" s="35"/>
+      <c r="N95" s="35"/>
+      <c r="O95" s="35"/>
+      <c r="P95" s="35"/>
     </row>
     <row r="96" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A96" s="7">
         <v>51</v>
       </c>
-      <c r="B96" s="45" t="s">
+      <c r="B96" s="35" t="s">
         <v>77</v>
       </c>
-      <c r="C96" s="45"/>
-      <c r="D96" s="45"/>
-      <c r="E96" s="45"/>
-      <c r="F96" s="45"/>
-      <c r="G96" s="45"/>
-      <c r="H96" s="45"/>
-      <c r="I96" s="45"/>
-      <c r="J96" s="45"/>
-      <c r="K96" s="45"/>
-      <c r="L96" s="45"/>
-      <c r="M96" s="45"/>
-      <c r="N96" s="45"/>
-      <c r="O96" s="45"/>
-      <c r="P96" s="45"/>
+      <c r="C96" s="35"/>
+      <c r="D96" s="35"/>
+      <c r="E96" s="35"/>
+      <c r="F96" s="35"/>
+      <c r="G96" s="35"/>
+      <c r="H96" s="35"/>
+      <c r="I96" s="35"/>
+      <c r="J96" s="35"/>
+      <c r="K96" s="35"/>
+      <c r="L96" s="35"/>
+      <c r="M96" s="35"/>
+      <c r="N96" s="35"/>
+      <c r="O96" s="35"/>
+      <c r="P96" s="35"/>
     </row>
     <row r="97" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A97" s="7">
         <v>52</v>
       </c>
-      <c r="B97" s="45" t="s">
+      <c r="B97" s="35" t="s">
         <v>80</v>
       </c>
-      <c r="C97" s="45"/>
-      <c r="D97" s="45"/>
-      <c r="E97" s="45"/>
-      <c r="F97" s="45"/>
-      <c r="G97" s="45"/>
-      <c r="H97" s="45"/>
-      <c r="I97" s="45"/>
-      <c r="J97" s="45"/>
-      <c r="K97" s="45"/>
-      <c r="L97" s="45"/>
-      <c r="M97" s="45"/>
-      <c r="N97" s="45"/>
-      <c r="O97" s="45"/>
-      <c r="P97" s="45"/>
+      <c r="C97" s="35"/>
+      <c r="D97" s="35"/>
+      <c r="E97" s="35"/>
+      <c r="F97" s="35"/>
+      <c r="G97" s="35"/>
+      <c r="H97" s="35"/>
+      <c r="I97" s="35"/>
+      <c r="J97" s="35"/>
+      <c r="K97" s="35"/>
+      <c r="L97" s="35"/>
+      <c r="M97" s="35"/>
+      <c r="N97" s="35"/>
+      <c r="O97" s="35"/>
+      <c r="P97" s="35"/>
     </row>
     <row r="98" spans="1:19" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="7">
         <v>53</v>
       </c>
-      <c r="B98" s="30" t="s">
+      <c r="B98" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="C98" s="30"/>
-      <c r="D98" s="30"/>
-      <c r="E98" s="30"/>
-      <c r="F98" s="30"/>
-      <c r="G98" s="30"/>
-      <c r="H98" s="30"/>
-      <c r="I98" s="30"/>
-      <c r="J98" s="30"/>
-      <c r="K98" s="30"/>
-      <c r="L98" s="30"/>
-      <c r="M98" s="30"/>
-      <c r="N98" s="30"/>
-      <c r="O98" s="30"/>
-      <c r="P98" s="30"/>
-      <c r="Q98" s="30"/>
-      <c r="R98" s="30"/>
-      <c r="S98" s="30"/>
+      <c r="C98" s="33"/>
+      <c r="D98" s="33"/>
+      <c r="E98" s="33"/>
+      <c r="F98" s="33"/>
+      <c r="G98" s="33"/>
+      <c r="H98" s="33"/>
+      <c r="I98" s="33"/>
+      <c r="J98" s="33"/>
+      <c r="K98" s="33"/>
+      <c r="L98" s="33"/>
+      <c r="M98" s="33"/>
+      <c r="N98" s="33"/>
+      <c r="O98" s="33"/>
+      <c r="P98" s="33"/>
+      <c r="Q98" s="33"/>
+      <c r="R98" s="33"/>
+      <c r="S98" s="33"/>
     </row>
     <row r="99" spans="1:19" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="7"/>
-      <c r="B99" s="45" t="s">
+      <c r="B99" s="35" t="s">
         <v>103</v>
       </c>
-      <c r="C99" s="45"/>
-      <c r="D99" s="45"/>
-      <c r="E99" s="45"/>
-      <c r="F99" s="45"/>
-      <c r="G99" s="45"/>
-      <c r="H99" s="45"/>
-      <c r="I99" s="45"/>
-      <c r="J99" s="45"/>
-      <c r="K99" s="45"/>
-      <c r="L99" s="45"/>
-      <c r="M99" s="45"/>
-      <c r="N99" s="45"/>
-      <c r="O99" s="45"/>
-      <c r="P99" s="45"/>
+      <c r="C99" s="35"/>
+      <c r="D99" s="35"/>
+      <c r="E99" s="35"/>
+      <c r="F99" s="35"/>
+      <c r="G99" s="35"/>
+      <c r="H99" s="35"/>
+      <c r="I99" s="35"/>
+      <c r="J99" s="35"/>
+      <c r="K99" s="35"/>
+      <c r="L99" s="35"/>
+      <c r="M99" s="35"/>
+      <c r="N99" s="35"/>
+      <c r="O99" s="35"/>
+      <c r="P99" s="35"/>
       <c r="Q99" s="7"/>
       <c r="R99" s="7"/>
       <c r="S99" s="7"/>
@@ -5300,176 +5483,176 @@
       <c r="A118" s="7">
         <v>54</v>
       </c>
-      <c r="B118" s="30" t="s">
+      <c r="B118" s="33" t="s">
         <v>87</v>
       </c>
-      <c r="C118" s="31"/>
-      <c r="D118" s="31"/>
-      <c r="E118" s="31"/>
-      <c r="F118" s="31"/>
-      <c r="G118" s="31"/>
-      <c r="H118" s="31"/>
-      <c r="I118" s="31"/>
-      <c r="J118" s="31"/>
-      <c r="K118" s="31"/>
-      <c r="L118" s="31"/>
-      <c r="M118" s="31"/>
-      <c r="N118" s="31"/>
-      <c r="O118" s="31"/>
-      <c r="P118" s="31"/>
-      <c r="Q118" s="31"/>
-      <c r="R118" s="31"/>
-      <c r="S118" s="31"/>
+      <c r="C118" s="37"/>
+      <c r="D118" s="37"/>
+      <c r="E118" s="37"/>
+      <c r="F118" s="37"/>
+      <c r="G118" s="37"/>
+      <c r="H118" s="37"/>
+      <c r="I118" s="37"/>
+      <c r="J118" s="37"/>
+      <c r="K118" s="37"/>
+      <c r="L118" s="37"/>
+      <c r="M118" s="37"/>
+      <c r="N118" s="37"/>
+      <c r="O118" s="37"/>
+      <c r="P118" s="37"/>
+      <c r="Q118" s="37"/>
+      <c r="R118" s="37"/>
+      <c r="S118" s="37"/>
     </row>
     <row r="119" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A119" s="7">
         <v>55</v>
       </c>
-      <c r="B119" s="30" t="s">
+      <c r="B119" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="C119" s="30"/>
-      <c r="D119" s="30"/>
-      <c r="E119" s="30"/>
-      <c r="F119" s="30"/>
-      <c r="G119" s="30"/>
-      <c r="H119" s="30"/>
-      <c r="I119" s="30"/>
-      <c r="J119" s="30"/>
-      <c r="K119" s="30"/>
-      <c r="L119" s="30"/>
-      <c r="M119" s="30"/>
-      <c r="N119" s="30"/>
-      <c r="O119" s="30"/>
-      <c r="P119" s="30"/>
-      <c r="Q119" s="30"/>
-      <c r="R119" s="30"/>
-      <c r="S119" s="30"/>
+      <c r="C119" s="33"/>
+      <c r="D119" s="33"/>
+      <c r="E119" s="33"/>
+      <c r="F119" s="33"/>
+      <c r="G119" s="33"/>
+      <c r="H119" s="33"/>
+      <c r="I119" s="33"/>
+      <c r="J119" s="33"/>
+      <c r="K119" s="33"/>
+      <c r="L119" s="33"/>
+      <c r="M119" s="33"/>
+      <c r="N119" s="33"/>
+      <c r="O119" s="33"/>
+      <c r="P119" s="33"/>
+      <c r="Q119" s="33"/>
+      <c r="R119" s="33"/>
+      <c r="S119" s="33"/>
     </row>
     <row r="120" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A120" s="7">
         <v>56</v>
       </c>
-      <c r="B120" s="30" t="s">
+      <c r="B120" s="33" t="s">
         <v>101</v>
       </c>
-      <c r="C120" s="30"/>
-      <c r="D120" s="30"/>
-      <c r="E120" s="30"/>
-      <c r="F120" s="30"/>
-      <c r="G120" s="30"/>
-      <c r="H120" s="30"/>
-      <c r="I120" s="30"/>
-      <c r="J120" s="30"/>
-      <c r="K120" s="30"/>
-      <c r="L120" s="30"/>
-      <c r="M120" s="30"/>
-      <c r="N120" s="30"/>
-      <c r="O120" s="30"/>
-      <c r="P120" s="30"/>
-      <c r="Q120" s="30"/>
-      <c r="R120" s="30"/>
-      <c r="S120" s="30"/>
+      <c r="C120" s="33"/>
+      <c r="D120" s="33"/>
+      <c r="E120" s="33"/>
+      <c r="F120" s="33"/>
+      <c r="G120" s="33"/>
+      <c r="H120" s="33"/>
+      <c r="I120" s="33"/>
+      <c r="J120" s="33"/>
+      <c r="K120" s="33"/>
+      <c r="L120" s="33"/>
+      <c r="M120" s="33"/>
+      <c r="N120" s="33"/>
+      <c r="O120" s="33"/>
+      <c r="P120" s="33"/>
+      <c r="Q120" s="33"/>
+      <c r="R120" s="33"/>
+      <c r="S120" s="33"/>
     </row>
     <row r="121" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A121" s="7">
         <v>57</v>
       </c>
-      <c r="B121" s="30" t="s">
+      <c r="B121" s="33" t="s">
         <v>90</v>
       </c>
-      <c r="C121" s="30"/>
-      <c r="D121" s="30"/>
-      <c r="E121" s="30"/>
-      <c r="F121" s="30"/>
-      <c r="G121" s="30"/>
-      <c r="H121" s="30"/>
-      <c r="I121" s="30"/>
-      <c r="J121" s="30"/>
-      <c r="K121" s="30"/>
-      <c r="L121" s="30"/>
-      <c r="M121" s="30"/>
-      <c r="N121" s="30"/>
-      <c r="O121" s="30"/>
-      <c r="P121" s="30"/>
-      <c r="Q121" s="30"/>
-      <c r="R121" s="30"/>
-      <c r="S121" s="30"/>
+      <c r="C121" s="33"/>
+      <c r="D121" s="33"/>
+      <c r="E121" s="33"/>
+      <c r="F121" s="33"/>
+      <c r="G121" s="33"/>
+      <c r="H121" s="33"/>
+      <c r="I121" s="33"/>
+      <c r="J121" s="33"/>
+      <c r="K121" s="33"/>
+      <c r="L121" s="33"/>
+      <c r="M121" s="33"/>
+      <c r="N121" s="33"/>
+      <c r="O121" s="33"/>
+      <c r="P121" s="33"/>
+      <c r="Q121" s="33"/>
+      <c r="R121" s="33"/>
+      <c r="S121" s="33"/>
     </row>
     <row r="122" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A122" s="7">
         <v>58</v>
       </c>
-      <c r="B122" s="30" t="s">
+      <c r="B122" s="33" t="s">
         <v>91</v>
       </c>
-      <c r="C122" s="30"/>
-      <c r="D122" s="30"/>
-      <c r="E122" s="30"/>
-      <c r="F122" s="30"/>
-      <c r="G122" s="30"/>
-      <c r="H122" s="30"/>
-      <c r="I122" s="30"/>
-      <c r="J122" s="30"/>
-      <c r="K122" s="30"/>
-      <c r="L122" s="30"/>
-      <c r="M122" s="30"/>
-      <c r="N122" s="30"/>
-      <c r="O122" s="30"/>
-      <c r="P122" s="30"/>
-      <c r="Q122" s="30"/>
-      <c r="R122" s="30"/>
-      <c r="S122" s="30"/>
+      <c r="C122" s="33"/>
+      <c r="D122" s="33"/>
+      <c r="E122" s="33"/>
+      <c r="F122" s="33"/>
+      <c r="G122" s="33"/>
+      <c r="H122" s="33"/>
+      <c r="I122" s="33"/>
+      <c r="J122" s="33"/>
+      <c r="K122" s="33"/>
+      <c r="L122" s="33"/>
+      <c r="M122" s="33"/>
+      <c r="N122" s="33"/>
+      <c r="O122" s="33"/>
+      <c r="P122" s="33"/>
+      <c r="Q122" s="33"/>
+      <c r="R122" s="33"/>
+      <c r="S122" s="33"/>
     </row>
     <row r="123" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A123" s="7">
         <v>59</v>
       </c>
-      <c r="B123" s="30" t="s">
+      <c r="B123" s="33" t="s">
         <v>92</v>
       </c>
-      <c r="C123" s="30"/>
-      <c r="D123" s="30"/>
-      <c r="E123" s="30"/>
-      <c r="F123" s="30"/>
-      <c r="G123" s="30"/>
-      <c r="H123" s="30"/>
-      <c r="I123" s="30"/>
-      <c r="J123" s="30"/>
-      <c r="K123" s="30"/>
-      <c r="L123" s="30"/>
-      <c r="M123" s="30"/>
-      <c r="N123" s="30"/>
-      <c r="O123" s="30"/>
-      <c r="P123" s="30"/>
-      <c r="Q123" s="30"/>
-      <c r="R123" s="30"/>
-      <c r="S123" s="30"/>
+      <c r="C123" s="33"/>
+      <c r="D123" s="33"/>
+      <c r="E123" s="33"/>
+      <c r="F123" s="33"/>
+      <c r="G123" s="33"/>
+      <c r="H123" s="33"/>
+      <c r="I123" s="33"/>
+      <c r="J123" s="33"/>
+      <c r="K123" s="33"/>
+      <c r="L123" s="33"/>
+      <c r="M123" s="33"/>
+      <c r="N123" s="33"/>
+      <c r="O123" s="33"/>
+      <c r="P123" s="33"/>
+      <c r="Q123" s="33"/>
+      <c r="R123" s="33"/>
+      <c r="S123" s="33"/>
     </row>
     <row r="124" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A124" s="7">
         <v>60</v>
       </c>
-      <c r="B124" s="30" t="s">
+      <c r="B124" s="33" t="s">
         <v>100</v>
       </c>
-      <c r="C124" s="30"/>
-      <c r="D124" s="30"/>
-      <c r="E124" s="30"/>
-      <c r="F124" s="30"/>
-      <c r="G124" s="30"/>
-      <c r="H124" s="30"/>
-      <c r="I124" s="30"/>
-      <c r="J124" s="30"/>
-      <c r="K124" s="30"/>
-      <c r="L124" s="30"/>
-      <c r="M124" s="30"/>
-      <c r="N124" s="30"/>
-      <c r="O124" s="30"/>
-      <c r="P124" s="30"/>
-      <c r="Q124" s="30"/>
-      <c r="R124" s="30"/>
-      <c r="S124" s="30"/>
+      <c r="C124" s="33"/>
+      <c r="D124" s="33"/>
+      <c r="E124" s="33"/>
+      <c r="F124" s="33"/>
+      <c r="G124" s="33"/>
+      <c r="H124" s="33"/>
+      <c r="I124" s="33"/>
+      <c r="J124" s="33"/>
+      <c r="K124" s="33"/>
+      <c r="L124" s="33"/>
+      <c r="M124" s="33"/>
+      <c r="N124" s="33"/>
+      <c r="O124" s="33"/>
+      <c r="P124" s="33"/>
+      <c r="Q124" s="33"/>
+      <c r="R124" s="33"/>
+      <c r="S124" s="33"/>
       <c r="T124" s="7"/>
       <c r="U124" s="7"/>
       <c r="V124" s="7"/>
@@ -5477,24 +5660,24 @@
     </row>
     <row r="125" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A125" s="7"/>
-      <c r="B125" s="30"/>
-      <c r="C125" s="30"/>
-      <c r="D125" s="30"/>
-      <c r="E125" s="30"/>
-      <c r="F125" s="30"/>
-      <c r="G125" s="30"/>
-      <c r="H125" s="30"/>
-      <c r="I125" s="30"/>
-      <c r="J125" s="30"/>
-      <c r="K125" s="30"/>
-      <c r="L125" s="30"/>
-      <c r="M125" s="30"/>
-      <c r="N125" s="30"/>
-      <c r="O125" s="30"/>
-      <c r="P125" s="30"/>
-      <c r="Q125" s="30"/>
-      <c r="R125" s="30"/>
-      <c r="S125" s="30"/>
+      <c r="B125" s="33"/>
+      <c r="C125" s="33"/>
+      <c r="D125" s="33"/>
+      <c r="E125" s="33"/>
+      <c r="F125" s="33"/>
+      <c r="G125" s="33"/>
+      <c r="H125" s="33"/>
+      <c r="I125" s="33"/>
+      <c r="J125" s="33"/>
+      <c r="K125" s="33"/>
+      <c r="L125" s="33"/>
+      <c r="M125" s="33"/>
+      <c r="N125" s="33"/>
+      <c r="O125" s="33"/>
+      <c r="P125" s="33"/>
+      <c r="Q125" s="33"/>
+      <c r="R125" s="33"/>
+      <c r="S125" s="33"/>
       <c r="T125" s="7"/>
       <c r="U125" s="7"/>
       <c r="V125" s="7"/>
@@ -6229,76 +6412,76 @@
       <c r="A155" s="7">
         <v>61</v>
       </c>
-      <c r="B155" s="30" t="s">
+      <c r="B155" s="33" t="s">
         <v>93</v>
       </c>
-      <c r="C155" s="30"/>
-      <c r="D155" s="30"/>
-      <c r="E155" s="30"/>
-      <c r="F155" s="30"/>
-      <c r="G155" s="30"/>
-      <c r="H155" s="30"/>
-      <c r="I155" s="30"/>
-      <c r="J155" s="30"/>
-      <c r="K155" s="30"/>
-      <c r="L155" s="30"/>
-      <c r="M155" s="30"/>
-      <c r="N155" s="30"/>
-      <c r="O155" s="30"/>
-      <c r="P155" s="30"/>
-      <c r="Q155" s="30"/>
-      <c r="R155" s="30"/>
-      <c r="S155" s="30"/>
+      <c r="C155" s="33"/>
+      <c r="D155" s="33"/>
+      <c r="E155" s="33"/>
+      <c r="F155" s="33"/>
+      <c r="G155" s="33"/>
+      <c r="H155" s="33"/>
+      <c r="I155" s="33"/>
+      <c r="J155" s="33"/>
+      <c r="K155" s="33"/>
+      <c r="L155" s="33"/>
+      <c r="M155" s="33"/>
+      <c r="N155" s="33"/>
+      <c r="O155" s="33"/>
+      <c r="P155" s="33"/>
+      <c r="Q155" s="33"/>
+      <c r="R155" s="33"/>
+      <c r="S155" s="33"/>
       <c r="T155" s="7"/>
-      <c r="U155" s="30"/>
-      <c r="V155" s="30"/>
-      <c r="W155" s="30"/>
-      <c r="X155" s="30"/>
+      <c r="U155" s="33"/>
+      <c r="V155" s="33"/>
+      <c r="W155" s="33"/>
+      <c r="X155" s="33"/>
     </row>
     <row r="156" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A156" s="7">
         <v>62</v>
       </c>
-      <c r="B156" s="30" t="s">
+      <c r="B156" s="33" t="s">
         <v>95</v>
       </c>
-      <c r="C156" s="30"/>
-      <c r="D156" s="30"/>
-      <c r="E156" s="30"/>
-      <c r="F156" s="30"/>
-      <c r="G156" s="30"/>
-      <c r="H156" s="30"/>
-      <c r="I156" s="30"/>
-      <c r="J156" s="30"/>
-      <c r="K156" s="30"/>
-      <c r="L156" s="30"/>
-      <c r="M156" s="30"/>
-      <c r="N156" s="30"/>
-      <c r="O156" s="30"/>
-      <c r="P156" s="30"/>
-      <c r="Q156" s="30"/>
-      <c r="R156" s="30"/>
-      <c r="S156" s="30"/>
+      <c r="C156" s="33"/>
+      <c r="D156" s="33"/>
+      <c r="E156" s="33"/>
+      <c r="F156" s="33"/>
+      <c r="G156" s="33"/>
+      <c r="H156" s="33"/>
+      <c r="I156" s="33"/>
+      <c r="J156" s="33"/>
+      <c r="K156" s="33"/>
+      <c r="L156" s="33"/>
+      <c r="M156" s="33"/>
+      <c r="N156" s="33"/>
+      <c r="O156" s="33"/>
+      <c r="P156" s="33"/>
+      <c r="Q156" s="33"/>
+      <c r="R156" s="33"/>
+      <c r="S156" s="33"/>
       <c r="T156" s="28"/>
-      <c r="U156" s="31"/>
-      <c r="V156" s="31"/>
-      <c r="W156" s="31"/>
+      <c r="U156" s="37"/>
+      <c r="V156" s="37"/>
+      <c r="W156" s="37"/>
     </row>
     <row r="157" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A157" s="7"/>
       <c r="B157" s="7"/>
       <c r="C157" s="7"/>
       <c r="D157" s="7"/>
-      <c r="E157" s="32" t="s">
+      <c r="E157" s="36" t="s">
         <v>97</v>
       </c>
-      <c r="F157" s="32"/>
-      <c r="G157" s="32"/>
-      <c r="H157" s="32"/>
-      <c r="I157" s="32"/>
-      <c r="J157" s="32"/>
-      <c r="K157" s="32"/>
-      <c r="L157" s="32"/>
+      <c r="F157" s="36"/>
+      <c r="G157" s="36"/>
+      <c r="H157" s="36"/>
+      <c r="I157" s="36"/>
+      <c r="J157" s="36"/>
+      <c r="K157" s="36"/>
+      <c r="L157" s="36"/>
       <c r="M157" s="7"/>
       <c r="N157" s="7"/>
       <c r="O157" s="7"/>
@@ -6312,16 +6495,16 @@
       <c r="B158" s="7"/>
       <c r="C158" s="7"/>
       <c r="D158" s="7"/>
-      <c r="E158" s="32" t="s">
+      <c r="E158" s="36" t="s">
         <v>98</v>
       </c>
-      <c r="F158" s="32"/>
-      <c r="G158" s="32"/>
-      <c r="H158" s="32"/>
-      <c r="I158" s="32"/>
-      <c r="J158" s="32"/>
-      <c r="K158" s="32"/>
-      <c r="L158" s="32"/>
+      <c r="F158" s="36"/>
+      <c r="G158" s="36"/>
+      <c r="H158" s="36"/>
+      <c r="I158" s="36"/>
+      <c r="J158" s="36"/>
+      <c r="K158" s="36"/>
+      <c r="L158" s="36"/>
       <c r="M158" s="7"/>
       <c r="N158" s="7"/>
       <c r="O158" s="7"/>
@@ -6337,26 +6520,26 @@
       <c r="A172" s="7">
         <v>63</v>
       </c>
-      <c r="B172" s="30" t="s">
+      <c r="B172" s="33" t="s">
         <v>111</v>
       </c>
-      <c r="C172" s="30"/>
-      <c r="D172" s="30"/>
-      <c r="E172" s="30"/>
-      <c r="F172" s="30"/>
-      <c r="G172" s="30"/>
-      <c r="H172" s="30"/>
-      <c r="I172" s="30"/>
-      <c r="J172" s="30"/>
-      <c r="K172" s="30"/>
-      <c r="L172" s="30"/>
-      <c r="M172" s="30"/>
-      <c r="N172" s="30"/>
-      <c r="O172" s="30"/>
-      <c r="P172" s="30"/>
-      <c r="Q172" s="30"/>
-      <c r="R172" s="30"/>
-      <c r="S172" s="30"/>
+      <c r="C172" s="33"/>
+      <c r="D172" s="33"/>
+      <c r="E172" s="33"/>
+      <c r="F172" s="33"/>
+      <c r="G172" s="33"/>
+      <c r="H172" s="33"/>
+      <c r="I172" s="33"/>
+      <c r="J172" s="33"/>
+      <c r="K172" s="33"/>
+      <c r="L172" s="33"/>
+      <c r="M172" s="33"/>
+      <c r="N172" s="33"/>
+      <c r="O172" s="33"/>
+      <c r="P172" s="33"/>
+      <c r="Q172" s="33"/>
+      <c r="R172" s="33"/>
+      <c r="S172" s="33"/>
       <c r="T172" s="28"/>
       <c r="U172" s="29"/>
     </row>
@@ -6364,26 +6547,26 @@
       <c r="A173" s="7">
         <v>64</v>
       </c>
-      <c r="B173" s="30" t="s">
+      <c r="B173" s="33" t="s">
         <v>96</v>
       </c>
-      <c r="C173" s="30"/>
-      <c r="D173" s="30"/>
-      <c r="E173" s="30"/>
-      <c r="F173" s="30"/>
-      <c r="G173" s="30"/>
-      <c r="H173" s="30"/>
-      <c r="I173" s="30"/>
-      <c r="J173" s="30"/>
-      <c r="K173" s="30"/>
-      <c r="L173" s="30"/>
-      <c r="M173" s="30"/>
-      <c r="N173" s="30"/>
-      <c r="O173" s="30"/>
-      <c r="P173" s="30"/>
-      <c r="Q173" s="30"/>
-      <c r="R173" s="30"/>
-      <c r="S173" s="30"/>
+      <c r="C173" s="33"/>
+      <c r="D173" s="33"/>
+      <c r="E173" s="33"/>
+      <c r="F173" s="33"/>
+      <c r="G173" s="33"/>
+      <c r="H173" s="33"/>
+      <c r="I173" s="33"/>
+      <c r="J173" s="33"/>
+      <c r="K173" s="33"/>
+      <c r="L173" s="33"/>
+      <c r="M173" s="33"/>
+      <c r="N173" s="33"/>
+      <c r="O173" s="33"/>
+      <c r="P173" s="33"/>
+      <c r="Q173" s="33"/>
+      <c r="R173" s="33"/>
+      <c r="S173" s="33"/>
       <c r="T173" s="28"/>
       <c r="U173" s="29"/>
     </row>
@@ -6391,51 +6574,51 @@
       <c r="A174" s="7">
         <v>65</v>
       </c>
-      <c r="B174" s="30" t="s">
+      <c r="B174" s="33" t="s">
         <v>99</v>
       </c>
-      <c r="C174" s="30"/>
-      <c r="D174" s="30"/>
-      <c r="E174" s="30"/>
-      <c r="F174" s="30"/>
-      <c r="G174" s="30"/>
-      <c r="H174" s="30"/>
-      <c r="I174" s="30"/>
-      <c r="J174" s="30"/>
-      <c r="K174" s="30"/>
-      <c r="L174" s="30"/>
-      <c r="M174" s="30"/>
-      <c r="N174" s="30"/>
-      <c r="O174" s="30"/>
-      <c r="P174" s="30"/>
-      <c r="Q174" s="30"/>
-      <c r="R174" s="30"/>
-      <c r="S174" s="30"/>
+      <c r="C174" s="33"/>
+      <c r="D174" s="33"/>
+      <c r="E174" s="33"/>
+      <c r="F174" s="33"/>
+      <c r="G174" s="33"/>
+      <c r="H174" s="33"/>
+      <c r="I174" s="33"/>
+      <c r="J174" s="33"/>
+      <c r="K174" s="33"/>
+      <c r="L174" s="33"/>
+      <c r="M174" s="33"/>
+      <c r="N174" s="33"/>
+      <c r="O174" s="33"/>
+      <c r="P174" s="33"/>
+      <c r="Q174" s="33"/>
+      <c r="R174" s="33"/>
+      <c r="S174" s="33"/>
     </row>
     <row r="175" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A175" s="7">
         <v>66</v>
       </c>
-      <c r="B175" s="30" t="s">
+      <c r="B175" s="33" t="s">
         <v>104</v>
       </c>
-      <c r="C175" s="30"/>
-      <c r="D175" s="30"/>
-      <c r="E175" s="30"/>
-      <c r="F175" s="30"/>
-      <c r="G175" s="30"/>
-      <c r="H175" s="30"/>
-      <c r="I175" s="30"/>
-      <c r="J175" s="30"/>
-      <c r="K175" s="30"/>
-      <c r="L175" s="30"/>
-      <c r="M175" s="30"/>
-      <c r="N175" s="30"/>
-      <c r="O175" s="30"/>
-      <c r="P175" s="30"/>
-      <c r="Q175" s="30"/>
-      <c r="R175" s="30"/>
-      <c r="S175" s="30"/>
+      <c r="C175" s="33"/>
+      <c r="D175" s="33"/>
+      <c r="E175" s="33"/>
+      <c r="F175" s="33"/>
+      <c r="G175" s="33"/>
+      <c r="H175" s="33"/>
+      <c r="I175" s="33"/>
+      <c r="J175" s="33"/>
+      <c r="K175" s="33"/>
+      <c r="L175" s="33"/>
+      <c r="M175" s="33"/>
+      <c r="N175" s="33"/>
+      <c r="O175" s="33"/>
+      <c r="P175" s="33"/>
+      <c r="Q175" s="33"/>
+      <c r="R175" s="33"/>
+      <c r="S175" s="33"/>
     </row>
     <row r="176" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A176" s="7"/>
@@ -6609,291 +6792,693 @@
       <c r="A184" s="7">
         <v>67</v>
       </c>
-      <c r="B184" s="30" t="s">
+      <c r="B184" s="33" t="s">
         <v>105</v>
       </c>
-      <c r="C184" s="30"/>
-      <c r="D184" s="30"/>
-      <c r="E184" s="30"/>
-      <c r="F184" s="30"/>
-      <c r="G184" s="30"/>
-      <c r="H184" s="30"/>
-      <c r="I184" s="30"/>
-      <c r="J184" s="30"/>
-      <c r="K184" s="30"/>
-      <c r="L184" s="30"/>
-      <c r="M184" s="30"/>
-      <c r="N184" s="30"/>
-      <c r="O184" s="30"/>
-      <c r="P184" s="30"/>
-      <c r="Q184" s="30"/>
-      <c r="R184" s="30"/>
-      <c r="S184" s="30"/>
+      <c r="C184" s="33"/>
+      <c r="D184" s="33"/>
+      <c r="E184" s="33"/>
+      <c r="F184" s="33"/>
+      <c r="G184" s="33"/>
+      <c r="H184" s="33"/>
+      <c r="I184" s="33"/>
+      <c r="J184" s="33"/>
+      <c r="K184" s="33"/>
+      <c r="L184" s="33"/>
+      <c r="M184" s="33"/>
+      <c r="N184" s="33"/>
+      <c r="O184" s="33"/>
+      <c r="P184" s="33"/>
+      <c r="Q184" s="33"/>
+      <c r="R184" s="33"/>
+      <c r="S184" s="33"/>
     </row>
     <row r="185" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="B185" s="30" t="s">
+      <c r="B185" s="33" t="s">
         <v>106</v>
       </c>
-      <c r="C185" s="30"/>
-      <c r="D185" s="30"/>
-      <c r="E185" s="30"/>
-      <c r="F185" s="30"/>
-      <c r="G185" s="30"/>
-      <c r="H185" s="30"/>
-      <c r="I185" s="30"/>
-      <c r="J185" s="30"/>
-      <c r="K185" s="30"/>
-      <c r="L185" s="30"/>
-      <c r="M185" s="30"/>
-      <c r="N185" s="30"/>
-      <c r="O185" s="30"/>
-      <c r="P185" s="30"/>
-      <c r="Q185" s="30"/>
-      <c r="R185" s="30"/>
-      <c r="S185" s="30"/>
+      <c r="C185" s="33"/>
+      <c r="D185" s="33"/>
+      <c r="E185" s="33"/>
+      <c r="F185" s="33"/>
+      <c r="G185" s="33"/>
+      <c r="H185" s="33"/>
+      <c r="I185" s="33"/>
+      <c r="J185" s="33"/>
+      <c r="K185" s="33"/>
+      <c r="L185" s="33"/>
+      <c r="M185" s="33"/>
+      <c r="N185" s="33"/>
+      <c r="O185" s="33"/>
+      <c r="P185" s="33"/>
+      <c r="Q185" s="33"/>
+      <c r="R185" s="33"/>
+      <c r="S185" s="33"/>
     </row>
     <row r="186" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A186" s="7">
         <v>68</v>
       </c>
-      <c r="B186" s="30" t="s">
+      <c r="B186" s="33" t="s">
         <v>110</v>
       </c>
-      <c r="C186" s="30"/>
-      <c r="D186" s="30"/>
-      <c r="E186" s="30"/>
-      <c r="F186" s="30"/>
-      <c r="G186" s="30"/>
-      <c r="H186" s="30"/>
-      <c r="I186" s="30"/>
-      <c r="J186" s="30"/>
-      <c r="K186" s="30"/>
-      <c r="L186" s="30"/>
-      <c r="M186" s="30"/>
-      <c r="N186" s="30"/>
-      <c r="O186" s="30"/>
-      <c r="P186" s="30"/>
-      <c r="Q186" s="30"/>
-      <c r="R186" s="30"/>
-      <c r="S186" s="30"/>
+      <c r="C186" s="33"/>
+      <c r="D186" s="33"/>
+      <c r="E186" s="33"/>
+      <c r="F186" s="33"/>
+      <c r="G186" s="33"/>
+      <c r="H186" s="33"/>
+      <c r="I186" s="33"/>
+      <c r="J186" s="33"/>
+      <c r="K186" s="33"/>
+      <c r="L186" s="33"/>
+      <c r="M186" s="33"/>
+      <c r="N186" s="33"/>
+      <c r="O186" s="33"/>
+      <c r="P186" s="33"/>
+      <c r="Q186" s="33"/>
+      <c r="R186" s="33"/>
+      <c r="S186" s="33"/>
     </row>
     <row r="187" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A187" s="7">
         <v>69</v>
       </c>
-      <c r="B187" s="30" t="s">
+      <c r="B187" s="33" t="s">
         <v>108</v>
       </c>
-      <c r="C187" s="30"/>
-      <c r="D187" s="30"/>
-      <c r="E187" s="30"/>
-      <c r="F187" s="30"/>
-      <c r="G187" s="30"/>
-      <c r="H187" s="30"/>
-      <c r="I187" s="30"/>
-      <c r="J187" s="30"/>
-      <c r="K187" s="30"/>
-      <c r="L187" s="30"/>
-      <c r="M187" s="30"/>
-      <c r="N187" s="30"/>
-      <c r="O187" s="30"/>
-      <c r="P187" s="30"/>
-      <c r="Q187" s="30"/>
-      <c r="R187" s="30"/>
-      <c r="S187" s="30"/>
+      <c r="C187" s="33"/>
+      <c r="D187" s="33"/>
+      <c r="E187" s="33"/>
+      <c r="F187" s="33"/>
+      <c r="G187" s="33"/>
+      <c r="H187" s="33"/>
+      <c r="I187" s="33"/>
+      <c r="J187" s="33"/>
+      <c r="K187" s="33"/>
+      <c r="L187" s="33"/>
+      <c r="M187" s="33"/>
+      <c r="N187" s="33"/>
+      <c r="O187" s="33"/>
+      <c r="P187" s="33"/>
+      <c r="Q187" s="33"/>
+      <c r="R187" s="33"/>
+      <c r="S187" s="33"/>
     </row>
     <row r="188" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A188" s="7">
         <v>70</v>
       </c>
-      <c r="B188" s="30" t="s">
+      <c r="B188" s="33" t="s">
         <v>107</v>
       </c>
-      <c r="C188" s="30"/>
-      <c r="D188" s="30"/>
-      <c r="E188" s="30"/>
-      <c r="F188" s="30"/>
-      <c r="G188" s="30"/>
-      <c r="H188" s="30"/>
-      <c r="I188" s="30"/>
-      <c r="J188" s="30"/>
-      <c r="K188" s="30"/>
-      <c r="L188" s="30"/>
-      <c r="M188" s="30"/>
-      <c r="N188" s="30"/>
-      <c r="O188" s="30"/>
-      <c r="P188" s="30"/>
-      <c r="Q188" s="30"/>
-      <c r="R188" s="30"/>
-      <c r="S188" s="30"/>
+      <c r="C188" s="33"/>
+      <c r="D188" s="33"/>
+      <c r="E188" s="33"/>
+      <c r="F188" s="33"/>
+      <c r="G188" s="33"/>
+      <c r="H188" s="33"/>
+      <c r="I188" s="33"/>
+      <c r="J188" s="33"/>
+      <c r="K188" s="33"/>
+      <c r="L188" s="33"/>
+      <c r="M188" s="33"/>
+      <c r="N188" s="33"/>
+      <c r="O188" s="33"/>
+      <c r="P188" s="33"/>
+      <c r="Q188" s="33"/>
+      <c r="R188" s="33"/>
+      <c r="S188" s="33"/>
     </row>
     <row r="189" spans="1:24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A189" s="7">
         <v>71</v>
       </c>
-      <c r="B189" s="30" t="s">
+      <c r="B189" s="33" t="s">
         <v>109</v>
       </c>
-      <c r="C189" s="30"/>
-      <c r="D189" s="30"/>
-      <c r="E189" s="30"/>
-      <c r="F189" s="30"/>
-      <c r="G189" s="30"/>
-      <c r="H189" s="30"/>
-      <c r="I189" s="30"/>
-      <c r="J189" s="30"/>
-      <c r="K189" s="30"/>
-      <c r="L189" s="30"/>
-      <c r="M189" s="30"/>
-      <c r="N189" s="30"/>
-      <c r="O189" s="30"/>
-      <c r="P189" s="30"/>
-      <c r="Q189" s="30"/>
-      <c r="R189" s="30"/>
-      <c r="S189" s="30"/>
+      <c r="C189" s="33"/>
+      <c r="D189" s="33"/>
+      <c r="E189" s="33"/>
+      <c r="F189" s="33"/>
+      <c r="G189" s="33"/>
+      <c r="H189" s="33"/>
+      <c r="I189" s="33"/>
+      <c r="J189" s="33"/>
+      <c r="K189" s="33"/>
+      <c r="L189" s="33"/>
+      <c r="M189" s="33"/>
+      <c r="N189" s="33"/>
+      <c r="O189" s="33"/>
+      <c r="P189" s="33"/>
+      <c r="Q189" s="33"/>
+      <c r="R189" s="33"/>
+      <c r="S189" s="33"/>
     </row>
     <row r="190" spans="1:24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A190" s="46">
+      <c r="A190" s="30">
         <v>72</v>
       </c>
-      <c r="B190" s="47" t="s">
+      <c r="B190" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="C190" s="47"/>
-      <c r="D190" s="47"/>
-      <c r="E190" s="47"/>
-      <c r="F190" s="47"/>
-      <c r="G190" s="47"/>
-      <c r="H190" s="47"/>
-      <c r="I190" s="47"/>
-      <c r="J190" s="47"/>
-      <c r="K190" s="47"/>
-      <c r="L190" s="47"/>
-      <c r="M190" s="47"/>
-      <c r="N190" s="47"/>
-      <c r="O190" s="47"/>
-      <c r="P190" s="47"/>
-      <c r="Q190" s="47"/>
-      <c r="R190" s="47"/>
-      <c r="S190" s="47"/>
-      <c r="T190" s="47"/>
-      <c r="U190" s="47"/>
-      <c r="V190" s="47"/>
-      <c r="W190" s="47"/>
-      <c r="X190" s="47"/>
-    </row>
-    <row r="199" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L199" s="8" t="s">
+      <c r="C190" s="50"/>
+      <c r="D190" s="50"/>
+      <c r="E190" s="50"/>
+      <c r="F190" s="50"/>
+      <c r="G190" s="50"/>
+      <c r="H190" s="50"/>
+      <c r="I190" s="50"/>
+      <c r="J190" s="50"/>
+      <c r="K190" s="50"/>
+      <c r="L190" s="50"/>
+      <c r="M190" s="50"/>
+      <c r="N190" s="50"/>
+      <c r="O190" s="50"/>
+      <c r="P190" s="50"/>
+      <c r="Q190" s="50"/>
+      <c r="R190" s="50"/>
+      <c r="S190" s="50"/>
+      <c r="T190" s="50"/>
+      <c r="U190" s="50"/>
+      <c r="V190" s="50"/>
+      <c r="W190" s="50"/>
+      <c r="X190" s="50"/>
+    </row>
+    <row r="199" spans="12:19" x14ac:dyDescent="0.25">
+      <c r="L199" s="33" t="s">
         <v>113</v>
       </c>
+      <c r="M199" s="33"/>
+      <c r="N199" s="33"/>
+      <c r="O199" s="33"/>
+      <c r="P199" s="33"/>
+      <c r="Q199" s="33"/>
+      <c r="R199" s="33"/>
+      <c r="S199" s="33"/>
     </row>
     <row r="219" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A219" s="7">
         <v>73</v>
       </c>
-      <c r="B219" s="30" t="s">
+      <c r="B219" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="C219" s="30"/>
-      <c r="D219" s="30"/>
-      <c r="E219" s="30"/>
-      <c r="F219" s="30"/>
-      <c r="G219" s="30"/>
-      <c r="H219" s="30"/>
-      <c r="I219" s="30"/>
-      <c r="J219" s="30"/>
-      <c r="K219" s="30"/>
-      <c r="L219" s="30"/>
-      <c r="M219" s="30"/>
-      <c r="N219" s="30"/>
-      <c r="O219" s="30"/>
-      <c r="P219" s="30"/>
+      <c r="C219" s="33"/>
+      <c r="D219" s="33"/>
+      <c r="E219" s="33"/>
+      <c r="F219" s="33"/>
+      <c r="G219" s="33"/>
+      <c r="H219" s="33"/>
+      <c r="I219" s="33"/>
+      <c r="J219" s="33"/>
+      <c r="K219" s="33"/>
+      <c r="L219" s="33"/>
+      <c r="M219" s="33"/>
+      <c r="N219" s="33"/>
+      <c r="O219" s="33"/>
+      <c r="P219" s="33"/>
     </row>
     <row r="220" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B220" s="48" t="s">
+      <c r="B220" s="32" t="s">
         <v>117</v>
       </c>
-      <c r="C220" s="30"/>
-      <c r="D220" s="30"/>
-      <c r="E220" s="30"/>
-      <c r="F220" s="30"/>
-      <c r="G220" s="30"/>
-      <c r="H220" s="30"/>
-      <c r="I220" s="30"/>
-      <c r="J220" s="30"/>
-      <c r="K220" s="30"/>
-      <c r="L220" s="30"/>
-      <c r="M220" s="30"/>
-      <c r="N220" s="30"/>
-      <c r="O220" s="30"/>
-      <c r="P220" s="30"/>
+      <c r="C220" s="33"/>
+      <c r="D220" s="33"/>
+      <c r="E220" s="33"/>
+      <c r="F220" s="33"/>
+      <c r="G220" s="33"/>
+      <c r="H220" s="33"/>
+      <c r="I220" s="33"/>
+      <c r="J220" s="33"/>
+      <c r="K220" s="33"/>
+      <c r="L220" s="33"/>
+      <c r="M220" s="33"/>
+      <c r="N220" s="33"/>
+      <c r="O220" s="33"/>
+      <c r="P220" s="33"/>
     </row>
     <row r="250" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="T250" s="7"/>
-      <c r="U250" s="30"/>
-      <c r="V250" s="30"/>
-      <c r="W250" s="30"/>
-      <c r="X250" s="30"/>
+      <c r="T250" s="28"/>
+      <c r="U250" s="34"/>
+      <c r="V250" s="34"/>
+      <c r="W250" s="34"/>
+      <c r="X250" s="34"/>
     </row>
     <row r="251" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="T251" s="7"/>
-      <c r="U251" s="30"/>
-      <c r="V251" s="30"/>
-      <c r="W251" s="30"/>
-      <c r="X251" s="30"/>
+      <c r="T251" s="28"/>
+      <c r="U251" s="34"/>
+      <c r="V251" s="34"/>
+      <c r="W251" s="34"/>
+      <c r="X251" s="34"/>
     </row>
     <row r="253" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A253" s="7">
         <v>74</v>
       </c>
-      <c r="B253" s="30" t="s">
+      <c r="B253" s="33" t="s">
         <v>115</v>
       </c>
-      <c r="C253" s="30"/>
-      <c r="D253" s="30"/>
-      <c r="E253" s="30"/>
-      <c r="F253" s="30"/>
-      <c r="G253" s="30"/>
-      <c r="H253" s="30"/>
-      <c r="I253" s="30"/>
-      <c r="J253" s="30"/>
-      <c r="K253" s="30"/>
-      <c r="L253" s="30"/>
-      <c r="M253" s="30"/>
-      <c r="N253" s="30"/>
-      <c r="O253" s="30"/>
-      <c r="P253" s="30"/>
-      <c r="Q253" s="30"/>
-      <c r="R253" s="30"/>
-      <c r="S253" s="30"/>
+      <c r="C253" s="33"/>
+      <c r="D253" s="33"/>
+      <c r="E253" s="33"/>
+      <c r="F253" s="33"/>
+      <c r="G253" s="33"/>
+      <c r="H253" s="33"/>
+      <c r="I253" s="33"/>
+      <c r="J253" s="33"/>
+      <c r="K253" s="33"/>
+      <c r="L253" s="33"/>
+      <c r="M253" s="33"/>
+      <c r="N253" s="33"/>
+      <c r="O253" s="33"/>
+      <c r="P253" s="33"/>
+      <c r="Q253" s="33"/>
+      <c r="R253" s="33"/>
+      <c r="S253" s="33"/>
     </row>
     <row r="254" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A254" s="7">
         <v>75</v>
       </c>
-      <c r="B254" s="30" t="s">
+      <c r="B254" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="C254" s="30"/>
-      <c r="D254" s="30"/>
-      <c r="E254" s="30"/>
-      <c r="F254" s="30"/>
-      <c r="G254" s="30"/>
-      <c r="H254" s="30"/>
-      <c r="I254" s="30"/>
-      <c r="J254" s="30"/>
-      <c r="K254" s="30"/>
-      <c r="L254" s="30"/>
-      <c r="M254" s="30"/>
-      <c r="N254" s="30"/>
-      <c r="O254" s="30"/>
-      <c r="P254" s="30"/>
-      <c r="Q254" s="30"/>
-      <c r="R254" s="30"/>
-      <c r="S254" s="30"/>
+      <c r="C254" s="33"/>
+      <c r="D254" s="33"/>
+      <c r="E254" s="33"/>
+      <c r="F254" s="33"/>
+      <c r="G254" s="33"/>
+      <c r="H254" s="33"/>
+      <c r="I254" s="33"/>
+      <c r="J254" s="33"/>
+      <c r="K254" s="33"/>
+      <c r="L254" s="33"/>
+      <c r="M254" s="33"/>
+      <c r="N254" s="33"/>
+      <c r="O254" s="33"/>
+      <c r="P254" s="33"/>
+      <c r="Q254" s="33"/>
+      <c r="R254" s="33"/>
+      <c r="S254" s="33"/>
+    </row>
+    <row r="255" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A255" s="7">
+        <v>76</v>
+      </c>
+      <c r="B255" s="33" t="s">
+        <v>119</v>
+      </c>
+      <c r="C255" s="33"/>
+      <c r="D255" s="33"/>
+      <c r="E255" s="33"/>
+      <c r="F255" s="33"/>
+      <c r="G255" s="33"/>
+      <c r="H255" s="33"/>
+      <c r="I255" s="33"/>
+      <c r="J255" s="33"/>
+      <c r="K255" s="33"/>
+      <c r="L255" s="33"/>
+      <c r="M255" s="33"/>
+      <c r="N255" s="33"/>
+      <c r="O255" s="33"/>
+      <c r="P255" s="33"/>
+      <c r="Q255" s="33"/>
+      <c r="R255" s="33"/>
+      <c r="S255" s="33"/>
+    </row>
+    <row r="257" spans="11:18" x14ac:dyDescent="0.25">
+      <c r="K257" s="51" t="s">
+        <v>124</v>
+      </c>
+      <c r="L257" s="7"/>
+      <c r="M257" s="7"/>
+      <c r="N257" s="7"/>
+      <c r="O257" s="7"/>
+      <c r="P257" s="7"/>
+      <c r="Q257" s="7"/>
+      <c r="R257" s="7"/>
+    </row>
+    <row r="258" spans="11:18" x14ac:dyDescent="0.25">
+      <c r="K258" s="7"/>
+      <c r="L258" s="7"/>
+      <c r="M258" s="7"/>
+      <c r="N258" s="7"/>
+      <c r="O258" s="7"/>
+      <c r="P258" s="7"/>
+      <c r="Q258" s="7"/>
+      <c r="R258" s="7"/>
+    </row>
+    <row r="259" spans="11:18" x14ac:dyDescent="0.25">
+      <c r="K259" s="51" t="s">
+        <v>125</v>
+      </c>
+      <c r="L259" s="7"/>
+      <c r="M259" s="7"/>
+      <c r="N259" s="7"/>
+      <c r="O259" s="7"/>
+      <c r="P259" s="7"/>
+      <c r="Q259" s="7"/>
+      <c r="R259" s="7"/>
+    </row>
+    <row r="260" spans="11:18" x14ac:dyDescent="0.25">
+      <c r="K260" s="51" t="s">
+        <v>127</v>
+      </c>
+      <c r="L260" s="7"/>
+      <c r="M260" s="7"/>
+      <c r="N260" s="7"/>
+      <c r="O260" s="7"/>
+      <c r="P260" s="7"/>
+      <c r="Q260" s="7"/>
+      <c r="R260" s="7"/>
+    </row>
+    <row r="261" spans="11:18" x14ac:dyDescent="0.25">
+      <c r="K261" s="7"/>
+      <c r="L261" s="7"/>
+      <c r="M261" s="7"/>
+      <c r="N261" s="7"/>
+      <c r="O261" s="7"/>
+      <c r="P261" s="7"/>
+      <c r="Q261" s="7"/>
+      <c r="R261" s="7"/>
+    </row>
+    <row r="262" spans="11:18" x14ac:dyDescent="0.25">
+      <c r="K262" s="52" t="s">
+        <v>126</v>
+      </c>
+      <c r="L262" s="52"/>
+      <c r="M262" s="52"/>
+      <c r="N262" s="7"/>
+      <c r="O262" s="7"/>
+      <c r="P262" s="7"/>
+      <c r="Q262" s="7"/>
+      <c r="R262" s="7"/>
+    </row>
+    <row r="274" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A274" s="7">
+        <v>77</v>
+      </c>
+      <c r="B274" s="32" t="s">
+        <v>136</v>
+      </c>
+      <c r="C274" s="33"/>
+      <c r="D274" s="33"/>
+      <c r="E274" s="33"/>
+      <c r="F274" s="33"/>
+      <c r="G274" s="33"/>
+      <c r="H274" s="33"/>
+      <c r="I274" s="33"/>
+      <c r="J274" s="33"/>
+      <c r="K274" s="33"/>
+      <c r="L274" s="33"/>
+      <c r="M274" s="33"/>
+      <c r="N274" s="33"/>
+      <c r="O274" s="33"/>
+    </row>
+    <row r="275" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A275" s="7">
+        <v>78</v>
+      </c>
+      <c r="B275" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="C275" s="33"/>
+      <c r="D275" s="33"/>
+      <c r="E275" s="33"/>
+      <c r="F275" s="33"/>
+      <c r="G275" s="33"/>
+      <c r="H275" s="33"/>
+      <c r="I275" s="33"/>
+      <c r="J275" s="33"/>
+      <c r="K275" s="33"/>
+      <c r="L275" s="33"/>
+      <c r="M275" s="33"/>
+      <c r="N275" s="33"/>
+      <c r="O275" s="33"/>
+      <c r="P275" s="33"/>
+      <c r="Q275" s="33"/>
+      <c r="R275" s="33"/>
+    </row>
+    <row r="276" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A276" s="7">
+        <v>79</v>
+      </c>
+      <c r="B276" s="36" t="s">
+        <v>121</v>
+      </c>
+      <c r="C276" s="36"/>
+      <c r="D276" s="36"/>
+      <c r="E276" s="36"/>
+      <c r="F276" s="36"/>
+      <c r="G276" s="36"/>
+      <c r="H276" s="36"/>
+      <c r="I276" s="36"/>
+      <c r="J276" s="36"/>
+      <c r="K276" s="36"/>
+      <c r="L276" s="36"/>
+      <c r="M276" s="36"/>
+      <c r="N276" s="36"/>
+      <c r="O276" s="36"/>
+      <c r="P276" s="36"/>
+      <c r="Q276" s="36"/>
+      <c r="R276" s="36"/>
+      <c r="S276" s="36"/>
+      <c r="T276" s="36"/>
+      <c r="U276" s="36"/>
+    </row>
+    <row r="277" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A277" s="7"/>
+      <c r="B277" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="C277" s="33"/>
+      <c r="D277" s="33"/>
+      <c r="E277" s="33"/>
+      <c r="F277" s="33"/>
+      <c r="G277" s="33"/>
+      <c r="H277" s="33"/>
+      <c r="I277" s="33"/>
+      <c r="J277" s="33"/>
+      <c r="K277" s="33"/>
+      <c r="L277" s="33"/>
+      <c r="M277" s="33"/>
+      <c r="N277" s="33"/>
+      <c r="O277" s="33"/>
+      <c r="P277" s="33"/>
+      <c r="Q277" s="33"/>
+      <c r="R277" s="33"/>
+      <c r="S277"/>
+      <c r="T277"/>
+      <c r="U277"/>
+    </row>
+    <row r="278" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A278" s="7">
+        <v>80</v>
+      </c>
+      <c r="B278" s="32" t="s">
+        <v>122</v>
+      </c>
+      <c r="C278" s="33"/>
+      <c r="D278" s="33"/>
+      <c r="E278" s="33"/>
+      <c r="F278" s="33"/>
+      <c r="G278" s="33"/>
+      <c r="H278" s="33"/>
+      <c r="I278" s="33"/>
+      <c r="J278" s="33"/>
+      <c r="K278" s="33"/>
+      <c r="L278" s="33"/>
+      <c r="M278" s="33"/>
+      <c r="N278" s="33"/>
+      <c r="O278" s="33"/>
+    </row>
+    <row r="279" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A279" s="7">
+        <v>81</v>
+      </c>
+      <c r="B279" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="C279" s="33"/>
+      <c r="D279" s="33"/>
+      <c r="E279" s="33"/>
+      <c r="F279" s="33"/>
+      <c r="G279" s="33"/>
+      <c r="H279" s="33"/>
+      <c r="I279" s="33"/>
+      <c r="J279" s="33"/>
+      <c r="K279" s="33"/>
+      <c r="L279" s="33"/>
+      <c r="M279" s="33"/>
+      <c r="N279" s="33"/>
+      <c r="O279" s="33"/>
+    </row>
+    <row r="280" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A280" s="7">
+        <v>82</v>
+      </c>
+      <c r="B280" s="32" t="s">
+        <v>129</v>
+      </c>
+      <c r="C280" s="33"/>
+      <c r="D280" s="33"/>
+      <c r="E280" s="33"/>
+      <c r="F280" s="33"/>
+      <c r="G280" s="33"/>
+      <c r="H280" s="33"/>
+      <c r="I280" s="33"/>
+      <c r="J280" s="33"/>
+      <c r="K280" s="33"/>
+      <c r="L280" s="33"/>
+      <c r="M280" s="33"/>
+      <c r="N280" s="33"/>
+      <c r="O280" s="33"/>
+    </row>
+    <row r="281" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A281" s="7"/>
+      <c r="B281" s="32" t="s">
+        <v>138</v>
+      </c>
+      <c r="C281" s="33"/>
+      <c r="D281" s="33"/>
+      <c r="E281" s="33"/>
+      <c r="F281" s="33"/>
+      <c r="G281" s="33"/>
+      <c r="H281" s="33"/>
+      <c r="I281" s="33"/>
+      <c r="J281" s="33"/>
+      <c r="K281" s="33"/>
+      <c r="L281" s="33"/>
+      <c r="M281" s="33"/>
+      <c r="N281" s="33"/>
+      <c r="O281" s="33"/>
+    </row>
+    <row r="282" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A282" s="7"/>
+      <c r="B282" s="32" t="s">
+        <v>128</v>
+      </c>
+      <c r="C282" s="33"/>
+      <c r="D282" s="33"/>
+      <c r="E282" s="33"/>
+      <c r="F282" s="33"/>
+      <c r="G282" s="33"/>
+      <c r="H282" s="33"/>
+      <c r="I282" s="33"/>
+      <c r="J282" s="33"/>
+      <c r="K282" s="33"/>
+      <c r="L282" s="33"/>
+      <c r="M282" s="33"/>
+      <c r="N282" s="33"/>
+      <c r="O282" s="33"/>
+    </row>
+    <row r="283" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A283" s="7"/>
+      <c r="B283" s="32" t="s">
+        <v>130</v>
+      </c>
+      <c r="C283" s="33"/>
+      <c r="D283" s="33"/>
+      <c r="E283" s="33"/>
+      <c r="F283" s="33"/>
+      <c r="G283" s="33"/>
+      <c r="H283" s="33"/>
+      <c r="I283" s="33"/>
+      <c r="J283" s="33"/>
+      <c r="K283" s="33"/>
+      <c r="L283" s="33"/>
+      <c r="M283" s="33"/>
+      <c r="N283" s="33"/>
+      <c r="O283" s="33"/>
+    </row>
+    <row r="284" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A284" s="7"/>
+      <c r="B284" s="32" t="s">
+        <v>131</v>
+      </c>
+      <c r="C284" s="33"/>
+      <c r="D284" s="33"/>
+      <c r="E284" s="33"/>
+      <c r="F284" s="33"/>
+      <c r="G284" s="33"/>
+      <c r="H284" s="33"/>
+      <c r="I284" s="33"/>
+      <c r="J284" s="33"/>
+      <c r="K284" s="33"/>
+      <c r="L284" s="33"/>
+      <c r="M284" s="33"/>
+      <c r="N284" s="33"/>
+      <c r="O284" s="33"/>
+    </row>
+    <row r="285" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A285" s="7">
+        <v>83</v>
+      </c>
+      <c r="B285" s="32" t="s">
+        <v>132</v>
+      </c>
+      <c r="C285" s="33"/>
+      <c r="D285" s="33"/>
+      <c r="E285" s="33"/>
+      <c r="F285" s="33"/>
+      <c r="G285" s="33"/>
+      <c r="H285" s="33"/>
+      <c r="I285" s="33"/>
+      <c r="J285" s="33"/>
+      <c r="K285" s="33"/>
+      <c r="L285" s="33"/>
+      <c r="M285" s="33"/>
+      <c r="N285" s="33"/>
+      <c r="O285" s="33"/>
+    </row>
+    <row r="286" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A286" s="8">
+        <v>84</v>
+      </c>
+      <c r="B286" s="31" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="288" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="M288" s="31" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="289" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="M289" s="31" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="299" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A299" s="7">
+        <v>85</v>
+      </c>
+      <c r="B299" s="33" t="s">
+        <v>137</v>
+      </c>
+      <c r="C299" s="33"/>
+      <c r="D299" s="33"/>
+      <c r="E299" s="33"/>
+      <c r="F299" s="33"/>
+      <c r="G299" s="33"/>
+      <c r="H299" s="33"/>
+      <c r="I299" s="33"/>
+      <c r="J299" s="33"/>
+      <c r="K299" s="33"/>
+      <c r="L299" s="33"/>
+      <c r="M299" s="33"/>
+      <c r="N299" s="33"/>
+      <c r="O299" s="33"/>
+      <c r="P299" s="33"/>
+      <c r="Q299" s="33"/>
+      <c r="R299" s="33"/>
+      <c r="S299" s="7"/>
+      <c r="T299" s="33"/>
+      <c r="U299" s="33"/>
     </row>
   </sheetData>
-  <mergeCells count="84">
+  <mergeCells count="100">
     <mergeCell ref="B187:S187"/>
     <mergeCell ref="B94:P94"/>
     <mergeCell ref="B95:P95"/>
@@ -6901,6 +7486,15 @@
     <mergeCell ref="B190:X190"/>
     <mergeCell ref="B98:S98"/>
     <mergeCell ref="B99:P99"/>
+    <mergeCell ref="B175:S175"/>
+    <mergeCell ref="B186:S186"/>
+    <mergeCell ref="U155:X155"/>
+    <mergeCell ref="U156:W156"/>
+    <mergeCell ref="B121:S121"/>
+    <mergeCell ref="B122:S122"/>
+    <mergeCell ref="B123:S123"/>
+    <mergeCell ref="B184:S184"/>
+    <mergeCell ref="B185:S185"/>
     <mergeCell ref="B69:P69"/>
     <mergeCell ref="B70:P70"/>
     <mergeCell ref="B71:P71"/>
@@ -6948,15 +7542,6 @@
     <mergeCell ref="B10:P10"/>
     <mergeCell ref="B11:P11"/>
     <mergeCell ref="B12:P12"/>
-    <mergeCell ref="B175:S175"/>
-    <mergeCell ref="B186:S186"/>
-    <mergeCell ref="U155:X155"/>
-    <mergeCell ref="U156:W156"/>
-    <mergeCell ref="B121:S121"/>
-    <mergeCell ref="B122:S122"/>
-    <mergeCell ref="B123:S123"/>
-    <mergeCell ref="B184:S184"/>
-    <mergeCell ref="B185:S185"/>
     <mergeCell ref="B173:S173"/>
     <mergeCell ref="B174:S174"/>
     <mergeCell ref="B97:P97"/>
@@ -6970,14 +7555,30 @@
     <mergeCell ref="B125:S125"/>
     <mergeCell ref="B155:S155"/>
     <mergeCell ref="B118:S118"/>
-    <mergeCell ref="B188:S188"/>
-    <mergeCell ref="B189:S189"/>
-    <mergeCell ref="B253:S253"/>
     <mergeCell ref="U250:X250"/>
     <mergeCell ref="B254:S254"/>
     <mergeCell ref="U251:X251"/>
     <mergeCell ref="B219:P219"/>
     <mergeCell ref="B220:P220"/>
+    <mergeCell ref="B274:O274"/>
+    <mergeCell ref="B275:R275"/>
+    <mergeCell ref="B278:O278"/>
+    <mergeCell ref="B188:S188"/>
+    <mergeCell ref="B189:S189"/>
+    <mergeCell ref="B253:S253"/>
+    <mergeCell ref="L199:S199"/>
+    <mergeCell ref="B276:U276"/>
+    <mergeCell ref="B255:S255"/>
+    <mergeCell ref="B279:O279"/>
+    <mergeCell ref="B299:R299"/>
+    <mergeCell ref="T299:U299"/>
+    <mergeCell ref="B277:R277"/>
+    <mergeCell ref="B280:O280"/>
+    <mergeCell ref="B281:O281"/>
+    <mergeCell ref="B282:O282"/>
+    <mergeCell ref="B283:O283"/>
+    <mergeCell ref="B284:O284"/>
+    <mergeCell ref="B285:O285"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>